<commit_message>
Endret litt på sorteringer og rekkefølger.
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -467,12 +467,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Tilbud</t>
+          <t>Etterspørsel</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Etterspørsel</t>
+          <t>Tilbud</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -491,13 +491,13 @@
         <v>2020</v>
       </c>
       <c r="C2" t="n">
-        <v>47126.0830648142</v>
+        <v>47126</v>
       </c>
       <c r="D2" t="n">
         <v>47126</v>
       </c>
       <c r="E2" t="n">
-        <v>0.08306481420004275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -506,13 +506,13 @@
         <v>2021</v>
       </c>
       <c r="C3" t="n">
-        <v>48004.62975839099</v>
+        <v>46632</v>
       </c>
       <c r="D3" t="n">
-        <v>46632.05371139223</v>
+        <v>48005</v>
       </c>
       <c r="E3" t="n">
-        <v>1372.576046998758</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="4">
@@ -521,13 +521,13 @@
         <v>2022</v>
       </c>
       <c r="C4" t="n">
-        <v>49054.44622535737</v>
+        <v>46204</v>
       </c>
       <c r="D4" t="n">
-        <v>46203.63378433167</v>
+        <v>49054</v>
       </c>
       <c r="E4" t="n">
-        <v>2850.812441025693</v>
+        <v>2851</v>
       </c>
     </row>
     <row r="5">
@@ -536,13 +536,13 @@
         <v>2023</v>
       </c>
       <c r="C5" t="n">
-        <v>50110.97840053061</v>
+        <v>46086</v>
       </c>
       <c r="D5" t="n">
-        <v>46086.26317118015</v>
+        <v>50111</v>
       </c>
       <c r="E5" t="n">
-        <v>4024.715229350455</v>
+        <v>4025</v>
       </c>
     </row>
     <row r="6">
@@ -551,13 +551,13 @@
         <v>2024</v>
       </c>
       <c r="C6" t="n">
-        <v>51172.69058717482</v>
+        <v>45874</v>
       </c>
       <c r="D6" t="n">
-        <v>45874.29644138199</v>
+        <v>51173</v>
       </c>
       <c r="E6" t="n">
-        <v>5298.39414579283</v>
+        <v>5298</v>
       </c>
     </row>
     <row r="7">
@@ -566,13 +566,13 @@
         <v>2025</v>
       </c>
       <c r="C7" t="n">
-        <v>52231.80099243067</v>
+        <v>45756</v>
       </c>
       <c r="D7" t="n">
-        <v>45755.53768733664</v>
+        <v>52232</v>
       </c>
       <c r="E7" t="n">
-        <v>6476.263305094028</v>
+        <v>6476</v>
       </c>
     </row>
     <row r="8">
@@ -581,13 +581,13 @@
         <v>2026</v>
       </c>
       <c r="C8" t="n">
-        <v>53290.26089850663</v>
+        <v>45706</v>
       </c>
       <c r="D8" t="n">
-        <v>45705.91705328642</v>
+        <v>53290</v>
       </c>
       <c r="E8" t="n">
-        <v>7584.34384522021</v>
+        <v>7584</v>
       </c>
     </row>
     <row r="9">
@@ -596,13 +596,13 @@
         <v>2027</v>
       </c>
       <c r="C9" t="n">
-        <v>54321.80285858336</v>
+        <v>45740</v>
       </c>
       <c r="D9" t="n">
-        <v>45740.46102809843</v>
+        <v>54322</v>
       </c>
       <c r="E9" t="n">
-        <v>8581.341830484926</v>
+        <v>8581</v>
       </c>
     </row>
     <row r="10">
@@ -611,13 +611,13 @@
         <v>2028</v>
       </c>
       <c r="C10" t="n">
-        <v>55326.60830323036</v>
+        <v>45850</v>
       </c>
       <c r="D10" t="n">
-        <v>45850.33969078168</v>
+        <v>55327</v>
       </c>
       <c r="E10" t="n">
-        <v>9476.268612448686</v>
+        <v>9476</v>
       </c>
     </row>
     <row r="11">
@@ -626,13 +626,13 @@
         <v>2029</v>
       </c>
       <c r="C11" t="n">
-        <v>56273.13606764919</v>
+        <v>46028</v>
       </c>
       <c r="D11" t="n">
-        <v>46027.7014749285</v>
+        <v>56273</v>
       </c>
       <c r="E11" t="n">
-        <v>10245.43459272069</v>
+        <v>10245</v>
       </c>
     </row>
     <row r="12">
@@ -641,13 +641,13 @@
         <v>2030</v>
       </c>
       <c r="C12" t="n">
-        <v>57142.08589957682</v>
+        <v>46237</v>
       </c>
       <c r="D12" t="n">
-        <v>46236.93642715757</v>
+        <v>57142</v>
       </c>
       <c r="E12" t="n">
-        <v>10905.14947241925</v>
+        <v>10905</v>
       </c>
     </row>
     <row r="13">
@@ -656,13 +656,13 @@
         <v>2031</v>
       </c>
       <c r="C13" t="n">
-        <v>57934.60162376797</v>
+        <v>46459</v>
       </c>
       <c r="D13" t="n">
-        <v>46458.65971752989</v>
+        <v>57935</v>
       </c>
       <c r="E13" t="n">
-        <v>11475.94190623808</v>
+        <v>11476</v>
       </c>
     </row>
     <row r="14">
@@ -671,13 +671,13 @@
         <v>2032</v>
       </c>
       <c r="C14" t="n">
-        <v>58628.39962179886</v>
+        <v>46681</v>
       </c>
       <c r="D14" t="n">
-        <v>46680.78018808762</v>
+        <v>58628</v>
       </c>
       <c r="E14" t="n">
-        <v>11947.61943371124</v>
+        <v>11948</v>
       </c>
     </row>
     <row r="15">
@@ -686,13 +686,13 @@
         <v>2033</v>
       </c>
       <c r="C15" t="n">
-        <v>59226.91288950575</v>
+        <v>46909</v>
       </c>
       <c r="D15" t="n">
-        <v>46909.01548062159</v>
+        <v>59227</v>
       </c>
       <c r="E15" t="n">
-        <v>12317.89740888416</v>
+        <v>12318</v>
       </c>
     </row>
     <row r="16">
@@ -701,13 +701,13 @@
         <v>2034</v>
       </c>
       <c r="C16" t="n">
-        <v>59747.48109903088</v>
+        <v>47175</v>
       </c>
       <c r="D16" t="n">
-        <v>47174.72820068857</v>
+        <v>59747</v>
       </c>
       <c r="E16" t="n">
-        <v>12572.75289834232</v>
+        <v>12573</v>
       </c>
     </row>
     <row r="17">
@@ -716,13 +716,13 @@
         <v>2035</v>
       </c>
       <c r="C17" t="n">
-        <v>60180.21425103192</v>
+        <v>47470</v>
       </c>
       <c r="D17" t="n">
-        <v>47470.08737204528</v>
+        <v>60180</v>
       </c>
       <c r="E17" t="n">
-        <v>12710.12687898664</v>
+        <v>12710</v>
       </c>
     </row>
     <row r="18">
@@ -731,13 +731,13 @@
         <v>2036</v>
       </c>
       <c r="C18" t="n">
-        <v>60568.44161486525</v>
+        <v>47788</v>
       </c>
       <c r="D18" t="n">
-        <v>47787.54030191174</v>
+        <v>60568</v>
       </c>
       <c r="E18" t="n">
-        <v>12780.90131295351</v>
+        <v>12781</v>
       </c>
     </row>
     <row r="19">
@@ -746,13 +746,13 @@
         <v>2037</v>
       </c>
       <c r="C19" t="n">
-        <v>60934.61678389546</v>
+        <v>48120</v>
       </c>
       <c r="D19" t="n">
-        <v>48120.37219422121</v>
+        <v>60935</v>
       </c>
       <c r="E19" t="n">
-        <v>12814.24458967425</v>
+        <v>12814</v>
       </c>
     </row>
     <row r="20">
@@ -761,13 +761,13 @@
         <v>2038</v>
       </c>
       <c r="C20" t="n">
-        <v>61311.64786945219</v>
+        <v>48432</v>
       </c>
       <c r="D20" t="n">
-        <v>48431.50910648081</v>
+        <v>61312</v>
       </c>
       <c r="E20" t="n">
-        <v>12880.13876297138</v>
+        <v>12880</v>
       </c>
     </row>
     <row r="21">
@@ -776,13 +776,13 @@
         <v>2039</v>
       </c>
       <c r="C21" t="n">
-        <v>61717.09137831684</v>
+        <v>48682</v>
       </c>
       <c r="D21" t="n">
-        <v>48681.69907458359</v>
+        <v>61717</v>
       </c>
       <c r="E21" t="n">
-        <v>13035.39230373325</v>
+        <v>13035</v>
       </c>
     </row>
     <row r="22">
@@ -791,32 +791,32 @@
         <v>2040</v>
       </c>
       <c r="C22" t="n">
-        <v>62174.31169826203</v>
+        <v>48869</v>
       </c>
       <c r="D22" t="n">
-        <v>48868.6385166429</v>
+        <v>62174</v>
       </c>
       <c r="E22" t="n">
-        <v>13305.67318161912</v>
+        <v>13306</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>fa</t>
+          <t>gr</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C23" t="n">
-        <v>16557.0175625449</v>
+        <v>52381</v>
       </c>
       <c r="D23" t="n">
-        <v>16557</v>
+        <v>52381</v>
       </c>
       <c r="E23" t="n">
-        <v>0.01756254490101128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -825,13 +825,13 @@
         <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>17577.87934576339</v>
+        <v>52370</v>
       </c>
       <c r="D24" t="n">
-        <v>16581.60029429819</v>
+        <v>52772</v>
       </c>
       <c r="E24" t="n">
-        <v>996.2790514652006</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25">
@@ -840,13 +840,13 @@
         <v>2022</v>
       </c>
       <c r="C25" t="n">
-        <v>18645.61915878023</v>
+        <v>52430</v>
       </c>
       <c r="D25" t="n">
-        <v>16636.59193662015</v>
+        <v>53230</v>
       </c>
       <c r="E25" t="n">
-        <v>2009.027222160079</v>
+        <v>800</v>
       </c>
     </row>
     <row r="26">
@@ -855,13 +855,13 @@
         <v>2023</v>
       </c>
       <c r="C26" t="n">
-        <v>19743.70604522206</v>
+        <v>52329</v>
       </c>
       <c r="D26" t="n">
-        <v>16655.66568649303</v>
+        <v>53746</v>
       </c>
       <c r="E26" t="n">
-        <v>3088.040358729035</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="27">
@@ -870,13 +870,13 @@
         <v>2024</v>
       </c>
       <c r="C27" t="n">
-        <v>20844.41946195418</v>
+        <v>52127</v>
       </c>
       <c r="D27" t="n">
-        <v>16667.14683357005</v>
+        <v>54316</v>
       </c>
       <c r="E27" t="n">
-        <v>4177.272628384129</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="28">
@@ -885,13 +885,13 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>21945.75175176744</v>
+        <v>51767</v>
       </c>
       <c r="D28" t="n">
-        <v>16664.37145049756</v>
+        <v>54926</v>
       </c>
       <c r="E28" t="n">
-        <v>5281.380301269874</v>
+        <v>3159</v>
       </c>
     </row>
     <row r="29">
@@ -900,13 +900,13 @@
         <v>2026</v>
       </c>
       <c r="C29" t="n">
-        <v>23027.54210229625</v>
+        <v>51321</v>
       </c>
       <c r="D29" t="n">
-        <v>16651.45765121366</v>
+        <v>55541</v>
       </c>
       <c r="E29" t="n">
-        <v>6376.084451082599</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="30">
@@ -915,13 +915,13 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>24098.50986946456</v>
+        <v>50918</v>
       </c>
       <c r="D30" t="n">
-        <v>16638.14057224105</v>
+        <v>56186</v>
       </c>
       <c r="E30" t="n">
-        <v>7460.369297223511</v>
+        <v>5269</v>
       </c>
     </row>
     <row r="31">
@@ -930,13 +930,13 @@
         <v>2028</v>
       </c>
       <c r="C31" t="n">
-        <v>25139.93894012234</v>
+        <v>50561</v>
       </c>
       <c r="D31" t="n">
-        <v>16617.04537266534</v>
+        <v>56811</v>
       </c>
       <c r="E31" t="n">
-        <v>8522.893567457002</v>
+        <v>6250</v>
       </c>
     </row>
     <row r="32">
@@ -945,13 +945,13 @@
         <v>2029</v>
       </c>
       <c r="C32" t="n">
-        <v>26166.86252582542</v>
+        <v>50199</v>
       </c>
       <c r="D32" t="n">
-        <v>16590.70236897196</v>
+        <v>57397</v>
       </c>
       <c r="E32" t="n">
-        <v>9576.160156853457</v>
+        <v>7198</v>
       </c>
     </row>
     <row r="33">
@@ -960,13 +960,13 @@
         <v>2030</v>
       </c>
       <c r="C33" t="n">
-        <v>27160.4346195555</v>
+        <v>49939</v>
       </c>
       <c r="D33" t="n">
-        <v>16574.2630108919</v>
+        <v>57919</v>
       </c>
       <c r="E33" t="n">
-        <v>10586.1716086636</v>
+        <v>7980</v>
       </c>
     </row>
     <row r="34">
@@ -975,13 +975,13 @@
         <v>2031</v>
       </c>
       <c r="C34" t="n">
-        <v>28119.36292037232</v>
+        <v>49717</v>
       </c>
       <c r="D34" t="n">
-        <v>16566.21543007695</v>
+        <v>58381</v>
       </c>
       <c r="E34" t="n">
-        <v>11553.14749029537</v>
+        <v>8665</v>
       </c>
     </row>
     <row r="35">
@@ -990,13 +990,13 @@
         <v>2032</v>
       </c>
       <c r="C35" t="n">
-        <v>29053.36037310434</v>
+        <v>49544</v>
       </c>
       <c r="D35" t="n">
-        <v>16565.8275830602</v>
+        <v>58767</v>
       </c>
       <c r="E35" t="n">
-        <v>12487.53279004414</v>
+        <v>9223</v>
       </c>
     </row>
     <row r="36">
@@ -1005,13 +1005,13 @@
         <v>2033</v>
       </c>
       <c r="C36" t="n">
-        <v>29967.37574261661</v>
+        <v>49425</v>
       </c>
       <c r="D36" t="n">
-        <v>16575.65505496017</v>
+        <v>59072</v>
       </c>
       <c r="E36" t="n">
-        <v>13391.72068765645</v>
+        <v>9648</v>
       </c>
     </row>
     <row r="37">
@@ -1020,13 +1020,13 @@
         <v>2034</v>
       </c>
       <c r="C37" t="n">
-        <v>30877.02846514702</v>
+        <v>49440</v>
       </c>
       <c r="D37" t="n">
-        <v>16591.88881312788</v>
+        <v>59320</v>
       </c>
       <c r="E37" t="n">
-        <v>14285.13965201915</v>
+        <v>9879</v>
       </c>
     </row>
     <row r="38">
@@ -1035,13 +1035,13 @@
         <v>2035</v>
       </c>
       <c r="C38" t="n">
-        <v>31771.79498718357</v>
+        <v>49547</v>
       </c>
       <c r="D38" t="n">
-        <v>16613.27743607803</v>
+        <v>59510</v>
       </c>
       <c r="E38" t="n">
-        <v>15158.51755110553</v>
+        <v>9963</v>
       </c>
     </row>
     <row r="39">
@@ -1050,13 +1050,13 @@
         <v>2036</v>
       </c>
       <c r="C39" t="n">
-        <v>32647.51808621049</v>
+        <v>49711</v>
       </c>
       <c r="D39" t="n">
-        <v>16643.73533224204</v>
+        <v>59678</v>
       </c>
       <c r="E39" t="n">
-        <v>16003.78275396845</v>
+        <v>9966</v>
       </c>
     </row>
     <row r="40">
@@ -1065,13 +1065,13 @@
         <v>2037</v>
       </c>
       <c r="C40" t="n">
-        <v>33519.54383147429</v>
+        <v>49919</v>
       </c>
       <c r="D40" t="n">
-        <v>16689.65655793095</v>
+        <v>59837</v>
       </c>
       <c r="E40" t="n">
-        <v>16829.88727354335</v>
+        <v>9918</v>
       </c>
     </row>
     <row r="41">
@@ -1080,13 +1080,13 @@
         <v>2038</v>
       </c>
       <c r="C41" t="n">
-        <v>34392.68668550663</v>
+        <v>50169</v>
       </c>
       <c r="D41" t="n">
-        <v>16744.90293064848</v>
+        <v>59992</v>
       </c>
       <c r="E41" t="n">
-        <v>17647.78375485815</v>
+        <v>9823</v>
       </c>
     </row>
     <row r="42">
@@ -1095,13 +1095,13 @@
         <v>2039</v>
       </c>
       <c r="C42" t="n">
-        <v>35262.63151798461</v>
+        <v>50466</v>
       </c>
       <c r="D42" t="n">
-        <v>16804.37885757281</v>
+        <v>60171</v>
       </c>
       <c r="E42" t="n">
-        <v>18458.2526604118</v>
+        <v>9705</v>
       </c>
     </row>
     <row r="43">
@@ -1110,32 +1110,32 @@
         <v>2040</v>
       </c>
       <c r="C43" t="n">
-        <v>36117.01702962166</v>
+        <v>50778</v>
       </c>
       <c r="D43" t="n">
-        <v>16866.6372656306</v>
+        <v>60363</v>
       </c>
       <c r="E43" t="n">
-        <v>19250.37976399106</v>
+        <v>9585</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>gr</t>
+          <t>fa</t>
         </is>
       </c>
       <c r="B44" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C44" t="n">
-        <v>52381.191691951</v>
+        <v>16557</v>
       </c>
       <c r="D44" t="n">
-        <v>52381</v>
+        <v>16557</v>
       </c>
       <c r="E44" t="n">
-        <v>0.1916919509967556</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1144,13 +1144,13 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>52771.50889259383</v>
+        <v>16582</v>
       </c>
       <c r="D45" t="n">
-        <v>52369.64549817717</v>
+        <v>17578</v>
       </c>
       <c r="E45" t="n">
-        <v>401.8633944166577</v>
+        <v>996</v>
       </c>
     </row>
     <row r="46">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>53230.45469905735</v>
+        <v>16637</v>
       </c>
       <c r="D46" t="n">
-        <v>52430.21118808368</v>
+        <v>18646</v>
       </c>
       <c r="E46" t="n">
-        <v>800.2435109736689</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>53745.639771789</v>
+        <v>16656</v>
       </c>
       <c r="D47" t="n">
-        <v>52329.17888746204</v>
+        <v>19744</v>
       </c>
       <c r="E47" t="n">
-        <v>1416.46088432696</v>
+        <v>3088</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>54316.22725689525</v>
+        <v>16667</v>
       </c>
       <c r="D48" t="n">
-        <v>52127.37455195614</v>
+        <v>20844</v>
       </c>
       <c r="E48" t="n">
-        <v>2188.852704939112</v>
+        <v>4177</v>
       </c>
     </row>
     <row r="49">
@@ -1204,13 +1204,13 @@
         <v>2025</v>
       </c>
       <c r="C49" t="n">
-        <v>54925.54611958685</v>
+        <v>16664</v>
       </c>
       <c r="D49" t="n">
-        <v>51766.54034639468</v>
+        <v>21946</v>
       </c>
       <c r="E49" t="n">
-        <v>3159.00577319217</v>
+        <v>5281</v>
       </c>
     </row>
     <row r="50">
@@ -1219,13 +1219,13 @@
         <v>2026</v>
       </c>
       <c r="C50" t="n">
-        <v>55540.74215721468</v>
+        <v>16651</v>
       </c>
       <c r="D50" t="n">
-        <v>51321.47499681712</v>
+        <v>23028</v>
       </c>
       <c r="E50" t="n">
-        <v>4219.267160397554</v>
+        <v>6376</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>56186.03748628655</v>
+        <v>16638</v>
       </c>
       <c r="D51" t="n">
-        <v>50917.51578372745</v>
+        <v>24099</v>
       </c>
       <c r="E51" t="n">
-        <v>5268.521702559105</v>
+        <v>7460</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>56810.50994648657</v>
+        <v>16617</v>
       </c>
       <c r="D52" t="n">
-        <v>50560.86691745833</v>
+        <v>25140</v>
       </c>
       <c r="E52" t="n">
-        <v>6249.643029028237</v>
+        <v>8523</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>57397.16605910769</v>
+        <v>16591</v>
       </c>
       <c r="D53" t="n">
-        <v>50199.43329568127</v>
+        <v>26167</v>
       </c>
       <c r="E53" t="n">
-        <v>7197.732763426422</v>
+        <v>9576</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1279,13 @@
         <v>2030</v>
       </c>
       <c r="C54" t="n">
-        <v>57918.78712431528</v>
+        <v>16574</v>
       </c>
       <c r="D54" t="n">
-        <v>49938.78735685929</v>
+        <v>27160</v>
       </c>
       <c r="E54" t="n">
-        <v>7979.999767455993</v>
+        <v>10586</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>58381.23317006562</v>
+        <v>16566</v>
       </c>
       <c r="D55" t="n">
-        <v>49716.59602351896</v>
+        <v>28119</v>
       </c>
       <c r="E55" t="n">
-        <v>8664.637146546665</v>
+        <v>11553</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>58767.28240764353</v>
+        <v>16566</v>
       </c>
       <c r="D56" t="n">
-        <v>49544.4426928484</v>
+        <v>29053</v>
       </c>
       <c r="E56" t="n">
-        <v>9222.839714795125</v>
+        <v>12488</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>59072.13288642734</v>
+        <v>16576</v>
       </c>
       <c r="D57" t="n">
-        <v>49424.50064940522</v>
+        <v>29967</v>
       </c>
       <c r="E57" t="n">
-        <v>9647.632237022117</v>
+        <v>13392</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>59319.62401592352</v>
+        <v>16592</v>
       </c>
       <c r="D58" t="n">
-        <v>49440.3080654768</v>
+        <v>30877</v>
       </c>
       <c r="E58" t="n">
-        <v>9879.315950446726</v>
+        <v>14285</v>
       </c>
     </row>
     <row r="59">
@@ -1354,13 +1354,13 @@
         <v>2035</v>
       </c>
       <c r="C59" t="n">
-        <v>59510.20409448468</v>
+        <v>16613</v>
       </c>
       <c r="D59" t="n">
-        <v>49547.04311871948</v>
+        <v>31772</v>
       </c>
       <c r="E59" t="n">
-        <v>9963.160975765197</v>
+        <v>15159</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>59677.51008775071</v>
+        <v>16644</v>
       </c>
       <c r="D60" t="n">
-        <v>49711.06473757153</v>
+        <v>32648</v>
       </c>
       <c r="E60" t="n">
-        <v>9966.445350179172</v>
+        <v>16004</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>59836.93420350074</v>
+        <v>16690</v>
       </c>
       <c r="D61" t="n">
-        <v>49919.05516612412</v>
+        <v>33520</v>
       </c>
       <c r="E61" t="n">
-        <v>9917.879037376617</v>
+        <v>16830</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>59991.91481397279</v>
+        <v>16745</v>
       </c>
       <c r="D62" t="n">
-        <v>50169.34384475125</v>
+        <v>34393</v>
       </c>
       <c r="E62" t="n">
-        <v>9822.570969221539</v>
+        <v>17648</v>
       </c>
     </row>
     <row r="63">
@@ -1414,13 +1414,13 @@
         <v>2039</v>
       </c>
       <c r="C63" t="n">
-        <v>60170.60982725364</v>
+        <v>16804</v>
       </c>
       <c r="D63" t="n">
-        <v>50465.95472455632</v>
+        <v>35263</v>
       </c>
       <c r="E63" t="n">
-        <v>9704.655102697317</v>
+        <v>18458</v>
       </c>
     </row>
     <row r="64">
@@ -1429,13 +1429,13 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>60362.63454706157</v>
+        <v>16867</v>
       </c>
       <c r="D64" t="n">
-        <v>50777.58543343424</v>
+        <v>36117</v>
       </c>
       <c r="E64" t="n">
-        <v>9585.049113627334</v>
+        <v>19250</v>
       </c>
     </row>
     <row r="65">
@@ -1448,13 +1448,13 @@
         <v>2020</v>
       </c>
       <c r="C65" t="n">
-        <v>30732.4941756971</v>
+        <v>30732</v>
       </c>
       <c r="D65" t="n">
         <v>30732</v>
       </c>
       <c r="E65" t="n">
-        <v>0.4941756971020368</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1463,13 +1463,13 @@
         <v>2021</v>
       </c>
       <c r="C66" t="n">
-        <v>30793.11365665312</v>
+        <v>30821</v>
       </c>
       <c r="D66" t="n">
-        <v>30821.12024387546</v>
+        <v>30793</v>
       </c>
       <c r="E66" t="n">
-        <v>-28.00658722233493</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="67">
@@ -1478,13 +1478,13 @@
         <v>2022</v>
       </c>
       <c r="C67" t="n">
-        <v>30889.45032449475</v>
+        <v>30975</v>
       </c>
       <c r="D67" t="n">
-        <v>30974.9572764656</v>
+        <v>30889</v>
       </c>
       <c r="E67" t="n">
-        <v>-85.50695197085224</v>
+        <v>-86</v>
       </c>
     </row>
     <row r="68">
@@ -1493,13 +1493,13 @@
         <v>2023</v>
       </c>
       <c r="C68" t="n">
-        <v>31003.61916535034</v>
+        <v>31104</v>
       </c>
       <c r="D68" t="n">
-        <v>31103.94157706718</v>
+        <v>31004</v>
       </c>
       <c r="E68" t="n">
-        <v>-100.3224117168356</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="69">
@@ -1508,13 +1508,13 @@
         <v>2024</v>
       </c>
       <c r="C69" t="n">
-        <v>31129.1515049316</v>
+        <v>31186</v>
       </c>
       <c r="D69" t="n">
-        <v>31186.10149359774</v>
+        <v>31129</v>
       </c>
       <c r="E69" t="n">
-        <v>-56.94998866613241</v>
+        <v>-57</v>
       </c>
     </row>
     <row r="70">
@@ -1523,13 +1523,13 @@
         <v>2025</v>
       </c>
       <c r="C70" t="n">
-        <v>31255.77283683757</v>
+        <v>31277</v>
       </c>
       <c r="D70" t="n">
-        <v>31276.5877043947</v>
+        <v>31256</v>
       </c>
       <c r="E70" t="n">
-        <v>-20.81486755713195</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="71">
@@ -1538,13 +1538,13 @@
         <v>2026</v>
       </c>
       <c r="C71" t="n">
-        <v>31383.55441270605</v>
+        <v>31334</v>
       </c>
       <c r="D71" t="n">
-        <v>31334.14674529331</v>
+        <v>31384</v>
       </c>
       <c r="E71" t="n">
-        <v>49.40766741273546</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72">
@@ -1553,13 +1553,13 @@
         <v>2027</v>
       </c>
       <c r="C72" t="n">
-        <v>31495.59099344995</v>
+        <v>31338</v>
       </c>
       <c r="D72" t="n">
-        <v>31337.9445698343</v>
+        <v>31496</v>
       </c>
       <c r="E72" t="n">
-        <v>157.6464236156498</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73">
@@ -1568,13 +1568,13 @@
         <v>2028</v>
       </c>
       <c r="C73" t="n">
-        <v>31592.84036535556</v>
+        <v>31213</v>
       </c>
       <c r="D73" t="n">
-        <v>31212.97522966661</v>
+        <v>31593</v>
       </c>
       <c r="E73" t="n">
-        <v>379.8651356889459</v>
+        <v>380</v>
       </c>
     </row>
     <row r="74">
@@ -1583,13 +1583,13 @@
         <v>2029</v>
       </c>
       <c r="C74" t="n">
-        <v>31671.15083897746</v>
+        <v>31036</v>
       </c>
       <c r="D74" t="n">
-        <v>31035.55492737661</v>
+        <v>31671</v>
       </c>
       <c r="E74" t="n">
-        <v>635.5959116008489</v>
+        <v>636</v>
       </c>
     </row>
     <row r="75">
@@ -1598,13 +1598,13 @@
         <v>2030</v>
       </c>
       <c r="C75" t="n">
-        <v>31716.43687060837</v>
+        <v>30852</v>
       </c>
       <c r="D75" t="n">
-        <v>30852.48129598876</v>
+        <v>31716</v>
       </c>
       <c r="E75" t="n">
-        <v>863.9555746196129</v>
+        <v>864</v>
       </c>
     </row>
     <row r="76">
@@ -1613,13 +1613,13 @@
         <v>2031</v>
       </c>
       <c r="C76" t="n">
-        <v>31724.60514893396</v>
+        <v>30725</v>
       </c>
       <c r="D76" t="n">
-        <v>30725.41589161201</v>
+        <v>31725</v>
       </c>
       <c r="E76" t="n">
-        <v>999.1892573219448</v>
+        <v>999</v>
       </c>
     </row>
     <row r="77">
@@ -1628,13 +1628,13 @@
         <v>2032</v>
       </c>
       <c r="C77" t="n">
-        <v>31698.14382138489</v>
+        <v>30641</v>
       </c>
       <c r="D77" t="n">
-        <v>30641.25198650448</v>
+        <v>31698</v>
       </c>
       <c r="E77" t="n">
-        <v>1056.891834880411</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="78">
@@ -1643,13 +1643,13 @@
         <v>2033</v>
       </c>
       <c r="C78" t="n">
-        <v>31631.88004594649</v>
+        <v>30624</v>
       </c>
       <c r="D78" t="n">
-        <v>30624.35667958554</v>
+        <v>31632</v>
       </c>
       <c r="E78" t="n">
-        <v>1007.523366360954</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="79">
@@ -1658,13 +1658,13 @@
         <v>2034</v>
       </c>
       <c r="C79" t="n">
-        <v>31551.62917878379</v>
+        <v>30558</v>
       </c>
       <c r="D79" t="n">
-        <v>30558.43648550644</v>
+        <v>31552</v>
       </c>
       <c r="E79" t="n">
-        <v>993.1926932773495</v>
+        <v>993</v>
       </c>
     </row>
     <row r="80">
@@ -1673,13 +1673,13 @@
         <v>2035</v>
       </c>
       <c r="C80" t="n">
-        <v>31436.52365036662</v>
+        <v>30469</v>
       </c>
       <c r="D80" t="n">
-        <v>30469.43855446423</v>
+        <v>31437</v>
       </c>
       <c r="E80" t="n">
-        <v>967.0850959023919</v>
+        <v>967</v>
       </c>
     </row>
     <row r="81">
@@ -1688,13 +1688,13 @@
         <v>2036</v>
       </c>
       <c r="C81" t="n">
-        <v>31321.12289151343</v>
+        <v>30408</v>
       </c>
       <c r="D81" t="n">
-        <v>30408.07017500239</v>
+        <v>31321</v>
       </c>
       <c r="E81" t="n">
-        <v>913.052716511047</v>
+        <v>913</v>
       </c>
     </row>
     <row r="82">
@@ -1703,13 +1703,13 @@
         <v>2037</v>
       </c>
       <c r="C82" t="n">
-        <v>31189.20441284174</v>
+        <v>30450</v>
       </c>
       <c r="D82" t="n">
-        <v>30449.97802304482</v>
+        <v>31189</v>
       </c>
       <c r="E82" t="n">
-        <v>739.2263897969169</v>
+        <v>739</v>
       </c>
     </row>
     <row r="83">
@@ -1718,13 +1718,13 @@
         <v>2038</v>
       </c>
       <c r="C83" t="n">
-        <v>31068.18394807317</v>
+        <v>30553</v>
       </c>
       <c r="D83" t="n">
-        <v>30552.6615528044</v>
+        <v>31068</v>
       </c>
       <c r="E83" t="n">
-        <v>515.5223952687702</v>
+        <v>516</v>
       </c>
     </row>
     <row r="84">
@@ -1733,13 +1733,13 @@
         <v>2039</v>
       </c>
       <c r="C84" t="n">
-        <v>30945.78821479743</v>
+        <v>30676</v>
       </c>
       <c r="D84" t="n">
-        <v>30676.281373244</v>
+        <v>30946</v>
       </c>
       <c r="E84" t="n">
-        <v>269.5068415534333</v>
+        <v>270</v>
       </c>
     </row>
     <row r="85">
@@ -1748,13 +1748,13 @@
         <v>2040</v>
       </c>
       <c r="C85" t="n">
-        <v>30833.75588955008</v>
+        <v>30821</v>
       </c>
       <c r="D85" t="n">
-        <v>30821.28899416169</v>
+        <v>30834</v>
       </c>
       <c r="E85" t="n">
-        <v>12.46689538838473</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86">
@@ -1767,13 +1767,13 @@
         <v>2020</v>
       </c>
       <c r="C86" t="n">
-        <v>13247.996343126</v>
+        <v>13248</v>
       </c>
       <c r="D86" t="n">
         <v>13248</v>
       </c>
       <c r="E86" t="n">
-        <v>-0.003656873999716481</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>13225.53629814894</v>
+        <v>13274</v>
       </c>
       <c r="D87" t="n">
-        <v>13273.73859970805</v>
+        <v>13226</v>
       </c>
       <c r="E87" t="n">
-        <v>-48.2023015591094</v>
+        <v>-48</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>13190.3489598656</v>
+        <v>13335</v>
       </c>
       <c r="D88" t="n">
-        <v>13334.59966336709</v>
+        <v>13190</v>
       </c>
       <c r="E88" t="n">
-        <v>-144.2507035014878</v>
+        <v>-144</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>13139.83922060289</v>
+        <v>13395</v>
       </c>
       <c r="D89" t="n">
-        <v>13394.55277209563</v>
+        <v>13140</v>
       </c>
       <c r="E89" t="n">
-        <v>-254.7135514927395</v>
+        <v>-255</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>13090.93648807719</v>
+        <v>13441</v>
       </c>
       <c r="D90" t="n">
-        <v>13440.95933576378</v>
+        <v>13091</v>
       </c>
       <c r="E90" t="n">
-        <v>-350.022847686585</v>
+        <v>-350</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>13023.97115190535</v>
+        <v>13512</v>
       </c>
       <c r="D91" t="n">
-        <v>13511.6728903575</v>
+        <v>13024</v>
       </c>
       <c r="E91" t="n">
-        <v>-487.7017384521478</v>
+        <v>-488</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>12944.71965886976</v>
+        <v>13577</v>
       </c>
       <c r="D92" t="n">
-        <v>13577.05469179901</v>
+        <v>12945</v>
       </c>
       <c r="E92" t="n">
-        <v>-632.3350329292589</v>
+        <v>-632</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>12865.45671456378</v>
+        <v>13610</v>
       </c>
       <c r="D93" t="n">
-        <v>13610.20732608411</v>
+        <v>12865</v>
       </c>
       <c r="E93" t="n">
-        <v>-744.7506115203287</v>
+        <v>-745</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>12762.97937391701</v>
+        <v>13569</v>
       </c>
       <c r="D94" t="n">
-        <v>13568.60273653104</v>
+        <v>12763</v>
       </c>
       <c r="E94" t="n">
-        <v>-805.6233626140292</v>
+        <v>-806</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>12663.60984640069</v>
+        <v>13500</v>
       </c>
       <c r="D95" t="n">
-        <v>13500.17041520007</v>
+        <v>12664</v>
       </c>
       <c r="E95" t="n">
-        <v>-836.5605687993884</v>
+        <v>-837</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>12555.22765529514</v>
+        <v>13418</v>
       </c>
       <c r="D96" t="n">
-        <v>13418.23235372904</v>
+        <v>12555</v>
       </c>
       <c r="E96" t="n">
-        <v>-863.0046984339006</v>
+        <v>-863</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>12434.05712962387</v>
+        <v>13360</v>
       </c>
       <c r="D97" t="n">
-        <v>13360.09524690133</v>
+        <v>12434</v>
       </c>
       <c r="E97" t="n">
-        <v>-926.0381172774541</v>
+        <v>-926</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>12320.4381537127</v>
+        <v>13316</v>
       </c>
       <c r="D98" t="n">
-        <v>13316.40781317062</v>
+        <v>12320</v>
       </c>
       <c r="E98" t="n">
-        <v>-995.9696594579164</v>
+        <v>-996</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>12190.82642391537</v>
+        <v>13299</v>
       </c>
       <c r="D99" t="n">
-        <v>13299.28575445196</v>
+        <v>12191</v>
       </c>
       <c r="E99" t="n">
-        <v>-1108.4593305366</v>
+        <v>-1108</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>12079.52161066612</v>
+        <v>13234</v>
       </c>
       <c r="D100" t="n">
-        <v>13233.80083274221</v>
+        <v>12080</v>
       </c>
       <c r="E100" t="n">
-        <v>-1154.279222076089</v>
+        <v>-1154</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>11961.02610840933</v>
+        <v>13141</v>
       </c>
       <c r="D101" t="n">
-        <v>13141.38099525944</v>
+        <v>11961</v>
       </c>
       <c r="E101" t="n">
-        <v>-1180.354886850108</v>
+        <v>-1180</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>11851.50997360486</v>
+        <v>13059</v>
       </c>
       <c r="D102" t="n">
-        <v>13059.13282328807</v>
+        <v>11852</v>
       </c>
       <c r="E102" t="n">
-        <v>-1207.622849683214</v>
+        <v>-1208</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>11747.94196284486</v>
+        <v>13031</v>
       </c>
       <c r="D103" t="n">
-        <v>13031.03988934283</v>
+        <v>11748</v>
       </c>
       <c r="E103" t="n">
-        <v>-1283.097926497969</v>
+        <v>-1283</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>11634.15990623534</v>
+        <v>13032</v>
       </c>
       <c r="D104" t="n">
-        <v>13031.63974672085</v>
+        <v>11634</v>
       </c>
       <c r="E104" t="n">
-        <v>-1397.479840485516</v>
+        <v>-1397</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>11541.31611966788</v>
+        <v>13036</v>
       </c>
       <c r="D105" t="n">
-        <v>13035.87148957256</v>
+        <v>11541</v>
       </c>
       <c r="E105" t="n">
-        <v>-1494.555369904683</v>
+        <v>-1495</v>
       </c>
     </row>
     <row r="106">
@@ -2067,13 +2067,13 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
-        <v>11442.80471970744</v>
+        <v>13052</v>
       </c>
       <c r="D106" t="n">
-        <v>13051.9368266657</v>
+        <v>11443</v>
       </c>
       <c r="E106" t="n">
-        <v>-1609.132106958266</v>
+        <v>-1609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Laget mer sexy utskrift.
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -484,7 +484,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>ba</t>
+          <t>Barnehagelærere</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
@@ -803,7 +803,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>gr</t>
+          <t>Grunnskolelærere</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
@@ -1122,7 +1122,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>fa</t>
+          <t>Faglærere</t>
         </is>
       </c>
       <c r="B44" s="1" t="n">
@@ -1441,7 +1441,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>ph</t>
+          <t>PPU Universitet og høyskole</t>
         </is>
       </c>
       <c r="B65" s="1" t="n">
@@ -1760,7 +1760,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>py</t>
+          <t>PPU Yrkesfag</t>
         </is>
       </c>
       <c r="B86" s="1" t="n">

</xml_diff>

<commit_message>
Fjernet bruk av beholdning.py og demografi.py
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -457,7 +457,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Yrke</t>
+          <t>Utdanning</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Barnehagelærere</t>
+          <t>Barnehagelærer</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
@@ -512,7 +512,7 @@
         <v>48005</v>
       </c>
       <c r="E3" t="n">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="4">
@@ -596,7 +596,7 @@
         <v>2027</v>
       </c>
       <c r="C9" t="n">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="D9" t="n">
         <v>54322</v>
@@ -677,7 +677,7 @@
         <v>58628</v>
       </c>
       <c r="E14" t="n">
-        <v>11948</v>
+        <v>11947</v>
       </c>
     </row>
     <row r="15">
@@ -746,7 +746,7 @@
         <v>2037</v>
       </c>
       <c r="C19" t="n">
-        <v>48120</v>
+        <v>48121</v>
       </c>
       <c r="D19" t="n">
         <v>60935</v>
@@ -797,13 +797,13 @@
         <v>62174</v>
       </c>
       <c r="E22" t="n">
-        <v>13306</v>
+        <v>13305</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Grunnskolelærere</t>
+          <t>Grunnskolelærer</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
@@ -825,7 +825,7 @@
         <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>52370</v>
+        <v>52369</v>
       </c>
       <c r="D24" t="n">
         <v>52772</v>
@@ -861,7 +861,7 @@
         <v>53746</v>
       </c>
       <c r="E26" t="n">
-        <v>1416</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="27">
@@ -885,7 +885,7 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>51767</v>
+        <v>51766</v>
       </c>
       <c r="D28" t="n">
         <v>54926</v>
@@ -915,7 +915,7 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>50918</v>
+        <v>50917</v>
       </c>
       <c r="D30" t="n">
         <v>56186</v>
@@ -975,7 +975,7 @@
         <v>2031</v>
       </c>
       <c r="C34" t="n">
-        <v>49717</v>
+        <v>49716</v>
       </c>
       <c r="D34" t="n">
         <v>58381</v>
@@ -1005,7 +1005,7 @@
         <v>2033</v>
       </c>
       <c r="C36" t="n">
-        <v>49425</v>
+        <v>49424</v>
       </c>
       <c r="D36" t="n">
         <v>59072</v>
@@ -1026,7 +1026,7 @@
         <v>59320</v>
       </c>
       <c r="E37" t="n">
-        <v>9879</v>
+        <v>9880</v>
       </c>
     </row>
     <row r="38">
@@ -1056,7 +1056,7 @@
         <v>59678</v>
       </c>
       <c r="E39" t="n">
-        <v>9966</v>
+        <v>9967</v>
       </c>
     </row>
     <row r="40">
@@ -1110,7 +1110,7 @@
         <v>2040</v>
       </c>
       <c r="C43" t="n">
-        <v>50778</v>
+        <v>50777</v>
       </c>
       <c r="D43" t="n">
         <v>60363</v>
@@ -1122,20 +1122,20 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Faglærere</t>
+          <t>Faglærer</t>
         </is>
       </c>
       <c r="B44" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C44" t="n">
-        <v>16557</v>
+        <v>16556</v>
       </c>
       <c r="D44" t="n">
         <v>16557</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1144,13 +1144,13 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>16582</v>
+        <v>16581</v>
       </c>
       <c r="D45" t="n">
         <v>17578</v>
       </c>
       <c r="E45" t="n">
-        <v>996</v>
+        <v>997</v>
       </c>
     </row>
     <row r="46">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>16637</v>
+        <v>16636</v>
       </c>
       <c r="D46" t="n">
         <v>18646</v>
       </c>
       <c r="E46" t="n">
-        <v>2009</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>16656</v>
+        <v>16655</v>
       </c>
       <c r="D47" t="n">
         <v>19744</v>
       </c>
       <c r="E47" t="n">
-        <v>3088</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>16667</v>
+        <v>16666</v>
       </c>
       <c r="D48" t="n">
         <v>20844</v>
       </c>
       <c r="E48" t="n">
-        <v>4177</v>
+        <v>4178</v>
       </c>
     </row>
     <row r="49">
@@ -1210,7 +1210,7 @@
         <v>21946</v>
       </c>
       <c r="E49" t="n">
-        <v>5281</v>
+        <v>5282</v>
       </c>
     </row>
     <row r="50">
@@ -1225,7 +1225,7 @@
         <v>23028</v>
       </c>
       <c r="E50" t="n">
-        <v>6376</v>
+        <v>6377</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>16638</v>
+        <v>16637</v>
       </c>
       <c r="D51" t="n">
         <v>24099</v>
       </c>
       <c r="E51" t="n">
-        <v>7460</v>
+        <v>7461</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>16617</v>
+        <v>16616</v>
       </c>
       <c r="D52" t="n">
         <v>25140</v>
       </c>
       <c r="E52" t="n">
-        <v>8523</v>
+        <v>8524</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>16591</v>
+        <v>16590</v>
       </c>
       <c r="D53" t="n">
         <v>26167</v>
       </c>
       <c r="E53" t="n">
-        <v>9576</v>
+        <v>9577</v>
       </c>
     </row>
     <row r="54">
@@ -1285,7 +1285,7 @@
         <v>27160</v>
       </c>
       <c r="E54" t="n">
-        <v>10586</v>
+        <v>10587</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>16566</v>
+        <v>16565</v>
       </c>
       <c r="D55" t="n">
         <v>28119</v>
       </c>
       <c r="E55" t="n">
-        <v>11553</v>
+        <v>11554</v>
       </c>
     </row>
     <row r="56">
@@ -1309,7 +1309,7 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>16566</v>
+        <v>16565</v>
       </c>
       <c r="D56" t="n">
         <v>29053</v>
@@ -1324,7 +1324,7 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>16576</v>
+        <v>16575</v>
       </c>
       <c r="D57" t="n">
         <v>29967</v>
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>16592</v>
+        <v>16591</v>
       </c>
       <c r="D58" t="n">
         <v>30877</v>
       </c>
       <c r="E58" t="n">
-        <v>14285</v>
+        <v>14286</v>
       </c>
     </row>
     <row r="59">
@@ -1369,7 +1369,7 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>16644</v>
+        <v>16643</v>
       </c>
       <c r="D60" t="n">
         <v>32648</v>
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>16690</v>
+        <v>16689</v>
       </c>
       <c r="D61" t="n">
         <v>33520</v>
       </c>
       <c r="E61" t="n">
-        <v>16830</v>
+        <v>16831</v>
       </c>
     </row>
     <row r="62">
@@ -1399,7 +1399,7 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>16745</v>
+        <v>16744</v>
       </c>
       <c r="D62" t="n">
         <v>34393</v>
@@ -1420,7 +1420,7 @@
         <v>35263</v>
       </c>
       <c r="E63" t="n">
-        <v>18458</v>
+        <v>18459</v>
       </c>
     </row>
     <row r="64">
@@ -1429,13 +1429,13 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>16867</v>
+        <v>16866</v>
       </c>
       <c r="D64" t="n">
         <v>36117</v>
       </c>
       <c r="E64" t="n">
-        <v>19250</v>
+        <v>19251</v>
       </c>
     </row>
     <row r="65">
@@ -1454,7 +1454,7 @@
         <v>30732</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -1754,7 +1754,7 @@
         <v>30834</v>
       </c>
       <c r="E85" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86">
@@ -1767,13 +1767,13 @@
         <v>2020</v>
       </c>
       <c r="C86" t="n">
-        <v>13248</v>
+        <v>13249</v>
       </c>
       <c r="D86" t="n">
         <v>13248</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="87">
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>13274</v>
+        <v>13275</v>
       </c>
       <c r="D87" t="n">
         <v>13226</v>
       </c>
       <c r="E87" t="n">
-        <v>-48</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>13335</v>
+        <v>13336</v>
       </c>
       <c r="D88" t="n">
         <v>13190</v>
       </c>
       <c r="E88" t="n">
-        <v>-144</v>
+        <v>-146</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>13395</v>
+        <v>13396</v>
       </c>
       <c r="D89" t="n">
         <v>13140</v>
       </c>
       <c r="E89" t="n">
-        <v>-255</v>
+        <v>-256</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>13441</v>
+        <v>13442</v>
       </c>
       <c r="D90" t="n">
         <v>13091</v>
       </c>
       <c r="E90" t="n">
-        <v>-350</v>
+        <v>-351</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>13512</v>
+        <v>13513</v>
       </c>
       <c r="D91" t="n">
         <v>13024</v>
       </c>
       <c r="E91" t="n">
-        <v>-488</v>
+        <v>-489</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>13577</v>
+        <v>13578</v>
       </c>
       <c r="D92" t="n">
         <v>12945</v>
       </c>
       <c r="E92" t="n">
-        <v>-632</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>13610</v>
+        <v>13612</v>
       </c>
       <c r="D93" t="n">
         <v>12865</v>
       </c>
       <c r="E93" t="n">
-        <v>-745</v>
+        <v>-746</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>13569</v>
+        <v>13570</v>
       </c>
       <c r="D94" t="n">
         <v>12763</v>
       </c>
       <c r="E94" t="n">
-        <v>-806</v>
+        <v>-807</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>13500</v>
+        <v>13502</v>
       </c>
       <c r="D95" t="n">
         <v>12664</v>
       </c>
       <c r="E95" t="n">
-        <v>-837</v>
+        <v>-838</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>13418</v>
+        <v>13420</v>
       </c>
       <c r="D96" t="n">
         <v>12555</v>
       </c>
       <c r="E96" t="n">
-        <v>-863</v>
+        <v>-864</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>13360</v>
+        <v>13362</v>
       </c>
       <c r="D97" t="n">
         <v>12434</v>
       </c>
       <c r="E97" t="n">
-        <v>-926</v>
+        <v>-927</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>13316</v>
+        <v>13318</v>
       </c>
       <c r="D98" t="n">
         <v>12320</v>
       </c>
       <c r="E98" t="n">
-        <v>-996</v>
+        <v>-997</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>13299</v>
+        <v>13301</v>
       </c>
       <c r="D99" t="n">
         <v>12191</v>
       </c>
       <c r="E99" t="n">
-        <v>-1108</v>
+        <v>-1110</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>13234</v>
+        <v>13235</v>
       </c>
       <c r="D100" t="n">
         <v>12080</v>
       </c>
       <c r="E100" t="n">
-        <v>-1154</v>
+        <v>-1156</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>13141</v>
+        <v>13143</v>
       </c>
       <c r="D101" t="n">
         <v>11961</v>
       </c>
       <c r="E101" t="n">
-        <v>-1180</v>
+        <v>-1182</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>13059</v>
+        <v>13061</v>
       </c>
       <c r="D102" t="n">
         <v>11852</v>
       </c>
       <c r="E102" t="n">
-        <v>-1208</v>
+        <v>-1209</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>13031</v>
+        <v>13033</v>
       </c>
       <c r="D103" t="n">
         <v>11748</v>
       </c>
       <c r="E103" t="n">
-        <v>-1283</v>
+        <v>-1285</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>13032</v>
+        <v>13033</v>
       </c>
       <c r="D104" t="n">
         <v>11634</v>
       </c>
       <c r="E104" t="n">
-        <v>-1397</v>
+        <v>-1399</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>13036</v>
+        <v>13037</v>
       </c>
       <c r="D105" t="n">
         <v>11541</v>
       </c>
       <c r="E105" t="n">
-        <v>-1495</v>
+        <v>-1496</v>
       </c>
     </row>
     <row r="106">
@@ -2067,13 +2067,13 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
-        <v>13052</v>
+        <v>13053</v>
       </c>
       <c r="D106" t="n">
         <v>11443</v>
       </c>
       <c r="E106" t="n">
-        <v>-1609</v>
+        <v>-1611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slettet beholdning.py og demografi.py. Forenklet input-filer. Fjernet ugyldige utdanninger (sp, st og an).
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -491,13 +491,13 @@
         <v>2020</v>
       </c>
       <c r="C2" t="n">
-        <v>47126</v>
+        <v>73231</v>
       </c>
       <c r="D2" t="n">
-        <v>47126</v>
+        <v>48590</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>-24641</v>
       </c>
     </row>
     <row r="3">
@@ -506,13 +506,13 @@
         <v>2021</v>
       </c>
       <c r="C3" t="n">
-        <v>46632</v>
+        <v>73077</v>
       </c>
       <c r="D3" t="n">
-        <v>48005</v>
+        <v>48790</v>
       </c>
       <c r="E3" t="n">
-        <v>1372</v>
+        <v>-24286</v>
       </c>
     </row>
     <row r="4">
@@ -521,13 +521,13 @@
         <v>2022</v>
       </c>
       <c r="C4" t="n">
-        <v>46204</v>
+        <v>73020</v>
       </c>
       <c r="D4" t="n">
-        <v>49054</v>
+        <v>49891</v>
       </c>
       <c r="E4" t="n">
-        <v>2851</v>
+        <v>-23129</v>
       </c>
     </row>
     <row r="5">
@@ -536,13 +536,13 @@
         <v>2023</v>
       </c>
       <c r="C5" t="n">
-        <v>46086</v>
+        <v>72811</v>
       </c>
       <c r="D5" t="n">
-        <v>50111</v>
+        <v>50914</v>
       </c>
       <c r="E5" t="n">
-        <v>4025</v>
+        <v>-21897</v>
       </c>
     </row>
     <row r="6">
@@ -551,13 +551,13 @@
         <v>2024</v>
       </c>
       <c r="C6" t="n">
-        <v>45874</v>
+        <v>72375</v>
       </c>
       <c r="D6" t="n">
-        <v>51173</v>
+        <v>52023</v>
       </c>
       <c r="E6" t="n">
-        <v>5298</v>
+        <v>-20352</v>
       </c>
     </row>
     <row r="7">
@@ -566,13 +566,13 @@
         <v>2025</v>
       </c>
       <c r="C7" t="n">
-        <v>45756</v>
+        <v>71710</v>
       </c>
       <c r="D7" t="n">
-        <v>52232</v>
+        <v>53104</v>
       </c>
       <c r="E7" t="n">
-        <v>6476</v>
+        <v>-18606</v>
       </c>
     </row>
     <row r="8">
@@ -581,13 +581,13 @@
         <v>2026</v>
       </c>
       <c r="C8" t="n">
-        <v>45706</v>
+        <v>70904</v>
       </c>
       <c r="D8" t="n">
-        <v>53290</v>
+        <v>54193</v>
       </c>
       <c r="E8" t="n">
-        <v>7584</v>
+        <v>-16712</v>
       </c>
     </row>
     <row r="9">
@@ -596,13 +596,13 @@
         <v>2027</v>
       </c>
       <c r="C9" t="n">
-        <v>45741</v>
+        <v>70143</v>
       </c>
       <c r="D9" t="n">
-        <v>54322</v>
+        <v>55227</v>
       </c>
       <c r="E9" t="n">
-        <v>8581</v>
+        <v>-14916</v>
       </c>
     </row>
     <row r="10">
@@ -611,13 +611,13 @@
         <v>2028</v>
       </c>
       <c r="C10" t="n">
-        <v>45850</v>
+        <v>69393</v>
       </c>
       <c r="D10" t="n">
-        <v>55327</v>
+        <v>56297</v>
       </c>
       <c r="E10" t="n">
-        <v>9476</v>
+        <v>-13097</v>
       </c>
     </row>
     <row r="11">
@@ -626,13 +626,13 @@
         <v>2029</v>
       </c>
       <c r="C11" t="n">
-        <v>46028</v>
+        <v>68616</v>
       </c>
       <c r="D11" t="n">
-        <v>56273</v>
+        <v>57341</v>
       </c>
       <c r="E11" t="n">
-        <v>10245</v>
+        <v>-11275</v>
       </c>
     </row>
     <row r="12">
@@ -641,13 +641,13 @@
         <v>2030</v>
       </c>
       <c r="C12" t="n">
-        <v>46237</v>
+        <v>67997</v>
       </c>
       <c r="D12" t="n">
-        <v>57142</v>
+        <v>58252</v>
       </c>
       <c r="E12" t="n">
-        <v>10905</v>
+        <v>-9745</v>
       </c>
     </row>
     <row r="13">
@@ -656,13 +656,13 @@
         <v>2031</v>
       </c>
       <c r="C13" t="n">
-        <v>46459</v>
+        <v>67472</v>
       </c>
       <c r="D13" t="n">
-        <v>57935</v>
+        <v>59055</v>
       </c>
       <c r="E13" t="n">
-        <v>11476</v>
+        <v>-8417</v>
       </c>
     </row>
     <row r="14">
@@ -671,13 +671,13 @@
         <v>2032</v>
       </c>
       <c r="C14" t="n">
-        <v>46681</v>
+        <v>67050</v>
       </c>
       <c r="D14" t="n">
-        <v>58628</v>
+        <v>59764</v>
       </c>
       <c r="E14" t="n">
-        <v>11947</v>
+        <v>-7286</v>
       </c>
     </row>
     <row r="15">
@@ -686,13 +686,13 @@
         <v>2033</v>
       </c>
       <c r="C15" t="n">
-        <v>46909</v>
+        <v>66749</v>
       </c>
       <c r="D15" t="n">
-        <v>59227</v>
+        <v>60372</v>
       </c>
       <c r="E15" t="n">
-        <v>12318</v>
+        <v>-6378</v>
       </c>
     </row>
     <row r="16">
@@ -701,13 +701,13 @@
         <v>2034</v>
       </c>
       <c r="C16" t="n">
-        <v>47175</v>
+        <v>66636</v>
       </c>
       <c r="D16" t="n">
-        <v>59747</v>
+        <v>60889</v>
       </c>
       <c r="E16" t="n">
-        <v>12573</v>
+        <v>-5747</v>
       </c>
     </row>
     <row r="17">
@@ -716,13 +716,13 @@
         <v>2035</v>
       </c>
       <c r="C17" t="n">
-        <v>47470</v>
+        <v>66656</v>
       </c>
       <c r="D17" t="n">
-        <v>60180</v>
+        <v>61320</v>
       </c>
       <c r="E17" t="n">
-        <v>12710</v>
+        <v>-5336</v>
       </c>
     </row>
     <row r="18">
@@ -731,13 +731,13 @@
         <v>2036</v>
       </c>
       <c r="C18" t="n">
-        <v>47788</v>
+        <v>66784</v>
       </c>
       <c r="D18" t="n">
-        <v>60568</v>
+        <v>61694</v>
       </c>
       <c r="E18" t="n">
-        <v>12781</v>
+        <v>-5089</v>
       </c>
     </row>
     <row r="19">
@@ -746,13 +746,13 @@
         <v>2037</v>
       </c>
       <c r="C19" t="n">
-        <v>48121</v>
+        <v>67042</v>
       </c>
       <c r="D19" t="n">
-        <v>60935</v>
+        <v>62093</v>
       </c>
       <c r="E19" t="n">
-        <v>12814</v>
+        <v>-4949</v>
       </c>
     </row>
     <row r="20">
@@ -761,13 +761,13 @@
         <v>2038</v>
       </c>
       <c r="C20" t="n">
-        <v>48432</v>
+        <v>67402</v>
       </c>
       <c r="D20" t="n">
-        <v>61312</v>
+        <v>62450</v>
       </c>
       <c r="E20" t="n">
-        <v>12880</v>
+        <v>-4952</v>
       </c>
     </row>
     <row r="21">
@@ -776,13 +776,13 @@
         <v>2039</v>
       </c>
       <c r="C21" t="n">
-        <v>48682</v>
+        <v>67843</v>
       </c>
       <c r="D21" t="n">
-        <v>61717</v>
+        <v>62849</v>
       </c>
       <c r="E21" t="n">
-        <v>13035</v>
+        <v>-4994</v>
       </c>
     </row>
     <row r="22">
@@ -791,13 +791,13 @@
         <v>2040</v>
       </c>
       <c r="C22" t="n">
-        <v>48869</v>
+        <v>68317</v>
       </c>
       <c r="D22" t="n">
-        <v>62174</v>
+        <v>63308</v>
       </c>
       <c r="E22" t="n">
-        <v>13305</v>
+        <v>-5009</v>
       </c>
     </row>
     <row r="23">
@@ -810,13 +810,13 @@
         <v>2020</v>
       </c>
       <c r="C23" t="n">
-        <v>52381</v>
+        <v>-7040</v>
       </c>
       <c r="D23" t="n">
         <v>52381</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>59421</v>
       </c>
     </row>
     <row r="24">
@@ -825,13 +825,13 @@
         <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>52369</v>
+        <v>-7026</v>
       </c>
       <c r="D24" t="n">
         <v>52772</v>
       </c>
       <c r="E24" t="n">
-        <v>402</v>
+        <v>59797</v>
       </c>
     </row>
     <row r="25">
@@ -840,13 +840,13 @@
         <v>2022</v>
       </c>
       <c r="C25" t="n">
-        <v>52430</v>
+        <v>-7018</v>
       </c>
       <c r="D25" t="n">
         <v>53230</v>
       </c>
       <c r="E25" t="n">
-        <v>800</v>
+        <v>60249</v>
       </c>
     </row>
     <row r="26">
@@ -855,13 +855,13 @@
         <v>2023</v>
       </c>
       <c r="C26" t="n">
-        <v>52329</v>
+        <v>-6983</v>
       </c>
       <c r="D26" t="n">
         <v>53746</v>
       </c>
       <c r="E26" t="n">
-        <v>1417</v>
+        <v>60728</v>
       </c>
     </row>
     <row r="27">
@@ -870,13 +870,13 @@
         <v>2024</v>
       </c>
       <c r="C27" t="n">
-        <v>52127</v>
+        <v>-6924</v>
       </c>
       <c r="D27" t="n">
         <v>54316</v>
       </c>
       <c r="E27" t="n">
-        <v>2189</v>
+        <v>61240</v>
       </c>
     </row>
     <row r="28">
@@ -885,13 +885,13 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>51766</v>
+        <v>-6828</v>
       </c>
       <c r="D28" t="n">
         <v>54926</v>
       </c>
       <c r="E28" t="n">
-        <v>3159</v>
+        <v>61754</v>
       </c>
     </row>
     <row r="29">
@@ -900,13 +900,13 @@
         <v>2026</v>
       </c>
       <c r="C29" t="n">
-        <v>51321</v>
+        <v>-6715</v>
       </c>
       <c r="D29" t="n">
         <v>55541</v>
       </c>
       <c r="E29" t="n">
-        <v>4219</v>
+        <v>62255</v>
       </c>
     </row>
     <row r="30">
@@ -915,13 +915,13 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>50917</v>
+        <v>-6612</v>
       </c>
       <c r="D30" t="n">
         <v>56186</v>
       </c>
       <c r="E30" t="n">
-        <v>5269</v>
+        <v>62799</v>
       </c>
     </row>
     <row r="31">
@@ -930,13 +930,13 @@
         <v>2028</v>
       </c>
       <c r="C31" t="n">
-        <v>50561</v>
+        <v>-6526</v>
       </c>
       <c r="D31" t="n">
         <v>56811</v>
       </c>
       <c r="E31" t="n">
-        <v>6250</v>
+        <v>63337</v>
       </c>
     </row>
     <row r="32">
@@ -945,13 +945,13 @@
         <v>2029</v>
       </c>
       <c r="C32" t="n">
-        <v>50199</v>
+        <v>-6441</v>
       </c>
       <c r="D32" t="n">
         <v>57397</v>
       </c>
       <c r="E32" t="n">
-        <v>7198</v>
+        <v>63838</v>
       </c>
     </row>
     <row r="33">
@@ -960,13 +960,13 @@
         <v>2030</v>
       </c>
       <c r="C33" t="n">
-        <v>49939</v>
+        <v>-6379</v>
       </c>
       <c r="D33" t="n">
         <v>57919</v>
       </c>
       <c r="E33" t="n">
-        <v>7980</v>
+        <v>64297</v>
       </c>
     </row>
     <row r="34">
@@ -975,13 +975,13 @@
         <v>2031</v>
       </c>
       <c r="C34" t="n">
-        <v>49716</v>
+        <v>-6323</v>
       </c>
       <c r="D34" t="n">
         <v>58381</v>
       </c>
       <c r="E34" t="n">
-        <v>8665</v>
+        <v>64704</v>
       </c>
     </row>
     <row r="35">
@@ -990,13 +990,13 @@
         <v>2032</v>
       </c>
       <c r="C35" t="n">
-        <v>49544</v>
+        <v>-6277</v>
       </c>
       <c r="D35" t="n">
         <v>58767</v>
       </c>
       <c r="E35" t="n">
-        <v>9223</v>
+        <v>65045</v>
       </c>
     </row>
     <row r="36">
@@ -1005,13 +1005,13 @@
         <v>2033</v>
       </c>
       <c r="C36" t="n">
-        <v>49424</v>
+        <v>-6241</v>
       </c>
       <c r="D36" t="n">
         <v>59072</v>
       </c>
       <c r="E36" t="n">
-        <v>9648</v>
+        <v>65314</v>
       </c>
     </row>
     <row r="37">
@@ -1020,13 +1020,13 @@
         <v>2034</v>
       </c>
       <c r="C37" t="n">
-        <v>49440</v>
+        <v>-6239</v>
       </c>
       <c r="D37" t="n">
         <v>59320</v>
       </c>
       <c r="E37" t="n">
-        <v>9880</v>
+        <v>65559</v>
       </c>
     </row>
     <row r="38">
@@ -1035,13 +1035,13 @@
         <v>2035</v>
       </c>
       <c r="C38" t="n">
-        <v>49547</v>
+        <v>-6259</v>
       </c>
       <c r="D38" t="n">
         <v>59510</v>
       </c>
       <c r="E38" t="n">
-        <v>9963</v>
+        <v>65769</v>
       </c>
     </row>
     <row r="39">
@@ -1050,13 +1050,13 @@
         <v>2036</v>
       </c>
       <c r="C39" t="n">
-        <v>49711</v>
+        <v>-6290</v>
       </c>
       <c r="D39" t="n">
         <v>59678</v>
       </c>
       <c r="E39" t="n">
-        <v>9967</v>
+        <v>65967</v>
       </c>
     </row>
     <row r="40">
@@ -1065,13 +1065,13 @@
         <v>2037</v>
       </c>
       <c r="C40" t="n">
-        <v>49919</v>
+        <v>-6326</v>
       </c>
       <c r="D40" t="n">
         <v>59837</v>
       </c>
       <c r="E40" t="n">
-        <v>9918</v>
+        <v>66163</v>
       </c>
     </row>
     <row r="41">
@@ -1080,13 +1080,13 @@
         <v>2038</v>
       </c>
       <c r="C41" t="n">
-        <v>50169</v>
+        <v>-6370</v>
       </c>
       <c r="D41" t="n">
         <v>59992</v>
       </c>
       <c r="E41" t="n">
-        <v>9823</v>
+        <v>66362</v>
       </c>
     </row>
     <row r="42">
@@ -1095,13 +1095,13 @@
         <v>2039</v>
       </c>
       <c r="C42" t="n">
-        <v>50466</v>
+        <v>-6424</v>
       </c>
       <c r="D42" t="n">
         <v>60171</v>
       </c>
       <c r="E42" t="n">
-        <v>9705</v>
+        <v>66595</v>
       </c>
     </row>
     <row r="43">
@@ -1110,13 +1110,13 @@
         <v>2040</v>
       </c>
       <c r="C43" t="n">
-        <v>50777</v>
+        <v>-6481</v>
       </c>
       <c r="D43" t="n">
         <v>60363</v>
       </c>
       <c r="E43" t="n">
-        <v>9585</v>
+        <v>66843</v>
       </c>
     </row>
     <row r="44">
@@ -1129,13 +1129,13 @@
         <v>2020</v>
       </c>
       <c r="C44" t="n">
-        <v>16556</v>
+        <v>-3255</v>
       </c>
       <c r="D44" t="n">
         <v>16557</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>19812</v>
       </c>
     </row>
     <row r="45">
@@ -1144,13 +1144,13 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>16581</v>
+        <v>-3265</v>
       </c>
       <c r="D45" t="n">
         <v>17578</v>
       </c>
       <c r="E45" t="n">
-        <v>997</v>
+        <v>20843</v>
       </c>
     </row>
     <row r="46">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>16636</v>
+        <v>-3288</v>
       </c>
       <c r="D46" t="n">
         <v>18646</v>
       </c>
       <c r="E46" t="n">
-        <v>2010</v>
+        <v>21933</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>16655</v>
+        <v>-3323</v>
       </c>
       <c r="D47" t="n">
         <v>19744</v>
       </c>
       <c r="E47" t="n">
-        <v>3089</v>
+        <v>23067</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>16666</v>
+        <v>-3351</v>
       </c>
       <c r="D48" t="n">
         <v>20844</v>
       </c>
       <c r="E48" t="n">
-        <v>4178</v>
+        <v>24195</v>
       </c>
     </row>
     <row r="49">
@@ -1204,13 +1204,13 @@
         <v>2025</v>
       </c>
       <c r="C49" t="n">
-        <v>16664</v>
+        <v>-3398</v>
       </c>
       <c r="D49" t="n">
         <v>21946</v>
       </c>
       <c r="E49" t="n">
-        <v>5282</v>
+        <v>25344</v>
       </c>
     </row>
     <row r="50">
@@ -1219,13 +1219,13 @@
         <v>2026</v>
       </c>
       <c r="C50" t="n">
-        <v>16651</v>
+        <v>-3445</v>
       </c>
       <c r="D50" t="n">
         <v>23028</v>
       </c>
       <c r="E50" t="n">
-        <v>6377</v>
+        <v>26472</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>16637</v>
+        <v>-3470</v>
       </c>
       <c r="D51" t="n">
         <v>24099</v>
       </c>
       <c r="E51" t="n">
-        <v>7461</v>
+        <v>27568</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>16616</v>
+        <v>-3446</v>
       </c>
       <c r="D52" t="n">
         <v>25140</v>
       </c>
       <c r="E52" t="n">
-        <v>8524</v>
+        <v>28586</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>16590</v>
+        <v>-3405</v>
       </c>
       <c r="D53" t="n">
         <v>26167</v>
       </c>
       <c r="E53" t="n">
-        <v>9577</v>
+        <v>29572</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1279,13 @@
         <v>2030</v>
       </c>
       <c r="C54" t="n">
-        <v>16574</v>
+        <v>-3352</v>
       </c>
       <c r="D54" t="n">
         <v>27160</v>
       </c>
       <c r="E54" t="n">
-        <v>10587</v>
+        <v>30512</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>16565</v>
+        <v>-3313</v>
       </c>
       <c r="D55" t="n">
         <v>28119</v>
       </c>
       <c r="E55" t="n">
-        <v>11554</v>
+        <v>31433</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>16565</v>
+        <v>-3283</v>
       </c>
       <c r="D56" t="n">
         <v>29053</v>
       </c>
       <c r="E56" t="n">
-        <v>12488</v>
+        <v>32337</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>16575</v>
+        <v>-3269</v>
       </c>
       <c r="D57" t="n">
         <v>29967</v>
       </c>
       <c r="E57" t="n">
-        <v>13392</v>
+        <v>33236</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>16591</v>
+        <v>-3221</v>
       </c>
       <c r="D58" t="n">
         <v>30877</v>
       </c>
       <c r="E58" t="n">
-        <v>14286</v>
+        <v>34098</v>
       </c>
     </row>
     <row r="59">
@@ -1354,13 +1354,13 @@
         <v>2035</v>
       </c>
       <c r="C59" t="n">
-        <v>16613</v>
+        <v>-3154</v>
       </c>
       <c r="D59" t="n">
         <v>31772</v>
       </c>
       <c r="E59" t="n">
-        <v>15159</v>
+        <v>34926</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>16643</v>
+        <v>-3091</v>
       </c>
       <c r="D60" t="n">
         <v>32648</v>
       </c>
       <c r="E60" t="n">
-        <v>16004</v>
+        <v>35739</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>16689</v>
+        <v>-3061</v>
       </c>
       <c r="D61" t="n">
         <v>33520</v>
       </c>
       <c r="E61" t="n">
-        <v>16831</v>
+        <v>36580</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>16744</v>
+        <v>-3047</v>
       </c>
       <c r="D62" t="n">
         <v>34393</v>
       </c>
       <c r="E62" t="n">
-        <v>17648</v>
+        <v>37440</v>
       </c>
     </row>
     <row r="63">
@@ -1414,13 +1414,13 @@
         <v>2039</v>
       </c>
       <c r="C63" t="n">
-        <v>16804</v>
+        <v>-3035</v>
       </c>
       <c r="D63" t="n">
         <v>35263</v>
       </c>
       <c r="E63" t="n">
-        <v>18459</v>
+        <v>38298</v>
       </c>
     </row>
     <row r="64">
@@ -1429,13 +1429,13 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>16866</v>
+        <v>-3031</v>
       </c>
       <c r="D64" t="n">
         <v>36117</v>
       </c>
       <c r="E64" t="n">
-        <v>19251</v>
+        <v>39148</v>
       </c>
     </row>
     <row r="65">
@@ -1448,13 +1448,13 @@
         <v>2020</v>
       </c>
       <c r="C65" t="n">
-        <v>30732</v>
+        <v>-5960</v>
       </c>
       <c r="D65" t="n">
         <v>30732</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>36692</v>
       </c>
     </row>
     <row r="66">
@@ -1463,13 +1463,13 @@
         <v>2021</v>
       </c>
       <c r="C66" t="n">
-        <v>30821</v>
+        <v>-5927</v>
       </c>
       <c r="D66" t="n">
         <v>30793</v>
       </c>
       <c r="E66" t="n">
-        <v>-28</v>
+        <v>36720</v>
       </c>
     </row>
     <row r="67">
@@ -1478,13 +1478,13 @@
         <v>2022</v>
       </c>
       <c r="C67" t="n">
-        <v>30975</v>
+        <v>-5912</v>
       </c>
       <c r="D67" t="n">
         <v>30889</v>
       </c>
       <c r="E67" t="n">
-        <v>-86</v>
+        <v>36801</v>
       </c>
     </row>
     <row r="68">
@@ -1493,13 +1493,13 @@
         <v>2023</v>
       </c>
       <c r="C68" t="n">
-        <v>31104</v>
+        <v>-5877</v>
       </c>
       <c r="D68" t="n">
         <v>31004</v>
       </c>
       <c r="E68" t="n">
-        <v>-100</v>
+        <v>36881</v>
       </c>
     </row>
     <row r="69">
@@ -1508,13 +1508,13 @@
         <v>2024</v>
       </c>
       <c r="C69" t="n">
-        <v>31186</v>
+        <v>-5859</v>
       </c>
       <c r="D69" t="n">
         <v>31129</v>
       </c>
       <c r="E69" t="n">
-        <v>-57</v>
+        <v>36988</v>
       </c>
     </row>
     <row r="70">
@@ -1523,13 +1523,13 @@
         <v>2025</v>
       </c>
       <c r="C70" t="n">
-        <v>31277</v>
+        <v>-5847</v>
       </c>
       <c r="D70" t="n">
         <v>31256</v>
       </c>
       <c r="E70" t="n">
-        <v>-21</v>
+        <v>37103</v>
       </c>
     </row>
     <row r="71">
@@ -1538,13 +1538,13 @@
         <v>2026</v>
       </c>
       <c r="C71" t="n">
-        <v>31334</v>
+        <v>-5848</v>
       </c>
       <c r="D71" t="n">
         <v>31384</v>
       </c>
       <c r="E71" t="n">
-        <v>49</v>
+        <v>37232</v>
       </c>
     </row>
     <row r="72">
@@ -1553,13 +1553,13 @@
         <v>2027</v>
       </c>
       <c r="C72" t="n">
-        <v>31338</v>
+        <v>-5857</v>
       </c>
       <c r="D72" t="n">
         <v>31496</v>
       </c>
       <c r="E72" t="n">
-        <v>158</v>
+        <v>37353</v>
       </c>
     </row>
     <row r="73">
@@ -1568,13 +1568,13 @@
         <v>2028</v>
       </c>
       <c r="C73" t="n">
-        <v>31213</v>
+        <v>-5881</v>
       </c>
       <c r="D73" t="n">
         <v>31593</v>
       </c>
       <c r="E73" t="n">
-        <v>380</v>
+        <v>37474</v>
       </c>
     </row>
     <row r="74">
@@ -1583,13 +1583,13 @@
         <v>2029</v>
       </c>
       <c r="C74" t="n">
-        <v>31036</v>
+        <v>-5913</v>
       </c>
       <c r="D74" t="n">
         <v>31671</v>
       </c>
       <c r="E74" t="n">
-        <v>636</v>
+        <v>37584</v>
       </c>
     </row>
     <row r="75">
@@ -1598,13 +1598,13 @@
         <v>2030</v>
       </c>
       <c r="C75" t="n">
-        <v>30852</v>
+        <v>-5945</v>
       </c>
       <c r="D75" t="n">
         <v>31716</v>
       </c>
       <c r="E75" t="n">
-        <v>864</v>
+        <v>37661</v>
       </c>
     </row>
     <row r="76">
@@ -1613,13 +1613,13 @@
         <v>2031</v>
       </c>
       <c r="C76" t="n">
-        <v>30725</v>
+        <v>-5964</v>
       </c>
       <c r="D76" t="n">
         <v>31725</v>
       </c>
       <c r="E76" t="n">
-        <v>999</v>
+        <v>37688</v>
       </c>
     </row>
     <row r="77">
@@ -1628,13 +1628,13 @@
         <v>2032</v>
       </c>
       <c r="C77" t="n">
-        <v>30641</v>
+        <v>-5969</v>
       </c>
       <c r="D77" t="n">
         <v>31698</v>
       </c>
       <c r="E77" t="n">
-        <v>1057</v>
+        <v>37667</v>
       </c>
     </row>
     <row r="78">
@@ -1643,13 +1643,13 @@
         <v>2033</v>
       </c>
       <c r="C78" t="n">
-        <v>30624</v>
+        <v>-5957</v>
       </c>
       <c r="D78" t="n">
         <v>31632</v>
       </c>
       <c r="E78" t="n">
-        <v>1008</v>
+        <v>37589</v>
       </c>
     </row>
     <row r="79">
@@ -1658,13 +1658,13 @@
         <v>2034</v>
       </c>
       <c r="C79" t="n">
-        <v>30558</v>
+        <v>-5933</v>
       </c>
       <c r="D79" t="n">
         <v>31552</v>
       </c>
       <c r="E79" t="n">
-        <v>993</v>
+        <v>37485</v>
       </c>
     </row>
     <row r="80">
@@ -1673,13 +1673,13 @@
         <v>2035</v>
       </c>
       <c r="C80" t="n">
-        <v>30469</v>
+        <v>-5902</v>
       </c>
       <c r="D80" t="n">
         <v>31437</v>
       </c>
       <c r="E80" t="n">
-        <v>967</v>
+        <v>37338</v>
       </c>
     </row>
     <row r="81">
@@ -1688,13 +1688,13 @@
         <v>2036</v>
       </c>
       <c r="C81" t="n">
-        <v>30408</v>
+        <v>-5868</v>
       </c>
       <c r="D81" t="n">
         <v>31321</v>
       </c>
       <c r="E81" t="n">
-        <v>913</v>
+        <v>37189</v>
       </c>
     </row>
     <row r="82">
@@ -1703,13 +1703,13 @@
         <v>2037</v>
       </c>
       <c r="C82" t="n">
-        <v>30450</v>
+        <v>-5826</v>
       </c>
       <c r="D82" t="n">
         <v>31189</v>
       </c>
       <c r="E82" t="n">
-        <v>739</v>
+        <v>37016</v>
       </c>
     </row>
     <row r="83">
@@ -1718,13 +1718,13 @@
         <v>2038</v>
       </c>
       <c r="C83" t="n">
-        <v>30553</v>
+        <v>-5777</v>
       </c>
       <c r="D83" t="n">
         <v>31068</v>
       </c>
       <c r="E83" t="n">
-        <v>516</v>
+        <v>36845</v>
       </c>
     </row>
     <row r="84">
@@ -1733,13 +1733,13 @@
         <v>2039</v>
       </c>
       <c r="C84" t="n">
-        <v>30676</v>
+        <v>-5717</v>
       </c>
       <c r="D84" t="n">
         <v>30946</v>
       </c>
       <c r="E84" t="n">
-        <v>270</v>
+        <v>36663</v>
       </c>
     </row>
     <row r="85">
@@ -1748,13 +1748,13 @@
         <v>2040</v>
       </c>
       <c r="C85" t="n">
-        <v>30821</v>
+        <v>-5657</v>
       </c>
       <c r="D85" t="n">
         <v>30834</v>
       </c>
       <c r="E85" t="n">
-        <v>13</v>
+        <v>36491</v>
       </c>
     </row>
     <row r="86">
@@ -1767,13 +1767,13 @@
         <v>2020</v>
       </c>
       <c r="C86" t="n">
-        <v>13249</v>
+        <v>-2863</v>
       </c>
       <c r="D86" t="n">
         <v>13248</v>
       </c>
       <c r="E86" t="n">
-        <v>-1</v>
+        <v>16111</v>
       </c>
     </row>
     <row r="87">
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>13275</v>
+        <v>-2876</v>
       </c>
       <c r="D87" t="n">
         <v>13226</v>
       </c>
       <c r="E87" t="n">
-        <v>-50</v>
+        <v>16101</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>13336</v>
+        <v>-2894</v>
       </c>
       <c r="D88" t="n">
         <v>13190</v>
       </c>
       <c r="E88" t="n">
-        <v>-146</v>
+        <v>16084</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>13396</v>
+        <v>-2904</v>
       </c>
       <c r="D89" t="n">
         <v>13140</v>
       </c>
       <c r="E89" t="n">
-        <v>-256</v>
+        <v>16044</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>13442</v>
+        <v>-2919</v>
       </c>
       <c r="D90" t="n">
         <v>13091</v>
       </c>
       <c r="E90" t="n">
-        <v>-351</v>
+        <v>16010</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>13513</v>
+        <v>-2933</v>
       </c>
       <c r="D91" t="n">
         <v>13024</v>
       </c>
       <c r="E91" t="n">
-        <v>-489</v>
+        <v>15957</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>13578</v>
+        <v>-2947</v>
       </c>
       <c r="D92" t="n">
         <v>12945</v>
       </c>
       <c r="E92" t="n">
-        <v>-634</v>
+        <v>15892</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>13612</v>
+        <v>-2961</v>
       </c>
       <c r="D93" t="n">
         <v>12865</v>
       </c>
       <c r="E93" t="n">
-        <v>-746</v>
+        <v>15827</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>13570</v>
+        <v>-2975</v>
       </c>
       <c r="D94" t="n">
         <v>12763</v>
       </c>
       <c r="E94" t="n">
-        <v>-807</v>
+        <v>15738</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>13502</v>
+        <v>-2989</v>
       </c>
       <c r="D95" t="n">
         <v>12664</v>
       </c>
       <c r="E95" t="n">
-        <v>-838</v>
+        <v>15652</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>13420</v>
+        <v>-3002</v>
       </c>
       <c r="D96" t="n">
         <v>12555</v>
       </c>
       <c r="E96" t="n">
-        <v>-864</v>
+        <v>15558</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>13362</v>
+        <v>-3016</v>
       </c>
       <c r="D97" t="n">
         <v>12434</v>
       </c>
       <c r="E97" t="n">
-        <v>-927</v>
+        <v>15450</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>13318</v>
+        <v>-3029</v>
       </c>
       <c r="D98" t="n">
         <v>12320</v>
       </c>
       <c r="E98" t="n">
-        <v>-997</v>
+        <v>15349</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>13301</v>
+        <v>-3042</v>
       </c>
       <c r="D99" t="n">
         <v>12191</v>
       </c>
       <c r="E99" t="n">
-        <v>-1110</v>
+        <v>15233</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>13235</v>
+        <v>-3054</v>
       </c>
       <c r="D100" t="n">
         <v>12080</v>
       </c>
       <c r="E100" t="n">
-        <v>-1156</v>
+        <v>15134</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>13143</v>
+        <v>-3067</v>
       </c>
       <c r="D101" t="n">
         <v>11961</v>
       </c>
       <c r="E101" t="n">
-        <v>-1182</v>
+        <v>15028</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>13061</v>
+        <v>-3079</v>
       </c>
       <c r="D102" t="n">
         <v>11852</v>
       </c>
       <c r="E102" t="n">
-        <v>-1209</v>
+        <v>14931</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>13033</v>
+        <v>-3091</v>
       </c>
       <c r="D103" t="n">
         <v>11748</v>
       </c>
       <c r="E103" t="n">
-        <v>-1285</v>
+        <v>14839</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>13033</v>
+        <v>-3102</v>
       </c>
       <c r="D104" t="n">
         <v>11634</v>
       </c>
       <c r="E104" t="n">
-        <v>-1399</v>
+        <v>14736</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>13037</v>
+        <v>-3113</v>
       </c>
       <c r="D105" t="n">
         <v>11541</v>
       </c>
       <c r="E105" t="n">
-        <v>-1496</v>
+        <v>14654</v>
       </c>
     </row>
     <row r="106">
@@ -2067,13 +2067,13 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
-        <v>13053</v>
+        <v>-3123</v>
       </c>
       <c r="D106" t="n">
         <v>11443</v>
       </c>
       <c r="E106" t="n">
-        <v>-1611</v>
+        <v>14566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lagt til alternativ for ingen vakanse.
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -506,13 +506,13 @@
         <v>2021</v>
       </c>
       <c r="C3" t="n">
-        <v>46632</v>
+        <v>46514</v>
       </c>
       <c r="D3" t="n">
         <v>48005</v>
       </c>
       <c r="E3" t="n">
-        <v>1373</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="4">
@@ -521,13 +521,13 @@
         <v>2022</v>
       </c>
       <c r="C4" t="n">
-        <v>46204</v>
+        <v>45964</v>
       </c>
       <c r="D4" t="n">
         <v>49054</v>
       </c>
       <c r="E4" t="n">
-        <v>2851</v>
+        <v>3090</v>
       </c>
     </row>
     <row r="5">
@@ -536,13 +536,13 @@
         <v>2023</v>
       </c>
       <c r="C5" t="n">
-        <v>46086</v>
+        <v>45811</v>
       </c>
       <c r="D5" t="n">
         <v>50111</v>
       </c>
       <c r="E5" t="n">
-        <v>4025</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="6">
@@ -551,13 +551,13 @@
         <v>2024</v>
       </c>
       <c r="C6" t="n">
-        <v>45874</v>
+        <v>45543</v>
       </c>
       <c r="D6" t="n">
         <v>51173</v>
       </c>
       <c r="E6" t="n">
-        <v>5298</v>
+        <v>5630</v>
       </c>
     </row>
     <row r="7">
@@ -566,13 +566,13 @@
         <v>2025</v>
       </c>
       <c r="C7" t="n">
-        <v>45756</v>
+        <v>45395</v>
       </c>
       <c r="D7" t="n">
         <v>52232</v>
       </c>
       <c r="E7" t="n">
-        <v>6476</v>
+        <v>6836</v>
       </c>
     </row>
     <row r="8">
@@ -581,13 +581,13 @@
         <v>2026</v>
       </c>
       <c r="C8" t="n">
-        <v>45706</v>
+        <v>45335</v>
       </c>
       <c r="D8" t="n">
         <v>53290</v>
       </c>
       <c r="E8" t="n">
-        <v>7584</v>
+        <v>7955</v>
       </c>
     </row>
     <row r="9">
@@ -596,13 +596,13 @@
         <v>2027</v>
       </c>
       <c r="C9" t="n">
-        <v>45740</v>
+        <v>45373</v>
       </c>
       <c r="D9" t="n">
         <v>54322</v>
       </c>
       <c r="E9" t="n">
-        <v>8581</v>
+        <v>8949</v>
       </c>
     </row>
     <row r="10">
@@ -611,13 +611,13 @@
         <v>2028</v>
       </c>
       <c r="C10" t="n">
-        <v>45850</v>
+        <v>45497</v>
       </c>
       <c r="D10" t="n">
         <v>55327</v>
       </c>
       <c r="E10" t="n">
-        <v>9476</v>
+        <v>9830</v>
       </c>
     </row>
     <row r="11">
@@ -626,13 +626,13 @@
         <v>2029</v>
       </c>
       <c r="C11" t="n">
-        <v>46028</v>
+        <v>45701</v>
       </c>
       <c r="D11" t="n">
         <v>56273</v>
       </c>
       <c r="E11" t="n">
-        <v>10245</v>
+        <v>10572</v>
       </c>
     </row>
     <row r="12">
@@ -641,13 +641,13 @@
         <v>2030</v>
       </c>
       <c r="C12" t="n">
-        <v>46237</v>
+        <v>45938</v>
       </c>
       <c r="D12" t="n">
         <v>57142</v>
       </c>
       <c r="E12" t="n">
-        <v>10905</v>
+        <v>11204</v>
       </c>
     </row>
     <row r="13">
@@ -656,13 +656,13 @@
         <v>2031</v>
       </c>
       <c r="C13" t="n">
-        <v>46459</v>
+        <v>46188</v>
       </c>
       <c r="D13" t="n">
         <v>57935</v>
       </c>
       <c r="E13" t="n">
-        <v>11476</v>
+        <v>11747</v>
       </c>
     </row>
     <row r="14">
@@ -671,13 +671,13 @@
         <v>2032</v>
       </c>
       <c r="C14" t="n">
-        <v>46681</v>
+        <v>46436</v>
       </c>
       <c r="D14" t="n">
         <v>58628</v>
       </c>
       <c r="E14" t="n">
-        <v>11948</v>
+        <v>12192</v>
       </c>
     </row>
     <row r="15">
@@ -686,13 +686,13 @@
         <v>2033</v>
       </c>
       <c r="C15" t="n">
-        <v>46909</v>
+        <v>46690</v>
       </c>
       <c r="D15" t="n">
         <v>59227</v>
       </c>
       <c r="E15" t="n">
-        <v>12318</v>
+        <v>12536</v>
       </c>
     </row>
     <row r="16">
@@ -701,13 +701,13 @@
         <v>2034</v>
       </c>
       <c r="C16" t="n">
-        <v>47175</v>
+        <v>46981</v>
       </c>
       <c r="D16" t="n">
         <v>59747</v>
       </c>
       <c r="E16" t="n">
-        <v>12573</v>
+        <v>12766</v>
       </c>
     </row>
     <row r="17">
@@ -716,13 +716,13 @@
         <v>2035</v>
       </c>
       <c r="C17" t="n">
-        <v>47470</v>
+        <v>47303</v>
       </c>
       <c r="D17" t="n">
         <v>60180</v>
       </c>
       <c r="E17" t="n">
-        <v>12710</v>
+        <v>12878</v>
       </c>
     </row>
     <row r="18">
@@ -731,13 +731,13 @@
         <v>2036</v>
       </c>
       <c r="C18" t="n">
-        <v>47788</v>
+        <v>47647</v>
       </c>
       <c r="D18" t="n">
         <v>60568</v>
       </c>
       <c r="E18" t="n">
-        <v>12781</v>
+        <v>12921</v>
       </c>
     </row>
     <row r="19">
@@ -746,13 +746,13 @@
         <v>2037</v>
       </c>
       <c r="C19" t="n">
-        <v>48120</v>
+        <v>48009</v>
       </c>
       <c r="D19" t="n">
         <v>60935</v>
       </c>
       <c r="E19" t="n">
-        <v>12814</v>
+        <v>12926</v>
       </c>
     </row>
     <row r="20">
@@ -761,13 +761,13 @@
         <v>2038</v>
       </c>
       <c r="C20" t="n">
-        <v>48432</v>
+        <v>48343</v>
       </c>
       <c r="D20" t="n">
         <v>61312</v>
       </c>
       <c r="E20" t="n">
-        <v>12880</v>
+        <v>12968</v>
       </c>
     </row>
     <row r="21">
@@ -776,13 +776,13 @@
         <v>2039</v>
       </c>
       <c r="C21" t="n">
-        <v>48682</v>
+        <v>48604</v>
       </c>
       <c r="D21" t="n">
         <v>61717</v>
       </c>
       <c r="E21" t="n">
-        <v>13035</v>
+        <v>13113</v>
       </c>
     </row>
     <row r="22">
@@ -791,13 +791,13 @@
         <v>2040</v>
       </c>
       <c r="C22" t="n">
-        <v>48869</v>
+        <v>48789</v>
       </c>
       <c r="D22" t="n">
         <v>62174</v>
       </c>
       <c r="E22" t="n">
-        <v>13306</v>
+        <v>13385</v>
       </c>
     </row>
     <row r="23">
@@ -825,13 +825,13 @@
         <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>52370</v>
+        <v>52344</v>
       </c>
       <c r="D24" t="n">
         <v>52772</v>
       </c>
       <c r="E24" t="n">
-        <v>402</v>
+        <v>428</v>
       </c>
     </row>
     <row r="25">
@@ -840,13 +840,13 @@
         <v>2022</v>
       </c>
       <c r="C25" t="n">
-        <v>52430</v>
+        <v>52374</v>
       </c>
       <c r="D25" t="n">
         <v>53230</v>
       </c>
       <c r="E25" t="n">
-        <v>800</v>
+        <v>857</v>
       </c>
     </row>
     <row r="26">
@@ -855,13 +855,13 @@
         <v>2023</v>
       </c>
       <c r="C26" t="n">
-        <v>52329</v>
+        <v>52235</v>
       </c>
       <c r="D26" t="n">
         <v>53746</v>
       </c>
       <c r="E26" t="n">
-        <v>1416</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="27">
@@ -870,13 +870,13 @@
         <v>2024</v>
       </c>
       <c r="C27" t="n">
-        <v>52127</v>
+        <v>51975</v>
       </c>
       <c r="D27" t="n">
         <v>54316</v>
       </c>
       <c r="E27" t="n">
-        <v>2189</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="28">
@@ -885,13 +885,13 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>51767</v>
+        <v>51531</v>
       </c>
       <c r="D28" t="n">
         <v>54926</v>
       </c>
       <c r="E28" t="n">
-        <v>3159</v>
+        <v>3395</v>
       </c>
     </row>
     <row r="29">
@@ -900,13 +900,13 @@
         <v>2026</v>
       </c>
       <c r="C29" t="n">
-        <v>51321</v>
+        <v>50990</v>
       </c>
       <c r="D29" t="n">
         <v>55541</v>
       </c>
       <c r="E29" t="n">
-        <v>4219</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="30">
@@ -915,13 +915,13 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>50918</v>
+        <v>50499</v>
       </c>
       <c r="D30" t="n">
         <v>56186</v>
       </c>
       <c r="E30" t="n">
-        <v>5269</v>
+        <v>5687</v>
       </c>
     </row>
     <row r="31">
@@ -930,13 +930,13 @@
         <v>2028</v>
       </c>
       <c r="C31" t="n">
-        <v>50561</v>
+        <v>50066</v>
       </c>
       <c r="D31" t="n">
         <v>56811</v>
       </c>
       <c r="E31" t="n">
-        <v>6250</v>
+        <v>6744</v>
       </c>
     </row>
     <row r="32">
@@ -945,13 +945,13 @@
         <v>2029</v>
       </c>
       <c r="C32" t="n">
-        <v>50199</v>
+        <v>49630</v>
       </c>
       <c r="D32" t="n">
         <v>57397</v>
       </c>
       <c r="E32" t="n">
-        <v>7198</v>
+        <v>7767</v>
       </c>
     </row>
     <row r="33">
@@ -960,13 +960,13 @@
         <v>2030</v>
       </c>
       <c r="C33" t="n">
-        <v>49939</v>
+        <v>49310</v>
       </c>
       <c r="D33" t="n">
         <v>57919</v>
       </c>
       <c r="E33" t="n">
-        <v>7980</v>
+        <v>8609</v>
       </c>
     </row>
     <row r="34">
@@ -975,13 +975,13 @@
         <v>2031</v>
       </c>
       <c r="C34" t="n">
-        <v>49717</v>
+        <v>49033</v>
       </c>
       <c r="D34" t="n">
         <v>58381</v>
       </c>
       <c r="E34" t="n">
-        <v>8665</v>
+        <v>9349</v>
       </c>
     </row>
     <row r="35">
@@ -990,13 +990,13 @@
         <v>2032</v>
       </c>
       <c r="C35" t="n">
-        <v>49544</v>
+        <v>48813</v>
       </c>
       <c r="D35" t="n">
         <v>58767</v>
       </c>
       <c r="E35" t="n">
-        <v>9223</v>
+        <v>9954</v>
       </c>
     </row>
     <row r="36">
@@ -1005,13 +1005,13 @@
         <v>2033</v>
       </c>
       <c r="C36" t="n">
-        <v>49425</v>
+        <v>48652</v>
       </c>
       <c r="D36" t="n">
         <v>59072</v>
       </c>
       <c r="E36" t="n">
-        <v>9648</v>
+        <v>10420</v>
       </c>
     </row>
     <row r="37">
@@ -1020,13 +1020,13 @@
         <v>2034</v>
       </c>
       <c r="C37" t="n">
-        <v>49440</v>
+        <v>48651</v>
       </c>
       <c r="D37" t="n">
         <v>59320</v>
       </c>
       <c r="E37" t="n">
-        <v>9879</v>
+        <v>10669</v>
       </c>
     </row>
     <row r="38">
@@ -1035,13 +1035,13 @@
         <v>2035</v>
       </c>
       <c r="C38" t="n">
-        <v>49547</v>
+        <v>48756</v>
       </c>
       <c r="D38" t="n">
         <v>59510</v>
       </c>
       <c r="E38" t="n">
-        <v>9963</v>
+        <v>10754</v>
       </c>
     </row>
     <row r="39">
@@ -1050,13 +1050,13 @@
         <v>2036</v>
       </c>
       <c r="C39" t="n">
-        <v>49711</v>
+        <v>48927</v>
       </c>
       <c r="D39" t="n">
         <v>59678</v>
       </c>
       <c r="E39" t="n">
-        <v>9966</v>
+        <v>10751</v>
       </c>
     </row>
     <row r="40">
@@ -1065,13 +1065,13 @@
         <v>2037</v>
       </c>
       <c r="C40" t="n">
-        <v>49919</v>
+        <v>49144</v>
       </c>
       <c r="D40" t="n">
         <v>59837</v>
       </c>
       <c r="E40" t="n">
-        <v>9918</v>
+        <v>10693</v>
       </c>
     </row>
     <row r="41">
@@ -1080,13 +1080,13 @@
         <v>2038</v>
       </c>
       <c r="C41" t="n">
-        <v>50169</v>
+        <v>49409</v>
       </c>
       <c r="D41" t="n">
         <v>59992</v>
       </c>
       <c r="E41" t="n">
-        <v>9823</v>
+        <v>10583</v>
       </c>
     </row>
     <row r="42">
@@ -1095,13 +1095,13 @@
         <v>2039</v>
       </c>
       <c r="C42" t="n">
-        <v>50466</v>
+        <v>49728</v>
       </c>
       <c r="D42" t="n">
         <v>60171</v>
       </c>
       <c r="E42" t="n">
-        <v>9705</v>
+        <v>10442</v>
       </c>
     </row>
     <row r="43">
@@ -1110,13 +1110,13 @@
         <v>2040</v>
       </c>
       <c r="C43" t="n">
-        <v>50778</v>
+        <v>50065</v>
       </c>
       <c r="D43" t="n">
         <v>60363</v>
       </c>
       <c r="E43" t="n">
-        <v>9585</v>
+        <v>10298</v>
       </c>
     </row>
     <row r="44">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>16637</v>
+        <v>16643</v>
       </c>
       <c r="D46" t="n">
         <v>18646</v>
       </c>
       <c r="E46" t="n">
-        <v>2009</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>16656</v>
+        <v>16688</v>
       </c>
       <c r="D47" t="n">
         <v>19744</v>
       </c>
       <c r="E47" t="n">
-        <v>3088</v>
+        <v>3056</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>16667</v>
+        <v>16715</v>
       </c>
       <c r="D48" t="n">
         <v>20844</v>
       </c>
       <c r="E48" t="n">
-        <v>4177</v>
+        <v>4130</v>
       </c>
     </row>
     <row r="49">
@@ -1204,13 +1204,13 @@
         <v>2025</v>
       </c>
       <c r="C49" t="n">
-        <v>16664</v>
+        <v>16747</v>
       </c>
       <c r="D49" t="n">
         <v>21946</v>
       </c>
       <c r="E49" t="n">
-        <v>5281</v>
+        <v>5199</v>
       </c>
     </row>
     <row r="50">
@@ -1219,13 +1219,13 @@
         <v>2026</v>
       </c>
       <c r="C50" t="n">
-        <v>16651</v>
+        <v>16769</v>
       </c>
       <c r="D50" t="n">
         <v>23028</v>
       </c>
       <c r="E50" t="n">
-        <v>6376</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>16638</v>
+        <v>16769</v>
       </c>
       <c r="D51" t="n">
         <v>24099</v>
       </c>
       <c r="E51" t="n">
-        <v>7460</v>
+        <v>7329</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>16617</v>
+        <v>16717</v>
       </c>
       <c r="D52" t="n">
         <v>25140</v>
       </c>
       <c r="E52" t="n">
-        <v>8523</v>
+        <v>8423</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>16591</v>
+        <v>16644</v>
       </c>
       <c r="D53" t="n">
         <v>26167</v>
       </c>
       <c r="E53" t="n">
-        <v>9576</v>
+        <v>9523</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1279,13 @@
         <v>2030</v>
       </c>
       <c r="C54" t="n">
-        <v>16574</v>
+        <v>16569</v>
       </c>
       <c r="D54" t="n">
         <v>27160</v>
       </c>
       <c r="E54" t="n">
-        <v>10586</v>
+        <v>10592</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>16566</v>
+        <v>16516</v>
       </c>
       <c r="D55" t="n">
         <v>28119</v>
       </c>
       <c r="E55" t="n">
-        <v>11553</v>
+        <v>11604</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>16566</v>
+        <v>16478</v>
       </c>
       <c r="D56" t="n">
         <v>29053</v>
       </c>
       <c r="E56" t="n">
-        <v>12488</v>
+        <v>12576</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>16576</v>
+        <v>16465</v>
       </c>
       <c r="D57" t="n">
         <v>29967</v>
       </c>
       <c r="E57" t="n">
-        <v>13392</v>
+        <v>13502</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>16592</v>
+        <v>16427</v>
       </c>
       <c r="D58" t="n">
         <v>30877</v>
       </c>
       <c r="E58" t="n">
-        <v>14285</v>
+        <v>14450</v>
       </c>
     </row>
     <row r="59">
@@ -1354,13 +1354,13 @@
         <v>2035</v>
       </c>
       <c r="C59" t="n">
-        <v>16613</v>
+        <v>16377</v>
       </c>
       <c r="D59" t="n">
         <v>31772</v>
       </c>
       <c r="E59" t="n">
-        <v>15159</v>
+        <v>15395</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>16644</v>
+        <v>16340</v>
       </c>
       <c r="D60" t="n">
         <v>32648</v>
       </c>
       <c r="E60" t="n">
-        <v>16004</v>
+        <v>16308</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>16690</v>
+        <v>16347</v>
       </c>
       <c r="D61" t="n">
         <v>33520</v>
       </c>
       <c r="E61" t="n">
-        <v>16830</v>
+        <v>17172</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>16745</v>
+        <v>16380</v>
       </c>
       <c r="D62" t="n">
         <v>34393</v>
       </c>
       <c r="E62" t="n">
-        <v>17648</v>
+        <v>18013</v>
       </c>
     </row>
     <row r="63">
@@ -1414,13 +1414,13 @@
         <v>2039</v>
       </c>
       <c r="C63" t="n">
-        <v>16804</v>
+        <v>16419</v>
       </c>
       <c r="D63" t="n">
         <v>35263</v>
       </c>
       <c r="E63" t="n">
-        <v>18458</v>
+        <v>18844</v>
       </c>
     </row>
     <row r="64">
@@ -1429,13 +1429,13 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>16867</v>
+        <v>16468</v>
       </c>
       <c r="D64" t="n">
         <v>36117</v>
       </c>
       <c r="E64" t="n">
-        <v>19250</v>
+        <v>19649</v>
       </c>
     </row>
     <row r="65">
@@ -1463,13 +1463,13 @@
         <v>2021</v>
       </c>
       <c r="C66" t="n">
-        <v>30821</v>
+        <v>30773</v>
       </c>
       <c r="D66" t="n">
         <v>30793</v>
       </c>
       <c r="E66" t="n">
-        <v>-28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67">
@@ -1478,13 +1478,13 @@
         <v>2022</v>
       </c>
       <c r="C67" t="n">
-        <v>30975</v>
+        <v>30884</v>
       </c>
       <c r="D67" t="n">
         <v>30889</v>
       </c>
       <c r="E67" t="n">
-        <v>-86</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68">
@@ -1493,13 +1493,13 @@
         <v>2023</v>
       </c>
       <c r="C68" t="n">
-        <v>31104</v>
+        <v>30964</v>
       </c>
       <c r="D68" t="n">
         <v>31004</v>
       </c>
       <c r="E68" t="n">
-        <v>-100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="69">
@@ -1508,13 +1508,13 @@
         <v>2024</v>
       </c>
       <c r="C69" t="n">
-        <v>31186</v>
+        <v>31009</v>
       </c>
       <c r="D69" t="n">
         <v>31129</v>
       </c>
       <c r="E69" t="n">
-        <v>-57</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70">
@@ -1523,13 +1523,13 @@
         <v>2025</v>
       </c>
       <c r="C70" t="n">
-        <v>31277</v>
+        <v>31068</v>
       </c>
       <c r="D70" t="n">
         <v>31256</v>
       </c>
       <c r="E70" t="n">
-        <v>-21</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71">
@@ -1538,13 +1538,13 @@
         <v>2026</v>
       </c>
       <c r="C71" t="n">
-        <v>31334</v>
+        <v>31106</v>
       </c>
       <c r="D71" t="n">
         <v>31384</v>
       </c>
       <c r="E71" t="n">
-        <v>49</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72">
@@ -1553,13 +1553,13 @@
         <v>2027</v>
       </c>
       <c r="C72" t="n">
-        <v>31338</v>
+        <v>31101</v>
       </c>
       <c r="D72" t="n">
         <v>31496</v>
       </c>
       <c r="E72" t="n">
-        <v>158</v>
+        <v>394</v>
       </c>
     </row>
     <row r="73">
@@ -1568,13 +1568,13 @@
         <v>2028</v>
       </c>
       <c r="C73" t="n">
-        <v>31213</v>
+        <v>30987</v>
       </c>
       <c r="D73" t="n">
         <v>31593</v>
       </c>
       <c r="E73" t="n">
-        <v>380</v>
+        <v>606</v>
       </c>
     </row>
     <row r="74">
@@ -1583,13 +1583,13 @@
         <v>2029</v>
       </c>
       <c r="C74" t="n">
-        <v>31036</v>
+        <v>30830</v>
       </c>
       <c r="D74" t="n">
         <v>31671</v>
       </c>
       <c r="E74" t="n">
-        <v>636</v>
+        <v>841</v>
       </c>
     </row>
     <row r="75">
@@ -1598,13 +1598,13 @@
         <v>2030</v>
       </c>
       <c r="C75" t="n">
-        <v>30852</v>
+        <v>30668</v>
       </c>
       <c r="D75" t="n">
         <v>31716</v>
       </c>
       <c r="E75" t="n">
-        <v>864</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="76">
@@ -1613,13 +1613,13 @@
         <v>2031</v>
       </c>
       <c r="C76" t="n">
-        <v>30725</v>
+        <v>30548</v>
       </c>
       <c r="D76" t="n">
         <v>31725</v>
       </c>
       <c r="E76" t="n">
-        <v>999</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="77">
@@ -1628,13 +1628,13 @@
         <v>2032</v>
       </c>
       <c r="C77" t="n">
-        <v>30641</v>
+        <v>30457</v>
       </c>
       <c r="D77" t="n">
         <v>31698</v>
       </c>
       <c r="E77" t="n">
-        <v>1057</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="78">
@@ -1643,13 +1643,13 @@
         <v>2033</v>
       </c>
       <c r="C78" t="n">
-        <v>30624</v>
+        <v>30415</v>
       </c>
       <c r="D78" t="n">
         <v>31632</v>
       </c>
       <c r="E78" t="n">
-        <v>1008</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="79">
@@ -1658,13 +1658,13 @@
         <v>2034</v>
       </c>
       <c r="C79" t="n">
-        <v>30558</v>
+        <v>30317</v>
       </c>
       <c r="D79" t="n">
         <v>31552</v>
       </c>
       <c r="E79" t="n">
-        <v>993</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="80">
@@ -1673,13 +1673,13 @@
         <v>2035</v>
       </c>
       <c r="C80" t="n">
-        <v>30469</v>
+        <v>30190</v>
       </c>
       <c r="D80" t="n">
         <v>31437</v>
       </c>
       <c r="E80" t="n">
-        <v>967</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="81">
@@ -1688,13 +1688,13 @@
         <v>2036</v>
       </c>
       <c r="C81" t="n">
-        <v>30408</v>
+        <v>30088</v>
       </c>
       <c r="D81" t="n">
         <v>31321</v>
       </c>
       <c r="E81" t="n">
-        <v>913</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="82">
@@ -1703,13 +1703,13 @@
         <v>2037</v>
       </c>
       <c r="C82" t="n">
-        <v>30450</v>
+        <v>30078</v>
       </c>
       <c r="D82" t="n">
         <v>31189</v>
       </c>
       <c r="E82" t="n">
-        <v>739</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="83">
@@ -1718,13 +1718,13 @@
         <v>2038</v>
       </c>
       <c r="C83" t="n">
-        <v>30553</v>
+        <v>30118</v>
       </c>
       <c r="D83" t="n">
         <v>31068</v>
       </c>
       <c r="E83" t="n">
-        <v>516</v>
+        <v>950</v>
       </c>
     </row>
     <row r="84">
@@ -1733,13 +1733,13 @@
         <v>2039</v>
       </c>
       <c r="C84" t="n">
-        <v>30676</v>
+        <v>30171</v>
       </c>
       <c r="D84" t="n">
         <v>30946</v>
       </c>
       <c r="E84" t="n">
-        <v>270</v>
+        <v>775</v>
       </c>
     </row>
     <row r="85">
@@ -1748,13 +1748,13 @@
         <v>2040</v>
       </c>
       <c r="C85" t="n">
-        <v>30821</v>
+        <v>30244</v>
       </c>
       <c r="D85" t="n">
         <v>30834</v>
       </c>
       <c r="E85" t="n">
-        <v>12</v>
+        <v>590</v>
       </c>
     </row>
     <row r="86">
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>13274</v>
+        <v>13277</v>
       </c>
       <c r="D87" t="n">
         <v>13226</v>
       </c>
       <c r="E87" t="n">
-        <v>-48</v>
+        <v>-52</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>13335</v>
+        <v>13341</v>
       </c>
       <c r="D88" t="n">
         <v>13190</v>
       </c>
       <c r="E88" t="n">
-        <v>-144</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>13395</v>
+        <v>13402</v>
       </c>
       <c r="D89" t="n">
         <v>13140</v>
       </c>
       <c r="E89" t="n">
-        <v>-255</v>
+        <v>-262</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>13441</v>
+        <v>13451</v>
       </c>
       <c r="D90" t="n">
         <v>13091</v>
       </c>
       <c r="E90" t="n">
-        <v>-350</v>
+        <v>-360</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>13512</v>
+        <v>13522</v>
       </c>
       <c r="D91" t="n">
         <v>13024</v>
       </c>
       <c r="E91" t="n">
-        <v>-488</v>
+        <v>-498</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>13577</v>
+        <v>13589</v>
       </c>
       <c r="D92" t="n">
         <v>12945</v>
       </c>
       <c r="E92" t="n">
-        <v>-632</v>
+        <v>-644</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>13610</v>
+        <v>13624</v>
       </c>
       <c r="D93" t="n">
         <v>12865</v>
       </c>
       <c r="E93" t="n">
-        <v>-745</v>
+        <v>-759</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>13569</v>
+        <v>13588</v>
       </c>
       <c r="D94" t="n">
         <v>12763</v>
       </c>
       <c r="E94" t="n">
-        <v>-806</v>
+        <v>-825</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>13500</v>
+        <v>13527</v>
       </c>
       <c r="D95" t="n">
         <v>12664</v>
       </c>
       <c r="E95" t="n">
-        <v>-837</v>
+        <v>-863</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>13418</v>
+        <v>13453</v>
       </c>
       <c r="D96" t="n">
         <v>12555</v>
       </c>
       <c r="E96" t="n">
-        <v>-863</v>
+        <v>-897</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>13360</v>
+        <v>13401</v>
       </c>
       <c r="D97" t="n">
         <v>12434</v>
       </c>
       <c r="E97" t="n">
-        <v>-926</v>
+        <v>-967</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>13316</v>
+        <v>13363</v>
       </c>
       <c r="D98" t="n">
         <v>12320</v>
       </c>
       <c r="E98" t="n">
-        <v>-996</v>
+        <v>-1043</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>13299</v>
+        <v>13351</v>
       </c>
       <c r="D99" t="n">
         <v>12191</v>
       </c>
       <c r="E99" t="n">
-        <v>-1108</v>
+        <v>-1160</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>13234</v>
+        <v>13294</v>
       </c>
       <c r="D100" t="n">
         <v>12080</v>
       </c>
       <c r="E100" t="n">
-        <v>-1154</v>
+        <v>-1214</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>13141</v>
+        <v>13210</v>
       </c>
       <c r="D101" t="n">
         <v>11961</v>
       </c>
       <c r="E101" t="n">
-        <v>-1180</v>
+        <v>-1249</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>13059</v>
+        <v>13137</v>
       </c>
       <c r="D102" t="n">
         <v>11852</v>
       </c>
       <c r="E102" t="n">
-        <v>-1208</v>
+        <v>-1285</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>13031</v>
+        <v>13115</v>
       </c>
       <c r="D103" t="n">
         <v>11748</v>
       </c>
       <c r="E103" t="n">
-        <v>-1283</v>
+        <v>-1367</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>13032</v>
+        <v>13120</v>
       </c>
       <c r="D104" t="n">
         <v>11634</v>
       </c>
       <c r="E104" t="n">
-        <v>-1397</v>
+        <v>-1486</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>13036</v>
+        <v>13129</v>
       </c>
       <c r="D105" t="n">
         <v>11541</v>
       </c>
       <c r="E105" t="n">
-        <v>-1495</v>
+        <v>-1588</v>
       </c>
     </row>
     <row r="106">
@@ -2067,13 +2067,13 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
-        <v>13052</v>
+        <v>13149</v>
       </c>
       <c r="D106" t="n">
         <v>11443</v>
       </c>
       <c r="E106" t="n">
-        <v>-1609</v>
+        <v>-1706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fjernet de siste utfilene.
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -524,10 +524,10 @@
         <v>46204</v>
       </c>
       <c r="D4" t="n">
-        <v>49054</v>
+        <v>49055</v>
       </c>
       <c r="E4" t="n">
-        <v>2851</v>
+        <v>2852</v>
       </c>
     </row>
     <row r="5">
@@ -539,10 +539,10 @@
         <v>46086</v>
       </c>
       <c r="D5" t="n">
-        <v>50111</v>
+        <v>50112</v>
       </c>
       <c r="E5" t="n">
-        <v>4025</v>
+        <v>4026</v>
       </c>
     </row>
     <row r="6">
@@ -554,10 +554,10 @@
         <v>45874</v>
       </c>
       <c r="D6" t="n">
-        <v>51173</v>
+        <v>51175</v>
       </c>
       <c r="E6" t="n">
-        <v>5298</v>
+        <v>5300</v>
       </c>
     </row>
     <row r="7">
@@ -569,10 +569,10 @@
         <v>45756</v>
       </c>
       <c r="D7" t="n">
-        <v>52232</v>
+        <v>52234</v>
       </c>
       <c r="E7" t="n">
-        <v>6476</v>
+        <v>6478</v>
       </c>
     </row>
     <row r="8">
@@ -584,10 +584,10 @@
         <v>45706</v>
       </c>
       <c r="D8" t="n">
-        <v>53290</v>
+        <v>53293</v>
       </c>
       <c r="E8" t="n">
-        <v>7584</v>
+        <v>7587</v>
       </c>
     </row>
     <row r="9">
@@ -596,13 +596,13 @@
         <v>2027</v>
       </c>
       <c r="C9" t="n">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="D9" t="n">
-        <v>54322</v>
+        <v>54325</v>
       </c>
       <c r="E9" t="n">
-        <v>8581</v>
+        <v>8584</v>
       </c>
     </row>
     <row r="10">
@@ -614,10 +614,10 @@
         <v>45850</v>
       </c>
       <c r="D10" t="n">
-        <v>55327</v>
+        <v>55330</v>
       </c>
       <c r="E10" t="n">
-        <v>9476</v>
+        <v>9479</v>
       </c>
     </row>
     <row r="11">
@@ -629,10 +629,10 @@
         <v>46028</v>
       </c>
       <c r="D11" t="n">
-        <v>56273</v>
+        <v>56277</v>
       </c>
       <c r="E11" t="n">
-        <v>10245</v>
+        <v>10249</v>
       </c>
     </row>
     <row r="12">
@@ -644,10 +644,10 @@
         <v>46237</v>
       </c>
       <c r="D12" t="n">
-        <v>57142</v>
+        <v>57146</v>
       </c>
       <c r="E12" t="n">
-        <v>10905</v>
+        <v>10909</v>
       </c>
     </row>
     <row r="13">
@@ -659,10 +659,10 @@
         <v>46459</v>
       </c>
       <c r="D13" t="n">
-        <v>57935</v>
+        <v>57939</v>
       </c>
       <c r="E13" t="n">
-        <v>11476</v>
+        <v>11480</v>
       </c>
     </row>
     <row r="14">
@@ -674,10 +674,10 @@
         <v>46681</v>
       </c>
       <c r="D14" t="n">
-        <v>58628</v>
+        <v>58633</v>
       </c>
       <c r="E14" t="n">
-        <v>11948</v>
+        <v>11952</v>
       </c>
     </row>
     <row r="15">
@@ -689,10 +689,10 @@
         <v>46909</v>
       </c>
       <c r="D15" t="n">
-        <v>59227</v>
+        <v>59232</v>
       </c>
       <c r="E15" t="n">
-        <v>12318</v>
+        <v>12322</v>
       </c>
     </row>
     <row r="16">
@@ -704,10 +704,10 @@
         <v>47175</v>
       </c>
       <c r="D16" t="n">
-        <v>59747</v>
+        <v>59752</v>
       </c>
       <c r="E16" t="n">
-        <v>12573</v>
+        <v>12577</v>
       </c>
     </row>
     <row r="17">
@@ -719,10 +719,10 @@
         <v>47470</v>
       </c>
       <c r="D17" t="n">
-        <v>60180</v>
+        <v>60185</v>
       </c>
       <c r="E17" t="n">
-        <v>12710</v>
+        <v>12715</v>
       </c>
     </row>
     <row r="18">
@@ -734,10 +734,10 @@
         <v>47788</v>
       </c>
       <c r="D18" t="n">
-        <v>60568</v>
+        <v>60574</v>
       </c>
       <c r="E18" t="n">
-        <v>12781</v>
+        <v>12786</v>
       </c>
     </row>
     <row r="19">
@@ -746,13 +746,13 @@
         <v>2037</v>
       </c>
       <c r="C19" t="n">
-        <v>48120</v>
+        <v>48121</v>
       </c>
       <c r="D19" t="n">
-        <v>60935</v>
+        <v>60940</v>
       </c>
       <c r="E19" t="n">
-        <v>12814</v>
+        <v>12820</v>
       </c>
     </row>
     <row r="20">
@@ -764,10 +764,10 @@
         <v>48432</v>
       </c>
       <c r="D20" t="n">
-        <v>61312</v>
+        <v>61317</v>
       </c>
       <c r="E20" t="n">
-        <v>12880</v>
+        <v>12886</v>
       </c>
     </row>
     <row r="21">
@@ -779,10 +779,10 @@
         <v>48682</v>
       </c>
       <c r="D21" t="n">
-        <v>61717</v>
+        <v>61723</v>
       </c>
       <c r="E21" t="n">
-        <v>13035</v>
+        <v>13041</v>
       </c>
     </row>
     <row r="22">
@@ -794,10 +794,10 @@
         <v>48869</v>
       </c>
       <c r="D22" t="n">
-        <v>62174</v>
+        <v>62181</v>
       </c>
       <c r="E22" t="n">
-        <v>13306</v>
+        <v>13312</v>
       </c>
     </row>
     <row r="23">
@@ -825,13 +825,13 @@
         <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>52370</v>
+        <v>52369</v>
       </c>
       <c r="D24" t="n">
-        <v>52771</v>
+        <v>52773</v>
       </c>
       <c r="E24" t="n">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25">
@@ -843,10 +843,10 @@
         <v>52430</v>
       </c>
       <c r="D25" t="n">
-        <v>53230</v>
+        <v>53233</v>
       </c>
       <c r="E25" t="n">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="26">
@@ -858,10 +858,10 @@
         <v>52329</v>
       </c>
       <c r="D26" t="n">
-        <v>53746</v>
+        <v>53749</v>
       </c>
       <c r="E26" t="n">
-        <v>1416</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="27">
@@ -873,10 +873,10 @@
         <v>52127</v>
       </c>
       <c r="D27" t="n">
-        <v>54316</v>
+        <v>54321</v>
       </c>
       <c r="E27" t="n">
-        <v>2189</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="28">
@@ -885,13 +885,13 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>51767</v>
+        <v>51766</v>
       </c>
       <c r="D28" t="n">
-        <v>54926</v>
+        <v>54931</v>
       </c>
       <c r="E28" t="n">
-        <v>3159</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="29">
@@ -903,10 +903,10 @@
         <v>51321</v>
       </c>
       <c r="D29" t="n">
-        <v>55541</v>
+        <v>55547</v>
       </c>
       <c r="E29" t="n">
-        <v>4219</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="30">
@@ -915,13 +915,13 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>50918</v>
+        <v>50917</v>
       </c>
       <c r="D30" t="n">
-        <v>56186</v>
+        <v>56193</v>
       </c>
       <c r="E30" t="n">
-        <v>5269</v>
+        <v>5276</v>
       </c>
     </row>
     <row r="31">
@@ -933,10 +933,10 @@
         <v>50561</v>
       </c>
       <c r="D31" t="n">
-        <v>56811</v>
+        <v>56819</v>
       </c>
       <c r="E31" t="n">
-        <v>6250</v>
+        <v>6258</v>
       </c>
     </row>
     <row r="32">
@@ -948,10 +948,10 @@
         <v>50199</v>
       </c>
       <c r="D32" t="n">
-        <v>57397</v>
+        <v>57406</v>
       </c>
       <c r="E32" t="n">
-        <v>7198</v>
+        <v>7207</v>
       </c>
     </row>
     <row r="33">
@@ -963,10 +963,10 @@
         <v>49939</v>
       </c>
       <c r="D33" t="n">
-        <v>57919</v>
+        <v>57928</v>
       </c>
       <c r="E33" t="n">
-        <v>7980</v>
+        <v>7990</v>
       </c>
     </row>
     <row r="34">
@@ -975,13 +975,13 @@
         <v>2031</v>
       </c>
       <c r="C34" t="n">
-        <v>49717</v>
+        <v>49716</v>
       </c>
       <c r="D34" t="n">
-        <v>58381</v>
+        <v>58391</v>
       </c>
       <c r="E34" t="n">
-        <v>8665</v>
+        <v>8675</v>
       </c>
     </row>
     <row r="35">
@@ -993,10 +993,10 @@
         <v>49544</v>
       </c>
       <c r="D35" t="n">
-        <v>58767</v>
+        <v>58778</v>
       </c>
       <c r="E35" t="n">
-        <v>9223</v>
+        <v>9234</v>
       </c>
     </row>
     <row r="36">
@@ -1005,13 +1005,13 @@
         <v>2033</v>
       </c>
       <c r="C36" t="n">
-        <v>49425</v>
+        <v>49424</v>
       </c>
       <c r="D36" t="n">
-        <v>59072</v>
+        <v>59083</v>
       </c>
       <c r="E36" t="n">
-        <v>9648</v>
+        <v>9659</v>
       </c>
     </row>
     <row r="37">
@@ -1023,10 +1023,10 @@
         <v>49440</v>
       </c>
       <c r="D37" t="n">
-        <v>59320</v>
+        <v>59331</v>
       </c>
       <c r="E37" t="n">
-        <v>9879</v>
+        <v>9891</v>
       </c>
     </row>
     <row r="38">
@@ -1038,10 +1038,10 @@
         <v>49547</v>
       </c>
       <c r="D38" t="n">
-        <v>59510</v>
+        <v>59522</v>
       </c>
       <c r="E38" t="n">
-        <v>9963</v>
+        <v>9975</v>
       </c>
     </row>
     <row r="39">
@@ -1053,10 +1053,10 @@
         <v>49711</v>
       </c>
       <c r="D39" t="n">
-        <v>59677</v>
+        <v>59689</v>
       </c>
       <c r="E39" t="n">
-        <v>9966</v>
+        <v>9978</v>
       </c>
     </row>
     <row r="40">
@@ -1068,10 +1068,10 @@
         <v>49919</v>
       </c>
       <c r="D40" t="n">
-        <v>59837</v>
+        <v>59849</v>
       </c>
       <c r="E40" t="n">
-        <v>9918</v>
+        <v>9930</v>
       </c>
     </row>
     <row r="41">
@@ -1083,10 +1083,10 @@
         <v>50169</v>
       </c>
       <c r="D41" t="n">
-        <v>59992</v>
+        <v>60004</v>
       </c>
       <c r="E41" t="n">
-        <v>9823</v>
+        <v>9835</v>
       </c>
     </row>
     <row r="42">
@@ -1098,10 +1098,10 @@
         <v>50466</v>
       </c>
       <c r="D42" t="n">
-        <v>60171</v>
+        <v>60182</v>
       </c>
       <c r="E42" t="n">
-        <v>9705</v>
+        <v>9717</v>
       </c>
     </row>
     <row r="43">
@@ -1110,13 +1110,13 @@
         <v>2040</v>
       </c>
       <c r="C43" t="n">
-        <v>50778</v>
+        <v>50777</v>
       </c>
       <c r="D43" t="n">
-        <v>60363</v>
+        <v>60374</v>
       </c>
       <c r="E43" t="n">
-        <v>9585</v>
+        <v>9597</v>
       </c>
     </row>
     <row r="44">
@@ -1129,13 +1129,13 @@
         <v>2020</v>
       </c>
       <c r="C44" t="n">
-        <v>16557</v>
+        <v>16556</v>
       </c>
       <c r="D44" t="n">
         <v>16557</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1144,13 +1144,13 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>16582</v>
+        <v>16581</v>
       </c>
       <c r="D45" t="n">
         <v>17578</v>
       </c>
       <c r="E45" t="n">
-        <v>996</v>
+        <v>998</v>
       </c>
     </row>
     <row r="46">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>16637</v>
+        <v>16636</v>
       </c>
       <c r="D46" t="n">
-        <v>18646</v>
+        <v>18647</v>
       </c>
       <c r="E46" t="n">
-        <v>2009</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>16656</v>
+        <v>16655</v>
       </c>
       <c r="D47" t="n">
-        <v>19744</v>
+        <v>19746</v>
       </c>
       <c r="E47" t="n">
-        <v>3088</v>
+        <v>3091</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>16667</v>
+        <v>16666</v>
       </c>
       <c r="D48" t="n">
-        <v>20844</v>
+        <v>20847</v>
       </c>
       <c r="E48" t="n">
-        <v>4177</v>
+        <v>4181</v>
       </c>
     </row>
     <row r="49">
@@ -1207,10 +1207,10 @@
         <v>16664</v>
       </c>
       <c r="D49" t="n">
-        <v>21946</v>
+        <v>21949</v>
       </c>
       <c r="E49" t="n">
-        <v>5281</v>
+        <v>5285</v>
       </c>
     </row>
     <row r="50">
@@ -1222,10 +1222,10 @@
         <v>16651</v>
       </c>
       <c r="D50" t="n">
-        <v>23028</v>
+        <v>23031</v>
       </c>
       <c r="E50" t="n">
-        <v>6376</v>
+        <v>6381</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>16638</v>
+        <v>16637</v>
       </c>
       <c r="D51" t="n">
-        <v>24099</v>
+        <v>24103</v>
       </c>
       <c r="E51" t="n">
-        <v>7460</v>
+        <v>7466</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>16617</v>
+        <v>16616</v>
       </c>
       <c r="D52" t="n">
-        <v>25140</v>
+        <v>25145</v>
       </c>
       <c r="E52" t="n">
-        <v>8523</v>
+        <v>8529</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>16591</v>
+        <v>16590</v>
       </c>
       <c r="D53" t="n">
-        <v>26167</v>
+        <v>26173</v>
       </c>
       <c r="E53" t="n">
-        <v>9576</v>
+        <v>9583</v>
       </c>
     </row>
     <row r="54">
@@ -1282,10 +1282,10 @@
         <v>16574</v>
       </c>
       <c r="D54" t="n">
-        <v>27160</v>
+        <v>27167</v>
       </c>
       <c r="E54" t="n">
-        <v>10586</v>
+        <v>10594</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>16566</v>
+        <v>16565</v>
       </c>
       <c r="D55" t="n">
-        <v>28119</v>
+        <v>28127</v>
       </c>
       <c r="E55" t="n">
-        <v>11553</v>
+        <v>11561</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>16566</v>
+        <v>16565</v>
       </c>
       <c r="D56" t="n">
-        <v>29053</v>
+        <v>29061</v>
       </c>
       <c r="E56" t="n">
-        <v>12488</v>
+        <v>12496</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>16576</v>
+        <v>16575</v>
       </c>
       <c r="D57" t="n">
-        <v>29967</v>
+        <v>29976</v>
       </c>
       <c r="E57" t="n">
-        <v>13392</v>
+        <v>13401</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>16592</v>
+        <v>16591</v>
       </c>
       <c r="D58" t="n">
-        <v>30877</v>
+        <v>30886</v>
       </c>
       <c r="E58" t="n">
-        <v>14285</v>
+        <v>14295</v>
       </c>
     </row>
     <row r="59">
@@ -1357,10 +1357,10 @@
         <v>16613</v>
       </c>
       <c r="D59" t="n">
-        <v>31772</v>
+        <v>31782</v>
       </c>
       <c r="E59" t="n">
-        <v>15158</v>
+        <v>15169</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>16644</v>
+        <v>16643</v>
       </c>
       <c r="D60" t="n">
-        <v>32647</v>
+        <v>32658</v>
       </c>
       <c r="E60" t="n">
-        <v>16004</v>
+        <v>16015</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>16690</v>
+        <v>16689</v>
       </c>
       <c r="D61" t="n">
-        <v>33520</v>
+        <v>33531</v>
       </c>
       <c r="E61" t="n">
-        <v>16830</v>
+        <v>16842</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>16745</v>
+        <v>16744</v>
       </c>
       <c r="D62" t="n">
-        <v>34393</v>
+        <v>34404</v>
       </c>
       <c r="E62" t="n">
-        <v>17648</v>
+        <v>17660</v>
       </c>
     </row>
     <row r="63">
@@ -1417,10 +1417,10 @@
         <v>16804</v>
       </c>
       <c r="D63" t="n">
-        <v>35263</v>
+        <v>35275</v>
       </c>
       <c r="E63" t="n">
-        <v>18458</v>
+        <v>18471</v>
       </c>
     </row>
     <row r="64">
@@ -1429,13 +1429,13 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>16867</v>
+        <v>16866</v>
       </c>
       <c r="D64" t="n">
-        <v>36117</v>
+        <v>36130</v>
       </c>
       <c r="E64" t="n">
-        <v>19250</v>
+        <v>19264</v>
       </c>
     </row>
     <row r="65">
@@ -1481,7 +1481,7 @@
         <v>30975</v>
       </c>
       <c r="D67" t="n">
-        <v>30889</v>
+        <v>30890</v>
       </c>
       <c r="E67" t="n">
         <v>-85</v>
@@ -1511,7 +1511,7 @@
         <v>31186</v>
       </c>
       <c r="D69" t="n">
-        <v>31129</v>
+        <v>31130</v>
       </c>
       <c r="E69" t="n">
         <v>-57</v>
@@ -1529,7 +1529,7 @@
         <v>31256</v>
       </c>
       <c r="E70" t="n">
-        <v>-21</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="71">
@@ -1544,7 +1544,7 @@
         <v>31384</v>
       </c>
       <c r="E71" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72">
@@ -1571,10 +1571,10 @@
         <v>31213</v>
       </c>
       <c r="D73" t="n">
-        <v>31593</v>
+        <v>31594</v>
       </c>
       <c r="E73" t="n">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="74">
@@ -1586,10 +1586,10 @@
         <v>31036</v>
       </c>
       <c r="D74" t="n">
-        <v>31671</v>
+        <v>31672</v>
       </c>
       <c r="E74" t="n">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="75">
@@ -1601,10 +1601,10 @@
         <v>30852</v>
       </c>
       <c r="D75" t="n">
-        <v>31716</v>
+        <v>31717</v>
       </c>
       <c r="E75" t="n">
-        <v>864</v>
+        <v>865</v>
       </c>
     </row>
     <row r="76">
@@ -1616,10 +1616,10 @@
         <v>30725</v>
       </c>
       <c r="D76" t="n">
-        <v>31725</v>
+        <v>31726</v>
       </c>
       <c r="E76" t="n">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="77">
@@ -1631,10 +1631,10 @@
         <v>30641</v>
       </c>
       <c r="D77" t="n">
-        <v>31698</v>
+        <v>31699</v>
       </c>
       <c r="E77" t="n">
-        <v>1057</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="78">
@@ -1646,10 +1646,10 @@
         <v>30624</v>
       </c>
       <c r="D78" t="n">
-        <v>31632</v>
+        <v>31633</v>
       </c>
       <c r="E78" t="n">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="79">
@@ -1661,10 +1661,10 @@
         <v>30558</v>
       </c>
       <c r="D79" t="n">
-        <v>31552</v>
+        <v>31553</v>
       </c>
       <c r="E79" t="n">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="80">
@@ -1679,7 +1679,7 @@
         <v>31437</v>
       </c>
       <c r="E80" t="n">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row r="81">
@@ -1691,10 +1691,10 @@
         <v>30408</v>
       </c>
       <c r="D81" t="n">
-        <v>31321</v>
+        <v>31322</v>
       </c>
       <c r="E81" t="n">
-        <v>913</v>
+        <v>914</v>
       </c>
     </row>
     <row r="82">
@@ -1706,10 +1706,10 @@
         <v>30450</v>
       </c>
       <c r="D82" t="n">
-        <v>31189</v>
+        <v>31190</v>
       </c>
       <c r="E82" t="n">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="83">
@@ -1721,7 +1721,7 @@
         <v>30553</v>
       </c>
       <c r="D83" t="n">
-        <v>31068</v>
+        <v>31069</v>
       </c>
       <c r="E83" t="n">
         <v>516</v>
@@ -1754,7 +1754,7 @@
         <v>30834</v>
       </c>
       <c r="E85" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86">
@@ -1767,13 +1767,13 @@
         <v>2020</v>
       </c>
       <c r="C86" t="n">
-        <v>13248</v>
+        <v>13249</v>
       </c>
       <c r="D86" t="n">
         <v>13248</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="87">
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>13274</v>
+        <v>13275</v>
       </c>
       <c r="D87" t="n">
         <v>13226</v>
       </c>
       <c r="E87" t="n">
-        <v>-48</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>13335</v>
+        <v>13336</v>
       </c>
       <c r="D88" t="n">
         <v>13190</v>
       </c>
       <c r="E88" t="n">
-        <v>-144</v>
+        <v>-146</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>13395</v>
+        <v>13396</v>
       </c>
       <c r="D89" t="n">
         <v>13140</v>
       </c>
       <c r="E89" t="n">
-        <v>-255</v>
+        <v>-256</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>13441</v>
+        <v>13442</v>
       </c>
       <c r="D90" t="n">
         <v>13091</v>
       </c>
       <c r="E90" t="n">
-        <v>-350</v>
+        <v>-351</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>13512</v>
+        <v>13513</v>
       </c>
       <c r="D91" t="n">
         <v>13024</v>
       </c>
       <c r="E91" t="n">
-        <v>-488</v>
+        <v>-489</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>13577</v>
+        <v>13578</v>
       </c>
       <c r="D92" t="n">
         <v>12945</v>
       </c>
       <c r="E92" t="n">
-        <v>-632</v>
+        <v>-634</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>13610</v>
+        <v>13612</v>
       </c>
       <c r="D93" t="n">
-        <v>12865</v>
+        <v>12866</v>
       </c>
       <c r="E93" t="n">
-        <v>-745</v>
+        <v>-746</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>13569</v>
+        <v>13570</v>
       </c>
       <c r="D94" t="n">
         <v>12763</v>
       </c>
       <c r="E94" t="n">
-        <v>-806</v>
+        <v>-807</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>13500</v>
+        <v>13502</v>
       </c>
       <c r="D95" t="n">
         <v>12664</v>
       </c>
       <c r="E95" t="n">
-        <v>-837</v>
+        <v>-838</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>13418</v>
+        <v>13420</v>
       </c>
       <c r="D96" t="n">
         <v>12555</v>
       </c>
       <c r="E96" t="n">
-        <v>-863</v>
+        <v>-864</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>13360</v>
+        <v>13362</v>
       </c>
       <c r="D97" t="n">
         <v>12434</v>
       </c>
       <c r="E97" t="n">
-        <v>-926</v>
+        <v>-927</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>13316</v>
+        <v>13318</v>
       </c>
       <c r="D98" t="n">
-        <v>12320</v>
+        <v>12321</v>
       </c>
       <c r="E98" t="n">
-        <v>-996</v>
+        <v>-997</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>13299</v>
+        <v>13301</v>
       </c>
       <c r="D99" t="n">
         <v>12191</v>
       </c>
       <c r="E99" t="n">
-        <v>-1108</v>
+        <v>-1110</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>13234</v>
+        <v>13235</v>
       </c>
       <c r="D100" t="n">
         <v>12080</v>
       </c>
       <c r="E100" t="n">
-        <v>-1154</v>
+        <v>-1155</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>13141</v>
+        <v>13143</v>
       </c>
       <c r="D101" t="n">
         <v>11961</v>
       </c>
       <c r="E101" t="n">
-        <v>-1180</v>
+        <v>-1182</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>13059</v>
+        <v>13061</v>
       </c>
       <c r="D102" t="n">
         <v>11852</v>
       </c>
       <c r="E102" t="n">
-        <v>-1208</v>
+        <v>-1209</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>13031</v>
+        <v>13033</v>
       </c>
       <c r="D103" t="n">
         <v>11748</v>
       </c>
       <c r="E103" t="n">
-        <v>-1283</v>
+        <v>-1284</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>13032</v>
+        <v>13033</v>
       </c>
       <c r="D104" t="n">
-        <v>11634</v>
+        <v>11635</v>
       </c>
       <c r="E104" t="n">
-        <v>-1397</v>
+        <v>-1399</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>13036</v>
+        <v>13037</v>
       </c>
       <c r="D105" t="n">
-        <v>11541</v>
+        <v>11542</v>
       </c>
       <c r="E105" t="n">
-        <v>-1495</v>
+        <v>-1496</v>
       </c>
     </row>
     <row r="106">
@@ -2067,13 +2067,13 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
-        <v>13052</v>
+        <v>13053</v>
       </c>
       <c r="D106" t="n">
         <v>11443</v>
       </c>
       <c r="E106" t="n">
-        <v>-1609</v>
+        <v>-1610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fjernet bruk av "andre lærere".
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -491,13 +491,13 @@
         <v>2020</v>
       </c>
       <c r="C2" t="n">
-        <v>47126</v>
+        <v>47134</v>
       </c>
       <c r="D2" t="n">
         <v>47126</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="3">
@@ -506,13 +506,13 @@
         <v>2021</v>
       </c>
       <c r="C3" t="n">
-        <v>46632</v>
+        <v>46522</v>
       </c>
       <c r="D3" t="n">
         <v>48005</v>
       </c>
       <c r="E3" t="n">
-        <v>1373</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="4">
@@ -521,13 +521,13 @@
         <v>2022</v>
       </c>
       <c r="C4" t="n">
-        <v>46204</v>
+        <v>45972</v>
       </c>
       <c r="D4" t="n">
         <v>49055</v>
       </c>
       <c r="E4" t="n">
-        <v>2852</v>
+        <v>3083</v>
       </c>
     </row>
     <row r="5">
@@ -536,13 +536,13 @@
         <v>2023</v>
       </c>
       <c r="C5" t="n">
-        <v>46086</v>
+        <v>45818</v>
       </c>
       <c r="D5" t="n">
         <v>50112</v>
       </c>
       <c r="E5" t="n">
-        <v>4026</v>
+        <v>4294</v>
       </c>
     </row>
     <row r="6">
@@ -551,13 +551,13 @@
         <v>2024</v>
       </c>
       <c r="C6" t="n">
-        <v>45874</v>
+        <v>45550</v>
       </c>
       <c r="D6" t="n">
         <v>51175</v>
       </c>
       <c r="E6" t="n">
-        <v>5300</v>
+        <v>5624</v>
       </c>
     </row>
     <row r="7">
@@ -566,13 +566,13 @@
         <v>2025</v>
       </c>
       <c r="C7" t="n">
-        <v>45756</v>
+        <v>45403</v>
       </c>
       <c r="D7" t="n">
         <v>52234</v>
       </c>
       <c r="E7" t="n">
-        <v>6478</v>
+        <v>6831</v>
       </c>
     </row>
     <row r="8">
@@ -581,13 +581,13 @@
         <v>2026</v>
       </c>
       <c r="C8" t="n">
-        <v>45706</v>
+        <v>45343</v>
       </c>
       <c r="D8" t="n">
         <v>53293</v>
       </c>
       <c r="E8" t="n">
-        <v>7587</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="9">
@@ -596,13 +596,13 @@
         <v>2027</v>
       </c>
       <c r="C9" t="n">
-        <v>45741</v>
+        <v>45380</v>
       </c>
       <c r="D9" t="n">
         <v>54325</v>
       </c>
       <c r="E9" t="n">
-        <v>8584</v>
+        <v>8945</v>
       </c>
     </row>
     <row r="10">
@@ -611,13 +611,13 @@
         <v>2028</v>
       </c>
       <c r="C10" t="n">
-        <v>45850</v>
+        <v>45504</v>
       </c>
       <c r="D10" t="n">
         <v>55330</v>
       </c>
       <c r="E10" t="n">
-        <v>9479</v>
+        <v>9826</v>
       </c>
     </row>
     <row r="11">
@@ -626,13 +626,13 @@
         <v>2029</v>
       </c>
       <c r="C11" t="n">
-        <v>46028</v>
+        <v>45709</v>
       </c>
       <c r="D11" t="n">
         <v>56277</v>
       </c>
       <c r="E11" t="n">
-        <v>10249</v>
+        <v>10568</v>
       </c>
     </row>
     <row r="12">
@@ -641,13 +641,13 @@
         <v>2030</v>
       </c>
       <c r="C12" t="n">
-        <v>46237</v>
+        <v>45945</v>
       </c>
       <c r="D12" t="n">
         <v>57146</v>
       </c>
       <c r="E12" t="n">
-        <v>10909</v>
+        <v>11201</v>
       </c>
     </row>
     <row r="13">
@@ -656,13 +656,13 @@
         <v>2031</v>
       </c>
       <c r="C13" t="n">
-        <v>46459</v>
+        <v>46196</v>
       </c>
       <c r="D13" t="n">
         <v>57939</v>
       </c>
       <c r="E13" t="n">
-        <v>11480</v>
+        <v>11743</v>
       </c>
     </row>
     <row r="14">
@@ -671,13 +671,13 @@
         <v>2032</v>
       </c>
       <c r="C14" t="n">
-        <v>46681</v>
+        <v>46444</v>
       </c>
       <c r="D14" t="n">
         <v>58633</v>
       </c>
       <c r="E14" t="n">
-        <v>11952</v>
+        <v>12188</v>
       </c>
     </row>
     <row r="15">
@@ -686,13 +686,13 @@
         <v>2033</v>
       </c>
       <c r="C15" t="n">
-        <v>46909</v>
+        <v>46698</v>
       </c>
       <c r="D15" t="n">
         <v>59232</v>
       </c>
       <c r="E15" t="n">
-        <v>12322</v>
+        <v>12533</v>
       </c>
     </row>
     <row r="16">
@@ -701,13 +701,13 @@
         <v>2034</v>
       </c>
       <c r="C16" t="n">
-        <v>47175</v>
+        <v>46989</v>
       </c>
       <c r="D16" t="n">
         <v>59752</v>
       </c>
       <c r="E16" t="n">
-        <v>12577</v>
+        <v>12763</v>
       </c>
     </row>
     <row r="17">
@@ -716,13 +716,13 @@
         <v>2035</v>
       </c>
       <c r="C17" t="n">
-        <v>47470</v>
+        <v>47311</v>
       </c>
       <c r="D17" t="n">
         <v>60185</v>
       </c>
       <c r="E17" t="n">
-        <v>12715</v>
+        <v>12874</v>
       </c>
     </row>
     <row r="18">
@@ -731,13 +731,13 @@
         <v>2036</v>
       </c>
       <c r="C18" t="n">
-        <v>47788</v>
+        <v>47656</v>
       </c>
       <c r="D18" t="n">
         <v>60574</v>
       </c>
       <c r="E18" t="n">
-        <v>12786</v>
+        <v>12918</v>
       </c>
     </row>
     <row r="19">
@@ -746,13 +746,13 @@
         <v>2037</v>
       </c>
       <c r="C19" t="n">
-        <v>48121</v>
+        <v>48017</v>
       </c>
       <c r="D19" t="n">
         <v>60940</v>
       </c>
       <c r="E19" t="n">
-        <v>12820</v>
+        <v>12923</v>
       </c>
     </row>
     <row r="20">
@@ -761,13 +761,13 @@
         <v>2038</v>
       </c>
       <c r="C20" t="n">
-        <v>48432</v>
+        <v>48352</v>
       </c>
       <c r="D20" t="n">
         <v>61317</v>
       </c>
       <c r="E20" t="n">
-        <v>12886</v>
+        <v>12966</v>
       </c>
     </row>
     <row r="21">
@@ -776,13 +776,13 @@
         <v>2039</v>
       </c>
       <c r="C21" t="n">
-        <v>48682</v>
+        <v>48612</v>
       </c>
       <c r="D21" t="n">
         <v>61723</v>
       </c>
       <c r="E21" t="n">
-        <v>13041</v>
+        <v>13111</v>
       </c>
     </row>
     <row r="22">
@@ -791,13 +791,13 @@
         <v>2040</v>
       </c>
       <c r="C22" t="n">
-        <v>48869</v>
+        <v>48798</v>
       </c>
       <c r="D22" t="n">
         <v>62181</v>
       </c>
       <c r="E22" t="n">
-        <v>13312</v>
+        <v>13383</v>
       </c>
     </row>
     <row r="23">
@@ -810,13 +810,13 @@
         <v>2020</v>
       </c>
       <c r="C23" t="n">
-        <v>52381</v>
+        <v>52497</v>
       </c>
       <c r="D23" t="n">
         <v>52381</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>-116</v>
       </c>
     </row>
     <row r="24">
@@ -825,13 +825,13 @@
         <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>52369</v>
+        <v>52460</v>
       </c>
       <c r="D24" t="n">
         <v>52773</v>
       </c>
       <c r="E24" t="n">
-        <v>403</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25">
@@ -840,13 +840,13 @@
         <v>2022</v>
       </c>
       <c r="C25" t="n">
-        <v>52430</v>
+        <v>52490</v>
       </c>
       <c r="D25" t="n">
         <v>53233</v>
       </c>
       <c r="E25" t="n">
-        <v>803</v>
+        <v>743</v>
       </c>
     </row>
     <row r="26">
@@ -855,13 +855,13 @@
         <v>2023</v>
       </c>
       <c r="C26" t="n">
-        <v>52329</v>
+        <v>52350</v>
       </c>
       <c r="D26" t="n">
         <v>53749</v>
       </c>
       <c r="E26" t="n">
-        <v>1420</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="27">
@@ -870,13 +870,13 @@
         <v>2024</v>
       </c>
       <c r="C27" t="n">
-        <v>52127</v>
+        <v>52089</v>
       </c>
       <c r="D27" t="n">
         <v>54321</v>
       </c>
       <c r="E27" t="n">
-        <v>2194</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="28">
@@ -885,13 +885,13 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>51766</v>
+        <v>51644</v>
       </c>
       <c r="D28" t="n">
         <v>54931</v>
       </c>
       <c r="E28" t="n">
-        <v>3165</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="29">
@@ -900,13 +900,13 @@
         <v>2026</v>
       </c>
       <c r="C29" t="n">
-        <v>51321</v>
+        <v>51101</v>
       </c>
       <c r="D29" t="n">
         <v>55547</v>
       </c>
       <c r="E29" t="n">
-        <v>4226</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="30">
@@ -915,13 +915,13 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>50917</v>
+        <v>50608</v>
       </c>
       <c r="D30" t="n">
         <v>56193</v>
       </c>
       <c r="E30" t="n">
-        <v>5276</v>
+        <v>5586</v>
       </c>
     </row>
     <row r="31">
@@ -930,13 +930,13 @@
         <v>2028</v>
       </c>
       <c r="C31" t="n">
-        <v>50561</v>
+        <v>50174</v>
       </c>
       <c r="D31" t="n">
         <v>56819</v>
       </c>
       <c r="E31" t="n">
-        <v>6258</v>
+        <v>6645</v>
       </c>
     </row>
     <row r="32">
@@ -945,13 +945,13 @@
         <v>2029</v>
       </c>
       <c r="C32" t="n">
-        <v>50199</v>
+        <v>49736</v>
       </c>
       <c r="D32" t="n">
         <v>57406</v>
       </c>
       <c r="E32" t="n">
-        <v>7207</v>
+        <v>7670</v>
       </c>
     </row>
     <row r="33">
@@ -960,13 +960,13 @@
         <v>2030</v>
       </c>
       <c r="C33" t="n">
-        <v>49939</v>
+        <v>49415</v>
       </c>
       <c r="D33" t="n">
         <v>57928</v>
       </c>
       <c r="E33" t="n">
-        <v>7990</v>
+        <v>8514</v>
       </c>
     </row>
     <row r="34">
@@ -975,13 +975,13 @@
         <v>2031</v>
       </c>
       <c r="C34" t="n">
-        <v>49716</v>
+        <v>49137</v>
       </c>
       <c r="D34" t="n">
         <v>58391</v>
       </c>
       <c r="E34" t="n">
-        <v>8675</v>
+        <v>9254</v>
       </c>
     </row>
     <row r="35">
@@ -990,13 +990,13 @@
         <v>2032</v>
       </c>
       <c r="C35" t="n">
-        <v>49544</v>
+        <v>48916</v>
       </c>
       <c r="D35" t="n">
         <v>58778</v>
       </c>
       <c r="E35" t="n">
-        <v>9234</v>
+        <v>9861</v>
       </c>
     </row>
     <row r="36">
@@ -1005,13 +1005,13 @@
         <v>2033</v>
       </c>
       <c r="C36" t="n">
-        <v>49424</v>
+        <v>48755</v>
       </c>
       <c r="D36" t="n">
         <v>59083</v>
       </c>
       <c r="E36" t="n">
-        <v>9659</v>
+        <v>10328</v>
       </c>
     </row>
     <row r="37">
@@ -1020,13 +1020,13 @@
         <v>2034</v>
       </c>
       <c r="C37" t="n">
-        <v>49440</v>
+        <v>48754</v>
       </c>
       <c r="D37" t="n">
         <v>59331</v>
       </c>
       <c r="E37" t="n">
-        <v>9891</v>
+        <v>10577</v>
       </c>
     </row>
     <row r="38">
@@ -1035,13 +1035,13 @@
         <v>2035</v>
       </c>
       <c r="C38" t="n">
-        <v>49547</v>
+        <v>48860</v>
       </c>
       <c r="D38" t="n">
         <v>59522</v>
       </c>
       <c r="E38" t="n">
-        <v>9975</v>
+        <v>10662</v>
       </c>
     </row>
     <row r="39">
@@ -1050,13 +1050,13 @@
         <v>2036</v>
       </c>
       <c r="C39" t="n">
-        <v>49711</v>
+        <v>49030</v>
       </c>
       <c r="D39" t="n">
         <v>59689</v>
       </c>
       <c r="E39" t="n">
-        <v>9978</v>
+        <v>10659</v>
       </c>
     </row>
     <row r="40">
@@ -1065,13 +1065,13 @@
         <v>2037</v>
       </c>
       <c r="C40" t="n">
-        <v>49919</v>
+        <v>49248</v>
       </c>
       <c r="D40" t="n">
         <v>59849</v>
       </c>
       <c r="E40" t="n">
-        <v>9930</v>
+        <v>10600</v>
       </c>
     </row>
     <row r="41">
@@ -1080,13 +1080,13 @@
         <v>2038</v>
       </c>
       <c r="C41" t="n">
-        <v>50169</v>
+        <v>49514</v>
       </c>
       <c r="D41" t="n">
         <v>60004</v>
       </c>
       <c r="E41" t="n">
-        <v>9835</v>
+        <v>10490</v>
       </c>
     </row>
     <row r="42">
@@ -1095,13 +1095,13 @@
         <v>2039</v>
       </c>
       <c r="C42" t="n">
-        <v>50466</v>
+        <v>49834</v>
       </c>
       <c r="D42" t="n">
         <v>60182</v>
       </c>
       <c r="E42" t="n">
-        <v>9717</v>
+        <v>10348</v>
       </c>
     </row>
     <row r="43">
@@ -1110,13 +1110,13 @@
         <v>2040</v>
       </c>
       <c r="C43" t="n">
-        <v>50777</v>
+        <v>50172</v>
       </c>
       <c r="D43" t="n">
         <v>60374</v>
       </c>
       <c r="E43" t="n">
-        <v>9597</v>
+        <v>10203</v>
       </c>
     </row>
     <row r="44">
@@ -1129,13 +1129,13 @@
         <v>2020</v>
       </c>
       <c r="C44" t="n">
-        <v>16556</v>
+        <v>16600</v>
       </c>
       <c r="D44" t="n">
         <v>16557</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>-43</v>
       </c>
     </row>
     <row r="45">
@@ -1144,13 +1144,13 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>16581</v>
+        <v>16625</v>
       </c>
       <c r="D45" t="n">
         <v>17578</v>
       </c>
       <c r="E45" t="n">
-        <v>998</v>
+        <v>953</v>
       </c>
     </row>
     <row r="46">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>16636</v>
+        <v>16686</v>
       </c>
       <c r="D46" t="n">
         <v>18647</v>
       </c>
       <c r="E46" t="n">
-        <v>2011</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>16655</v>
+        <v>16732</v>
       </c>
       <c r="D47" t="n">
         <v>19746</v>
       </c>
       <c r="E47" t="n">
-        <v>3091</v>
+        <v>3014</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>16666</v>
+        <v>16759</v>
       </c>
       <c r="D48" t="n">
         <v>20847</v>
       </c>
       <c r="E48" t="n">
-        <v>4181</v>
+        <v>4088</v>
       </c>
     </row>
     <row r="49">
@@ -1204,13 +1204,13 @@
         <v>2025</v>
       </c>
       <c r="C49" t="n">
-        <v>16664</v>
+        <v>16792</v>
       </c>
       <c r="D49" t="n">
         <v>21949</v>
       </c>
       <c r="E49" t="n">
-        <v>5285</v>
+        <v>5157</v>
       </c>
     </row>
     <row r="50">
@@ -1219,13 +1219,13 @@
         <v>2026</v>
       </c>
       <c r="C50" t="n">
-        <v>16651</v>
+        <v>16814</v>
       </c>
       <c r="D50" t="n">
         <v>23031</v>
       </c>
       <c r="E50" t="n">
-        <v>6381</v>
+        <v>6217</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>16637</v>
+        <v>16815</v>
       </c>
       <c r="D51" t="n">
         <v>24103</v>
       </c>
       <c r="E51" t="n">
-        <v>7466</v>
+        <v>7288</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>16616</v>
+        <v>16763</v>
       </c>
       <c r="D52" t="n">
         <v>25145</v>
       </c>
       <c r="E52" t="n">
-        <v>8529</v>
+        <v>8383</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>16590</v>
+        <v>16689</v>
       </c>
       <c r="D53" t="n">
         <v>26173</v>
       </c>
       <c r="E53" t="n">
-        <v>9583</v>
+        <v>9484</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1279,13 @@
         <v>2030</v>
       </c>
       <c r="C54" t="n">
-        <v>16574</v>
+        <v>16613</v>
       </c>
       <c r="D54" t="n">
         <v>27167</v>
       </c>
       <c r="E54" t="n">
-        <v>10594</v>
+        <v>10554</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>16565</v>
+        <v>16559</v>
       </c>
       <c r="D55" t="n">
         <v>28127</v>
       </c>
       <c r="E55" t="n">
-        <v>11561</v>
+        <v>11567</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>16565</v>
+        <v>16521</v>
       </c>
       <c r="D56" t="n">
         <v>29061</v>
       </c>
       <c r="E56" t="n">
-        <v>12496</v>
+        <v>12540</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>16575</v>
+        <v>16508</v>
       </c>
       <c r="D57" t="n">
         <v>29976</v>
       </c>
       <c r="E57" t="n">
-        <v>13401</v>
+        <v>13468</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>16591</v>
+        <v>16470</v>
       </c>
       <c r="D58" t="n">
         <v>30886</v>
       </c>
       <c r="E58" t="n">
-        <v>14295</v>
+        <v>14416</v>
       </c>
     </row>
     <row r="59">
@@ -1354,13 +1354,13 @@
         <v>2035</v>
       </c>
       <c r="C59" t="n">
-        <v>16613</v>
+        <v>16419</v>
       </c>
       <c r="D59" t="n">
         <v>31782</v>
       </c>
       <c r="E59" t="n">
-        <v>15169</v>
+        <v>15363</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>16643</v>
+        <v>16381</v>
       </c>
       <c r="D60" t="n">
         <v>32658</v>
       </c>
       <c r="E60" t="n">
-        <v>16015</v>
+        <v>16277</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>16689</v>
+        <v>16388</v>
       </c>
       <c r="D61" t="n">
         <v>33531</v>
       </c>
       <c r="E61" t="n">
-        <v>16842</v>
+        <v>17143</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>16744</v>
+        <v>16420</v>
       </c>
       <c r="D62" t="n">
         <v>34404</v>
       </c>
       <c r="E62" t="n">
-        <v>17660</v>
+        <v>17984</v>
       </c>
     </row>
     <row r="63">
@@ -1414,13 +1414,13 @@
         <v>2039</v>
       </c>
       <c r="C63" t="n">
-        <v>16804</v>
+        <v>16459</v>
       </c>
       <c r="D63" t="n">
         <v>35275</v>
       </c>
       <c r="E63" t="n">
-        <v>18471</v>
+        <v>18815</v>
       </c>
     </row>
     <row r="64">
@@ -1429,13 +1429,13 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>16866</v>
+        <v>16508</v>
       </c>
       <c r="D64" t="n">
         <v>36130</v>
       </c>
       <c r="E64" t="n">
-        <v>19264</v>
+        <v>19622</v>
       </c>
     </row>
     <row r="65">
@@ -1448,13 +1448,13 @@
         <v>2020</v>
       </c>
       <c r="C65" t="n">
-        <v>30732</v>
+        <v>30789</v>
       </c>
       <c r="D65" t="n">
         <v>30733</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>-57</v>
       </c>
     </row>
     <row r="66">
@@ -1463,13 +1463,13 @@
         <v>2021</v>
       </c>
       <c r="C66" t="n">
-        <v>30821</v>
+        <v>30830</v>
       </c>
       <c r="D66" t="n">
         <v>30793</v>
       </c>
       <c r="E66" t="n">
-        <v>-28</v>
+        <v>-37</v>
       </c>
     </row>
     <row r="67">
@@ -1478,13 +1478,13 @@
         <v>2022</v>
       </c>
       <c r="C67" t="n">
-        <v>30975</v>
+        <v>30941</v>
       </c>
       <c r="D67" t="n">
         <v>30890</v>
       </c>
       <c r="E67" t="n">
-        <v>-85</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="68">
@@ -1493,13 +1493,13 @@
         <v>2023</v>
       </c>
       <c r="C68" t="n">
-        <v>31104</v>
+        <v>31020</v>
       </c>
       <c r="D68" t="n">
         <v>31004</v>
       </c>
       <c r="E68" t="n">
-        <v>-100</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="69">
@@ -1508,13 +1508,13 @@
         <v>2024</v>
       </c>
       <c r="C69" t="n">
-        <v>31186</v>
+        <v>31065</v>
       </c>
       <c r="D69" t="n">
         <v>31130</v>
       </c>
       <c r="E69" t="n">
-        <v>-57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70">
@@ -1523,13 +1523,13 @@
         <v>2025</v>
       </c>
       <c r="C70" t="n">
-        <v>31277</v>
+        <v>31124</v>
       </c>
       <c r="D70" t="n">
         <v>31256</v>
       </c>
       <c r="E70" t="n">
-        <v>-20</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71">
@@ -1538,13 +1538,13 @@
         <v>2026</v>
       </c>
       <c r="C71" t="n">
-        <v>31334</v>
+        <v>31163</v>
       </c>
       <c r="D71" t="n">
         <v>31384</v>
       </c>
       <c r="E71" t="n">
-        <v>50</v>
+        <v>221</v>
       </c>
     </row>
     <row r="72">
@@ -1553,13 +1553,13 @@
         <v>2027</v>
       </c>
       <c r="C72" t="n">
-        <v>31338</v>
+        <v>31158</v>
       </c>
       <c r="D72" t="n">
         <v>31496</v>
       </c>
       <c r="E72" t="n">
-        <v>158</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73">
@@ -1568,13 +1568,13 @@
         <v>2028</v>
       </c>
       <c r="C73" t="n">
-        <v>31213</v>
+        <v>31043</v>
       </c>
       <c r="D73" t="n">
         <v>31594</v>
       </c>
       <c r="E73" t="n">
-        <v>381</v>
+        <v>550</v>
       </c>
     </row>
     <row r="74">
@@ -1583,13 +1583,13 @@
         <v>2029</v>
       </c>
       <c r="C74" t="n">
-        <v>31036</v>
+        <v>30887</v>
       </c>
       <c r="D74" t="n">
         <v>31672</v>
       </c>
       <c r="E74" t="n">
-        <v>637</v>
+        <v>785</v>
       </c>
     </row>
     <row r="75">
@@ -1598,13 +1598,13 @@
         <v>2030</v>
       </c>
       <c r="C75" t="n">
-        <v>30852</v>
+        <v>30725</v>
       </c>
       <c r="D75" t="n">
         <v>31717</v>
       </c>
       <c r="E75" t="n">
-        <v>865</v>
+        <v>993</v>
       </c>
     </row>
     <row r="76">
@@ -1613,13 +1613,13 @@
         <v>2031</v>
       </c>
       <c r="C76" t="n">
-        <v>30725</v>
+        <v>30605</v>
       </c>
       <c r="D76" t="n">
         <v>31726</v>
       </c>
       <c r="E76" t="n">
-        <v>1000</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="77">
@@ -1628,13 +1628,13 @@
         <v>2032</v>
       </c>
       <c r="C77" t="n">
-        <v>30641</v>
+        <v>30514</v>
       </c>
       <c r="D77" t="n">
         <v>31699</v>
       </c>
       <c r="E77" t="n">
-        <v>1058</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="78">
@@ -1643,13 +1643,13 @@
         <v>2033</v>
       </c>
       <c r="C78" t="n">
-        <v>30624</v>
+        <v>30472</v>
       </c>
       <c r="D78" t="n">
         <v>31633</v>
       </c>
       <c r="E78" t="n">
-        <v>1009</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="79">
@@ -1658,13 +1658,13 @@
         <v>2034</v>
       </c>
       <c r="C79" t="n">
-        <v>30558</v>
+        <v>30374</v>
       </c>
       <c r="D79" t="n">
         <v>31553</v>
       </c>
       <c r="E79" t="n">
-        <v>994</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="80">
@@ -1673,13 +1673,13 @@
         <v>2035</v>
       </c>
       <c r="C80" t="n">
-        <v>30469</v>
+        <v>30247</v>
       </c>
       <c r="D80" t="n">
         <v>31437</v>
       </c>
       <c r="E80" t="n">
-        <v>968</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="81">
@@ -1688,13 +1688,13 @@
         <v>2036</v>
       </c>
       <c r="C81" t="n">
-        <v>30408</v>
+        <v>30145</v>
       </c>
       <c r="D81" t="n">
         <v>31322</v>
       </c>
       <c r="E81" t="n">
-        <v>914</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="82">
@@ -1703,13 +1703,13 @@
         <v>2037</v>
       </c>
       <c r="C82" t="n">
-        <v>30450</v>
+        <v>30134</v>
       </c>
       <c r="D82" t="n">
         <v>31190</v>
       </c>
       <c r="E82" t="n">
-        <v>740</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="83">
@@ -1718,13 +1718,13 @@
         <v>2038</v>
       </c>
       <c r="C83" t="n">
-        <v>30553</v>
+        <v>30174</v>
       </c>
       <c r="D83" t="n">
         <v>31069</v>
       </c>
       <c r="E83" t="n">
-        <v>516</v>
+        <v>895</v>
       </c>
     </row>
     <row r="84">
@@ -1733,13 +1733,13 @@
         <v>2039</v>
       </c>
       <c r="C84" t="n">
-        <v>30676</v>
+        <v>30226</v>
       </c>
       <c r="D84" t="n">
         <v>30946</v>
       </c>
       <c r="E84" t="n">
-        <v>270</v>
+        <v>721</v>
       </c>
     </row>
     <row r="85">
@@ -1748,13 +1748,13 @@
         <v>2040</v>
       </c>
       <c r="C85" t="n">
-        <v>30821</v>
+        <v>30298</v>
       </c>
       <c r="D85" t="n">
         <v>30834</v>
       </c>
       <c r="E85" t="n">
-        <v>13</v>
+        <v>536</v>
       </c>
     </row>
     <row r="86">
@@ -1767,13 +1767,13 @@
         <v>2020</v>
       </c>
       <c r="C86" t="n">
-        <v>13249</v>
+        <v>13299</v>
       </c>
       <c r="D86" t="n">
         <v>13248</v>
       </c>
       <c r="E86" t="n">
-        <v>-1</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="87">
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>13275</v>
+        <v>13329</v>
       </c>
       <c r="D87" t="n">
         <v>13226</v>
       </c>
       <c r="E87" t="n">
-        <v>-50</v>
+        <v>-103</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>13336</v>
+        <v>13392</v>
       </c>
       <c r="D88" t="n">
         <v>13190</v>
       </c>
       <c r="E88" t="n">
-        <v>-146</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>13396</v>
+        <v>13454</v>
       </c>
       <c r="D89" t="n">
         <v>13140</v>
       </c>
       <c r="E89" t="n">
-        <v>-256</v>
+        <v>-314</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>13442</v>
+        <v>13503</v>
       </c>
       <c r="D90" t="n">
         <v>13091</v>
       </c>
       <c r="E90" t="n">
-        <v>-351</v>
+        <v>-412</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>13513</v>
+        <v>13575</v>
       </c>
       <c r="D91" t="n">
         <v>13024</v>
       </c>
       <c r="E91" t="n">
-        <v>-489</v>
+        <v>-551</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>13578</v>
+        <v>13641</v>
       </c>
       <c r="D92" t="n">
         <v>12945</v>
       </c>
       <c r="E92" t="n">
-        <v>-634</v>
+        <v>-697</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>13612</v>
+        <v>13677</v>
       </c>
       <c r="D93" t="n">
         <v>12866</v>
       </c>
       <c r="E93" t="n">
-        <v>-746</v>
+        <v>-812</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>13570</v>
+        <v>13642</v>
       </c>
       <c r="D94" t="n">
         <v>12763</v>
       </c>
       <c r="E94" t="n">
-        <v>-807</v>
+        <v>-878</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>13502</v>
+        <v>13580</v>
       </c>
       <c r="D95" t="n">
         <v>12664</v>
       </c>
       <c r="E95" t="n">
-        <v>-838</v>
+        <v>-917</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>13420</v>
+        <v>13506</v>
       </c>
       <c r="D96" t="n">
         <v>12555</v>
       </c>
       <c r="E96" t="n">
-        <v>-864</v>
+        <v>-951</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>13362</v>
+        <v>13455</v>
       </c>
       <c r="D97" t="n">
         <v>12434</v>
       </c>
       <c r="E97" t="n">
-        <v>-927</v>
+        <v>-1021</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>13318</v>
+        <v>13417</v>
       </c>
       <c r="D98" t="n">
         <v>12321</v>
       </c>
       <c r="E98" t="n">
-        <v>-997</v>
+        <v>-1097</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>13301</v>
+        <v>13406</v>
       </c>
       <c r="D99" t="n">
         <v>12191</v>
       </c>
       <c r="E99" t="n">
-        <v>-1110</v>
+        <v>-1215</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>13235</v>
+        <v>13348</v>
       </c>
       <c r="D100" t="n">
         <v>12080</v>
       </c>
       <c r="E100" t="n">
-        <v>-1155</v>
+        <v>-1268</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>13143</v>
+        <v>13265</v>
       </c>
       <c r="D101" t="n">
         <v>11961</v>
       </c>
       <c r="E101" t="n">
-        <v>-1182</v>
+        <v>-1304</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>13061</v>
+        <v>13192</v>
       </c>
       <c r="D102" t="n">
         <v>11852</v>
       </c>
       <c r="E102" t="n">
-        <v>-1209</v>
+        <v>-1340</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>13033</v>
+        <v>13170</v>
       </c>
       <c r="D103" t="n">
         <v>11748</v>
       </c>
       <c r="E103" t="n">
-        <v>-1284</v>
+        <v>-1422</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>13033</v>
+        <v>13176</v>
       </c>
       <c r="D104" t="n">
         <v>11635</v>
       </c>
       <c r="E104" t="n">
-        <v>-1399</v>
+        <v>-1541</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>13037</v>
+        <v>13184</v>
       </c>
       <c r="D105" t="n">
         <v>11542</v>
       </c>
       <c r="E105" t="n">
-        <v>-1496</v>
+        <v>-1643</v>
       </c>
     </row>
     <row r="106">
@@ -2067,13 +2067,13 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
-        <v>13053</v>
+        <v>13204</v>
       </c>
       <c r="D106" t="n">
         <v>11443</v>
       </c>
       <c r="E106" t="n">
-        <v>-1610</v>
+        <v>-1761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Endret aldersinndeling for elever i videregående skole og satt tilbud i basisåret lik Sysselsatt lærere.
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -467,12 +467,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Etterspørsel</t>
+          <t>Tilbud</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Tilbud</t>
+          <t>Etterspørsel</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -494,10 +494,10 @@
         <v>47134</v>
       </c>
       <c r="D2" t="n">
-        <v>47126</v>
+        <v>47134</v>
       </c>
       <c r="E2" t="n">
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -506,13 +506,13 @@
         <v>2021</v>
       </c>
       <c r="C3" t="n">
+        <v>48005</v>
+      </c>
+      <c r="D3" t="n">
         <v>46522</v>
       </c>
-      <c r="D3" t="n">
-        <v>48005</v>
-      </c>
       <c r="E3" t="n">
-        <v>1483</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="4">
@@ -521,13 +521,13 @@
         <v>2022</v>
       </c>
       <c r="C4" t="n">
+        <v>49055</v>
+      </c>
+      <c r="D4" t="n">
         <v>45972</v>
       </c>
-      <c r="D4" t="n">
-        <v>49055</v>
-      </c>
       <c r="E4" t="n">
-        <v>3083</v>
+        <v>3084</v>
       </c>
     </row>
     <row r="5">
@@ -536,13 +536,13 @@
         <v>2023</v>
       </c>
       <c r="C5" t="n">
-        <v>45818</v>
+        <v>50112</v>
       </c>
       <c r="D5" t="n">
-        <v>50112</v>
+        <v>45817</v>
       </c>
       <c r="E5" t="n">
-        <v>4294</v>
+        <v>4295</v>
       </c>
     </row>
     <row r="6">
@@ -551,13 +551,13 @@
         <v>2024</v>
       </c>
       <c r="C6" t="n">
-        <v>45550</v>
+        <v>51175</v>
       </c>
       <c r="D6" t="n">
-        <v>51175</v>
+        <v>45549</v>
       </c>
       <c r="E6" t="n">
-        <v>5624</v>
+        <v>5625</v>
       </c>
     </row>
     <row r="7">
@@ -566,13 +566,13 @@
         <v>2025</v>
       </c>
       <c r="C7" t="n">
-        <v>45403</v>
+        <v>52234</v>
       </c>
       <c r="D7" t="n">
-        <v>52234</v>
+        <v>45402</v>
       </c>
       <c r="E7" t="n">
-        <v>6831</v>
+        <v>6832</v>
       </c>
     </row>
     <row r="8">
@@ -581,13 +581,13 @@
         <v>2026</v>
       </c>
       <c r="C8" t="n">
-        <v>45343</v>
+        <v>53293</v>
       </c>
       <c r="D8" t="n">
-        <v>53293</v>
+        <v>45341</v>
       </c>
       <c r="E8" t="n">
-        <v>7950</v>
+        <v>7951</v>
       </c>
     </row>
     <row r="9">
@@ -596,13 +596,13 @@
         <v>2027</v>
       </c>
       <c r="C9" t="n">
-        <v>45380</v>
+        <v>54325</v>
       </c>
       <c r="D9" t="n">
-        <v>54325</v>
+        <v>45379</v>
       </c>
       <c r="E9" t="n">
-        <v>8945</v>
+        <v>8946</v>
       </c>
     </row>
     <row r="10">
@@ -611,13 +611,13 @@
         <v>2028</v>
       </c>
       <c r="C10" t="n">
-        <v>45504</v>
+        <v>55330</v>
       </c>
       <c r="D10" t="n">
-        <v>55330</v>
+        <v>45502</v>
       </c>
       <c r="E10" t="n">
-        <v>9826</v>
+        <v>9827</v>
       </c>
     </row>
     <row r="11">
@@ -626,13 +626,13 @@
         <v>2029</v>
       </c>
       <c r="C11" t="n">
-        <v>45709</v>
+        <v>56277</v>
       </c>
       <c r="D11" t="n">
-        <v>56277</v>
+        <v>45707</v>
       </c>
       <c r="E11" t="n">
-        <v>10568</v>
+        <v>10570</v>
       </c>
     </row>
     <row r="12">
@@ -641,13 +641,13 @@
         <v>2030</v>
       </c>
       <c r="C12" t="n">
-        <v>45945</v>
+        <v>57146</v>
       </c>
       <c r="D12" t="n">
-        <v>57146</v>
+        <v>45943</v>
       </c>
       <c r="E12" t="n">
-        <v>11201</v>
+        <v>11203</v>
       </c>
     </row>
     <row r="13">
@@ -656,13 +656,13 @@
         <v>2031</v>
       </c>
       <c r="C13" t="n">
-        <v>46196</v>
+        <v>57939</v>
       </c>
       <c r="D13" t="n">
-        <v>57939</v>
+        <v>46193</v>
       </c>
       <c r="E13" t="n">
-        <v>11743</v>
+        <v>11746</v>
       </c>
     </row>
     <row r="14">
@@ -671,13 +671,13 @@
         <v>2032</v>
       </c>
       <c r="C14" t="n">
-        <v>46444</v>
+        <v>58633</v>
       </c>
       <c r="D14" t="n">
-        <v>58633</v>
+        <v>46442</v>
       </c>
       <c r="E14" t="n">
-        <v>12188</v>
+        <v>12191</v>
       </c>
     </row>
     <row r="15">
@@ -686,13 +686,13 @@
         <v>2033</v>
       </c>
       <c r="C15" t="n">
-        <v>46698</v>
+        <v>59232</v>
       </c>
       <c r="D15" t="n">
-        <v>59232</v>
+        <v>46696</v>
       </c>
       <c r="E15" t="n">
-        <v>12533</v>
+        <v>12536</v>
       </c>
     </row>
     <row r="16">
@@ -701,13 +701,13 @@
         <v>2034</v>
       </c>
       <c r="C16" t="n">
-        <v>46989</v>
+        <v>59752</v>
       </c>
       <c r="D16" t="n">
-        <v>59752</v>
+        <v>46986</v>
       </c>
       <c r="E16" t="n">
-        <v>12763</v>
+        <v>12766</v>
       </c>
     </row>
     <row r="17">
@@ -716,13 +716,13 @@
         <v>2035</v>
       </c>
       <c r="C17" t="n">
-        <v>47311</v>
+        <v>60185</v>
       </c>
       <c r="D17" t="n">
-        <v>60185</v>
+        <v>47308</v>
       </c>
       <c r="E17" t="n">
-        <v>12874</v>
+        <v>12878</v>
       </c>
     </row>
     <row r="18">
@@ -731,13 +731,13 @@
         <v>2036</v>
       </c>
       <c r="C18" t="n">
-        <v>47656</v>
+        <v>60574</v>
       </c>
       <c r="D18" t="n">
-        <v>60574</v>
+        <v>47652</v>
       </c>
       <c r="E18" t="n">
-        <v>12918</v>
+        <v>12922</v>
       </c>
     </row>
     <row r="19">
@@ -746,13 +746,13 @@
         <v>2037</v>
       </c>
       <c r="C19" t="n">
-        <v>48017</v>
+        <v>60940</v>
       </c>
       <c r="D19" t="n">
-        <v>60940</v>
+        <v>48013</v>
       </c>
       <c r="E19" t="n">
-        <v>12923</v>
+        <v>12927</v>
       </c>
     </row>
     <row r="20">
@@ -761,13 +761,13 @@
         <v>2038</v>
       </c>
       <c r="C20" t="n">
-        <v>48352</v>
+        <v>61317</v>
       </c>
       <c r="D20" t="n">
-        <v>61317</v>
+        <v>48348</v>
       </c>
       <c r="E20" t="n">
-        <v>12966</v>
+        <v>12970</v>
       </c>
     </row>
     <row r="21">
@@ -776,13 +776,13 @@
         <v>2039</v>
       </c>
       <c r="C21" t="n">
-        <v>48612</v>
+        <v>61723</v>
       </c>
       <c r="D21" t="n">
-        <v>61723</v>
+        <v>48608</v>
       </c>
       <c r="E21" t="n">
-        <v>13111</v>
+        <v>13115</v>
       </c>
     </row>
     <row r="22">
@@ -791,32 +791,32 @@
         <v>2040</v>
       </c>
       <c r="C22" t="n">
-        <v>48798</v>
+        <v>62181</v>
       </c>
       <c r="D22" t="n">
-        <v>62181</v>
+        <v>48793</v>
       </c>
       <c r="E22" t="n">
-        <v>13383</v>
+        <v>13387</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Grunnskolelærere</t>
+          <t>Faglærere</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C23" t="n">
-        <v>52497</v>
+        <v>16600</v>
       </c>
       <c r="D23" t="n">
-        <v>52381</v>
+        <v>16600</v>
       </c>
       <c r="E23" t="n">
-        <v>-116</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -825,13 +825,13 @@
         <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>52460</v>
+        <v>17578</v>
       </c>
       <c r="D24" t="n">
-        <v>52773</v>
+        <v>16622</v>
       </c>
       <c r="E24" t="n">
-        <v>313</v>
+        <v>956</v>
       </c>
     </row>
     <row r="25">
@@ -840,13 +840,13 @@
         <v>2022</v>
       </c>
       <c r="C25" t="n">
-        <v>52490</v>
+        <v>18647</v>
       </c>
       <c r="D25" t="n">
-        <v>53233</v>
+        <v>16681</v>
       </c>
       <c r="E25" t="n">
-        <v>743</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="26">
@@ -855,13 +855,13 @@
         <v>2023</v>
       </c>
       <c r="C26" t="n">
-        <v>52350</v>
+        <v>19746</v>
       </c>
       <c r="D26" t="n">
-        <v>53749</v>
+        <v>16724</v>
       </c>
       <c r="E26" t="n">
-        <v>1399</v>
+        <v>3022</v>
       </c>
     </row>
     <row r="27">
@@ -870,13 +870,13 @@
         <v>2024</v>
       </c>
       <c r="C27" t="n">
-        <v>52089</v>
+        <v>20847</v>
       </c>
       <c r="D27" t="n">
-        <v>54321</v>
+        <v>16749</v>
       </c>
       <c r="E27" t="n">
-        <v>2232</v>
+        <v>4098</v>
       </c>
     </row>
     <row r="28">
@@ -885,13 +885,13 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>51644</v>
+        <v>21949</v>
       </c>
       <c r="D28" t="n">
-        <v>54931</v>
+        <v>16780</v>
       </c>
       <c r="E28" t="n">
-        <v>3288</v>
+        <v>5169</v>
       </c>
     </row>
     <row r="29">
@@ -900,13 +900,13 @@
         <v>2026</v>
       </c>
       <c r="C29" t="n">
-        <v>51101</v>
+        <v>23031</v>
       </c>
       <c r="D29" t="n">
-        <v>55547</v>
+        <v>16801</v>
       </c>
       <c r="E29" t="n">
-        <v>4446</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="30">
@@ -915,13 +915,13 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>50608</v>
+        <v>24103</v>
       </c>
       <c r="D30" t="n">
-        <v>56193</v>
+        <v>16800</v>
       </c>
       <c r="E30" t="n">
-        <v>5586</v>
+        <v>7303</v>
       </c>
     </row>
     <row r="31">
@@ -930,13 +930,13 @@
         <v>2028</v>
       </c>
       <c r="C31" t="n">
-        <v>50174</v>
+        <v>25145</v>
       </c>
       <c r="D31" t="n">
-        <v>56819</v>
+        <v>16746</v>
       </c>
       <c r="E31" t="n">
-        <v>6645</v>
+        <v>8400</v>
       </c>
     </row>
     <row r="32">
@@ -945,13 +945,13 @@
         <v>2029</v>
       </c>
       <c r="C32" t="n">
-        <v>49736</v>
+        <v>26173</v>
       </c>
       <c r="D32" t="n">
-        <v>57406</v>
+        <v>16669</v>
       </c>
       <c r="E32" t="n">
-        <v>7670</v>
+        <v>9503</v>
       </c>
     </row>
     <row r="33">
@@ -960,13 +960,13 @@
         <v>2030</v>
       </c>
       <c r="C33" t="n">
-        <v>49415</v>
+        <v>27167</v>
       </c>
       <c r="D33" t="n">
-        <v>57928</v>
+        <v>16591</v>
       </c>
       <c r="E33" t="n">
-        <v>8514</v>
+        <v>10576</v>
       </c>
     </row>
     <row r="34">
@@ -975,13 +975,13 @@
         <v>2031</v>
       </c>
       <c r="C34" t="n">
-        <v>49137</v>
+        <v>28127</v>
       </c>
       <c r="D34" t="n">
-        <v>58391</v>
+        <v>16535</v>
       </c>
       <c r="E34" t="n">
-        <v>9254</v>
+        <v>11592</v>
       </c>
     </row>
     <row r="35">
@@ -990,13 +990,13 @@
         <v>2032</v>
       </c>
       <c r="C35" t="n">
-        <v>48916</v>
+        <v>29061</v>
       </c>
       <c r="D35" t="n">
-        <v>58778</v>
+        <v>16495</v>
       </c>
       <c r="E35" t="n">
-        <v>9861</v>
+        <v>12567</v>
       </c>
     </row>
     <row r="36">
@@ -1005,13 +1005,13 @@
         <v>2033</v>
       </c>
       <c r="C36" t="n">
-        <v>48755</v>
+        <v>29976</v>
       </c>
       <c r="D36" t="n">
-        <v>59083</v>
+        <v>16480</v>
       </c>
       <c r="E36" t="n">
-        <v>10328</v>
+        <v>13496</v>
       </c>
     </row>
     <row r="37">
@@ -1020,13 +1020,13 @@
         <v>2034</v>
       </c>
       <c r="C37" t="n">
-        <v>48754</v>
+        <v>30886</v>
       </c>
       <c r="D37" t="n">
-        <v>59331</v>
+        <v>16440</v>
       </c>
       <c r="E37" t="n">
-        <v>10577</v>
+        <v>14447</v>
       </c>
     </row>
     <row r="38">
@@ -1035,13 +1035,13 @@
         <v>2035</v>
       </c>
       <c r="C38" t="n">
-        <v>48860</v>
+        <v>31782</v>
       </c>
       <c r="D38" t="n">
-        <v>59522</v>
+        <v>16386</v>
       </c>
       <c r="E38" t="n">
-        <v>10662</v>
+        <v>15396</v>
       </c>
     </row>
     <row r="39">
@@ -1050,13 +1050,13 @@
         <v>2036</v>
       </c>
       <c r="C39" t="n">
-        <v>49030</v>
+        <v>32658</v>
       </c>
       <c r="D39" t="n">
-        <v>59689</v>
+        <v>16345</v>
       </c>
       <c r="E39" t="n">
-        <v>10659</v>
+        <v>16313</v>
       </c>
     </row>
     <row r="40">
@@ -1065,13 +1065,13 @@
         <v>2037</v>
       </c>
       <c r="C40" t="n">
-        <v>49248</v>
+        <v>33531</v>
       </c>
       <c r="D40" t="n">
-        <v>59849</v>
+        <v>16350</v>
       </c>
       <c r="E40" t="n">
-        <v>10600</v>
+        <v>17181</v>
       </c>
     </row>
     <row r="41">
@@ -1080,13 +1080,13 @@
         <v>2038</v>
       </c>
       <c r="C41" t="n">
-        <v>49514</v>
+        <v>34404</v>
       </c>
       <c r="D41" t="n">
-        <v>60004</v>
+        <v>16381</v>
       </c>
       <c r="E41" t="n">
-        <v>10490</v>
+        <v>18024</v>
       </c>
     </row>
     <row r="42">
@@ -1095,13 +1095,13 @@
         <v>2039</v>
       </c>
       <c r="C42" t="n">
-        <v>49834</v>
+        <v>35275</v>
       </c>
       <c r="D42" t="n">
-        <v>60182</v>
+        <v>16417</v>
       </c>
       <c r="E42" t="n">
-        <v>10348</v>
+        <v>18858</v>
       </c>
     </row>
     <row r="43">
@@ -1110,32 +1110,32 @@
         <v>2040</v>
       </c>
       <c r="C43" t="n">
-        <v>50172</v>
+        <v>36130</v>
       </c>
       <c r="D43" t="n">
-        <v>60374</v>
+        <v>16463</v>
       </c>
       <c r="E43" t="n">
-        <v>10203</v>
+        <v>19667</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Faglærere</t>
+          <t>Grunnskolelærere</t>
         </is>
       </c>
       <c r="B44" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C44" t="n">
-        <v>16600</v>
+        <v>52497</v>
       </c>
       <c r="D44" t="n">
-        <v>16557</v>
+        <v>52497</v>
       </c>
       <c r="E44" t="n">
-        <v>-43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1144,13 +1144,13 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>16625</v>
+        <v>52773</v>
       </c>
       <c r="D45" t="n">
-        <v>17578</v>
+        <v>52459</v>
       </c>
       <c r="E45" t="n">
-        <v>953</v>
+        <v>314</v>
       </c>
     </row>
     <row r="46">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>16686</v>
+        <v>53233</v>
       </c>
       <c r="D46" t="n">
-        <v>18647</v>
+        <v>52487</v>
       </c>
       <c r="E46" t="n">
-        <v>1960</v>
+        <v>746</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>16732</v>
+        <v>53749</v>
       </c>
       <c r="D47" t="n">
-        <v>19746</v>
+        <v>52346</v>
       </c>
       <c r="E47" t="n">
-        <v>3014</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>16759</v>
+        <v>54321</v>
       </c>
       <c r="D48" t="n">
-        <v>20847</v>
+        <v>52084</v>
       </c>
       <c r="E48" t="n">
-        <v>4088</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="49">
@@ -1204,13 +1204,13 @@
         <v>2025</v>
       </c>
       <c r="C49" t="n">
-        <v>16792</v>
+        <v>54931</v>
       </c>
       <c r="D49" t="n">
-        <v>21949</v>
+        <v>51638</v>
       </c>
       <c r="E49" t="n">
-        <v>5157</v>
+        <v>3294</v>
       </c>
     </row>
     <row r="50">
@@ -1219,13 +1219,13 @@
         <v>2026</v>
       </c>
       <c r="C50" t="n">
-        <v>16814</v>
+        <v>55547</v>
       </c>
       <c r="D50" t="n">
-        <v>23031</v>
+        <v>51095</v>
       </c>
       <c r="E50" t="n">
-        <v>6217</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>16815</v>
+        <v>56193</v>
       </c>
       <c r="D51" t="n">
-        <v>24103</v>
+        <v>50601</v>
       </c>
       <c r="E51" t="n">
-        <v>7288</v>
+        <v>5593</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>16763</v>
+        <v>56819</v>
       </c>
       <c r="D52" t="n">
-        <v>25145</v>
+        <v>50166</v>
       </c>
       <c r="E52" t="n">
-        <v>8383</v>
+        <v>6653</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>16689</v>
+        <v>57406</v>
       </c>
       <c r="D53" t="n">
-        <v>26173</v>
+        <v>49727</v>
       </c>
       <c r="E53" t="n">
-        <v>9484</v>
+        <v>7679</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1279,13 @@
         <v>2030</v>
       </c>
       <c r="C54" t="n">
-        <v>16613</v>
+        <v>57928</v>
       </c>
       <c r="D54" t="n">
-        <v>27167</v>
+        <v>49404</v>
       </c>
       <c r="E54" t="n">
-        <v>10554</v>
+        <v>8524</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>16559</v>
+        <v>58391</v>
       </c>
       <c r="D55" t="n">
-        <v>28127</v>
+        <v>49125</v>
       </c>
       <c r="E55" t="n">
-        <v>11567</v>
+        <v>9266</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>16521</v>
+        <v>58778</v>
       </c>
       <c r="D56" t="n">
-        <v>29061</v>
+        <v>48904</v>
       </c>
       <c r="E56" t="n">
-        <v>12540</v>
+        <v>9874</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>16508</v>
+        <v>59083</v>
       </c>
       <c r="D57" t="n">
-        <v>29976</v>
+        <v>48741</v>
       </c>
       <c r="E57" t="n">
-        <v>13468</v>
+        <v>10342</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>16470</v>
+        <v>59331</v>
       </c>
       <c r="D58" t="n">
-        <v>30886</v>
+        <v>48739</v>
       </c>
       <c r="E58" t="n">
-        <v>14416</v>
+        <v>10592</v>
       </c>
     </row>
     <row r="59">
@@ -1354,13 +1354,13 @@
         <v>2035</v>
       </c>
       <c r="C59" t="n">
-        <v>16419</v>
+        <v>59522</v>
       </c>
       <c r="D59" t="n">
-        <v>31782</v>
+        <v>48844</v>
       </c>
       <c r="E59" t="n">
-        <v>15363</v>
+        <v>10678</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>16381</v>
+        <v>59689</v>
       </c>
       <c r="D60" t="n">
-        <v>32658</v>
+        <v>49013</v>
       </c>
       <c r="E60" t="n">
-        <v>16277</v>
+        <v>10676</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>16388</v>
+        <v>59849</v>
       </c>
       <c r="D61" t="n">
-        <v>33531</v>
+        <v>49230</v>
       </c>
       <c r="E61" t="n">
-        <v>17143</v>
+        <v>10618</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>16420</v>
+        <v>60004</v>
       </c>
       <c r="D62" t="n">
-        <v>34404</v>
+        <v>49495</v>
       </c>
       <c r="E62" t="n">
-        <v>17984</v>
+        <v>10509</v>
       </c>
     </row>
     <row r="63">
@@ -1414,13 +1414,13 @@
         <v>2039</v>
       </c>
       <c r="C63" t="n">
-        <v>16459</v>
+        <v>60182</v>
       </c>
       <c r="D63" t="n">
-        <v>35275</v>
+        <v>49814</v>
       </c>
       <c r="E63" t="n">
-        <v>18815</v>
+        <v>10369</v>
       </c>
     </row>
     <row r="64">
@@ -1429,13 +1429,13 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>16508</v>
+        <v>60374</v>
       </c>
       <c r="D64" t="n">
-        <v>36130</v>
+        <v>50150</v>
       </c>
       <c r="E64" t="n">
-        <v>19622</v>
+        <v>10224</v>
       </c>
     </row>
     <row r="65">
@@ -1451,10 +1451,10 @@
         <v>30789</v>
       </c>
       <c r="D65" t="n">
-        <v>30733</v>
+        <v>30789</v>
       </c>
       <c r="E65" t="n">
-        <v>-57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1463,13 +1463,13 @@
         <v>2021</v>
       </c>
       <c r="C66" t="n">
-        <v>30830</v>
+        <v>30793</v>
       </c>
       <c r="D66" t="n">
-        <v>30793</v>
+        <v>30824</v>
       </c>
       <c r="E66" t="n">
-        <v>-37</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="67">
@@ -1478,13 +1478,13 @@
         <v>2022</v>
       </c>
       <c r="C67" t="n">
-        <v>30941</v>
+        <v>30890</v>
       </c>
       <c r="D67" t="n">
-        <v>30890</v>
+        <v>30930</v>
       </c>
       <c r="E67" t="n">
-        <v>-51</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="68">
@@ -1493,13 +1493,13 @@
         <v>2023</v>
       </c>
       <c r="C68" t="n">
-        <v>31020</v>
+        <v>31004</v>
       </c>
       <c r="D68" t="n">
         <v>31004</v>
       </c>
       <c r="E68" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1508,13 +1508,13 @@
         <v>2024</v>
       </c>
       <c r="C69" t="n">
-        <v>31065</v>
+        <v>31130</v>
       </c>
       <c r="D69" t="n">
-        <v>31130</v>
+        <v>31044</v>
       </c>
       <c r="E69" t="n">
-        <v>64</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70">
@@ -1523,13 +1523,13 @@
         <v>2025</v>
       </c>
       <c r="C70" t="n">
-        <v>31124</v>
+        <v>31256</v>
       </c>
       <c r="D70" t="n">
-        <v>31256</v>
+        <v>31100</v>
       </c>
       <c r="E70" t="n">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71">
@@ -1538,13 +1538,13 @@
         <v>2026</v>
       </c>
       <c r="C71" t="n">
-        <v>31163</v>
+        <v>31384</v>
       </c>
       <c r="D71" t="n">
-        <v>31384</v>
+        <v>31135</v>
       </c>
       <c r="E71" t="n">
-        <v>221</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72">
@@ -1553,13 +1553,13 @@
         <v>2027</v>
       </c>
       <c r="C72" t="n">
-        <v>31158</v>
+        <v>31496</v>
       </c>
       <c r="D72" t="n">
-        <v>31496</v>
+        <v>31127</v>
       </c>
       <c r="E72" t="n">
-        <v>339</v>
+        <v>369</v>
       </c>
     </row>
     <row r="73">
@@ -1568,13 +1568,13 @@
         <v>2028</v>
       </c>
       <c r="C73" t="n">
-        <v>31043</v>
+        <v>31594</v>
       </c>
       <c r="D73" t="n">
-        <v>31594</v>
+        <v>31009</v>
       </c>
       <c r="E73" t="n">
-        <v>550</v>
+        <v>585</v>
       </c>
     </row>
     <row r="74">
@@ -1583,13 +1583,13 @@
         <v>2029</v>
       </c>
       <c r="C74" t="n">
-        <v>30887</v>
+        <v>31672</v>
       </c>
       <c r="D74" t="n">
-        <v>31672</v>
+        <v>30847</v>
       </c>
       <c r="E74" t="n">
-        <v>785</v>
+        <v>825</v>
       </c>
     </row>
     <row r="75">
@@ -1598,13 +1598,13 @@
         <v>2030</v>
       </c>
       <c r="C75" t="n">
-        <v>30725</v>
+        <v>31717</v>
       </c>
       <c r="D75" t="n">
-        <v>31717</v>
+        <v>30680</v>
       </c>
       <c r="E75" t="n">
-        <v>993</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="76">
@@ -1613,13 +1613,13 @@
         <v>2031</v>
       </c>
       <c r="C76" t="n">
-        <v>30605</v>
+        <v>31726</v>
       </c>
       <c r="D76" t="n">
-        <v>31726</v>
+        <v>30555</v>
       </c>
       <c r="E76" t="n">
-        <v>1121</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="77">
@@ -1628,13 +1628,13 @@
         <v>2032</v>
       </c>
       <c r="C77" t="n">
-        <v>30514</v>
+        <v>31699</v>
       </c>
       <c r="D77" t="n">
-        <v>31699</v>
+        <v>30461</v>
       </c>
       <c r="E77" t="n">
-        <v>1185</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="78">
@@ -1643,13 +1643,13 @@
         <v>2033</v>
       </c>
       <c r="C78" t="n">
-        <v>30472</v>
+        <v>31633</v>
       </c>
       <c r="D78" t="n">
-        <v>31633</v>
+        <v>30414</v>
       </c>
       <c r="E78" t="n">
-        <v>1161</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="79">
@@ -1658,13 +1658,13 @@
         <v>2034</v>
       </c>
       <c r="C79" t="n">
-        <v>30374</v>
+        <v>31553</v>
       </c>
       <c r="D79" t="n">
-        <v>31553</v>
+        <v>30312</v>
       </c>
       <c r="E79" t="n">
-        <v>1179</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="80">
@@ -1673,13 +1673,13 @@
         <v>2035</v>
       </c>
       <c r="C80" t="n">
-        <v>30247</v>
+        <v>31437</v>
       </c>
       <c r="D80" t="n">
-        <v>31437</v>
+        <v>30180</v>
       </c>
       <c r="E80" t="n">
-        <v>1191</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="81">
@@ -1688,13 +1688,13 @@
         <v>2036</v>
       </c>
       <c r="C81" t="n">
-        <v>30145</v>
+        <v>31322</v>
       </c>
       <c r="D81" t="n">
-        <v>31322</v>
+        <v>30072</v>
       </c>
       <c r="E81" t="n">
-        <v>1177</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="82">
@@ -1703,13 +1703,13 @@
         <v>2037</v>
       </c>
       <c r="C82" t="n">
-        <v>30134</v>
+        <v>31190</v>
       </c>
       <c r="D82" t="n">
-        <v>31190</v>
+        <v>30057</v>
       </c>
       <c r="E82" t="n">
-        <v>1056</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="83">
@@ -1718,13 +1718,13 @@
         <v>2038</v>
       </c>
       <c r="C83" t="n">
-        <v>30174</v>
+        <v>31069</v>
       </c>
       <c r="D83" t="n">
-        <v>31069</v>
+        <v>30093</v>
       </c>
       <c r="E83" t="n">
-        <v>895</v>
+        <v>976</v>
       </c>
     </row>
     <row r="84">
@@ -1733,13 +1733,13 @@
         <v>2039</v>
       </c>
       <c r="C84" t="n">
-        <v>30226</v>
+        <v>30946</v>
       </c>
       <c r="D84" t="n">
-        <v>30946</v>
+        <v>30139</v>
       </c>
       <c r="E84" t="n">
-        <v>721</v>
+        <v>807</v>
       </c>
     </row>
     <row r="85">
@@ -1748,13 +1748,13 @@
         <v>2040</v>
       </c>
       <c r="C85" t="n">
-        <v>30298</v>
+        <v>30834</v>
       </c>
       <c r="D85" t="n">
-        <v>30834</v>
+        <v>30207</v>
       </c>
       <c r="E85" t="n">
-        <v>536</v>
+        <v>627</v>
       </c>
     </row>
     <row r="86">
@@ -1770,10 +1770,10 @@
         <v>13299</v>
       </c>
       <c r="D86" t="n">
-        <v>13248</v>
+        <v>13299</v>
       </c>
       <c r="E86" t="n">
-        <v>-51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>13329</v>
+        <v>13226</v>
       </c>
       <c r="D87" t="n">
-        <v>13226</v>
+        <v>13325</v>
       </c>
       <c r="E87" t="n">
-        <v>-103</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>13392</v>
+        <v>13190</v>
       </c>
       <c r="D88" t="n">
-        <v>13190</v>
+        <v>13386</v>
       </c>
       <c r="E88" t="n">
-        <v>-202</v>
+        <v>-196</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>13454</v>
+        <v>13140</v>
       </c>
       <c r="D89" t="n">
-        <v>13140</v>
+        <v>13444</v>
       </c>
       <c r="E89" t="n">
-        <v>-314</v>
+        <v>-304</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>13503</v>
+        <v>13091</v>
       </c>
       <c r="D90" t="n">
-        <v>13091</v>
+        <v>13491</v>
       </c>
       <c r="E90" t="n">
-        <v>-412</v>
+        <v>-400</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>13575</v>
+        <v>13024</v>
       </c>
       <c r="D91" t="n">
-        <v>13024</v>
+        <v>13561</v>
       </c>
       <c r="E91" t="n">
-        <v>-551</v>
+        <v>-536</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>13641</v>
+        <v>12945</v>
       </c>
       <c r="D92" t="n">
-        <v>12945</v>
+        <v>13626</v>
       </c>
       <c r="E92" t="n">
-        <v>-697</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>13677</v>
+        <v>12866</v>
       </c>
       <c r="D93" t="n">
-        <v>12866</v>
+        <v>13660</v>
       </c>
       <c r="E93" t="n">
-        <v>-812</v>
+        <v>-794</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>13642</v>
+        <v>12763</v>
       </c>
       <c r="D94" t="n">
-        <v>12763</v>
+        <v>13622</v>
       </c>
       <c r="E94" t="n">
-        <v>-878</v>
+        <v>-858</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>13580</v>
+        <v>12664</v>
       </c>
       <c r="D95" t="n">
-        <v>12664</v>
+        <v>13558</v>
       </c>
       <c r="E95" t="n">
-        <v>-917</v>
+        <v>-894</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>13506</v>
+        <v>12555</v>
       </c>
       <c r="D96" t="n">
-        <v>12555</v>
+        <v>13480</v>
       </c>
       <c r="E96" t="n">
-        <v>-951</v>
+        <v>-925</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>13455</v>
+        <v>12434</v>
       </c>
       <c r="D97" t="n">
-        <v>12434</v>
+        <v>13426</v>
       </c>
       <c r="E97" t="n">
-        <v>-1021</v>
+        <v>-992</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>13417</v>
+        <v>12321</v>
       </c>
       <c r="D98" t="n">
-        <v>12321</v>
+        <v>13386</v>
       </c>
       <c r="E98" t="n">
-        <v>-1097</v>
+        <v>-1066</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>13406</v>
+        <v>12191</v>
       </c>
       <c r="D99" t="n">
-        <v>12191</v>
+        <v>13372</v>
       </c>
       <c r="E99" t="n">
-        <v>-1215</v>
+        <v>-1181</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>13348</v>
+        <v>12080</v>
       </c>
       <c r="D100" t="n">
-        <v>12080</v>
+        <v>13312</v>
       </c>
       <c r="E100" t="n">
-        <v>-1268</v>
+        <v>-1232</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>13265</v>
+        <v>11961</v>
       </c>
       <c r="D101" t="n">
-        <v>11961</v>
+        <v>13226</v>
       </c>
       <c r="E101" t="n">
-        <v>-1304</v>
+        <v>-1265</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>13192</v>
+        <v>11852</v>
       </c>
       <c r="D102" t="n">
-        <v>11852</v>
+        <v>13150</v>
       </c>
       <c r="E102" t="n">
-        <v>-1340</v>
+        <v>-1298</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>13170</v>
+        <v>11748</v>
       </c>
       <c r="D103" t="n">
-        <v>11748</v>
+        <v>13126</v>
       </c>
       <c r="E103" t="n">
-        <v>-1422</v>
+        <v>-1377</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>13176</v>
+        <v>11635</v>
       </c>
       <c r="D104" t="n">
-        <v>11635</v>
+        <v>13129</v>
       </c>
       <c r="E104" t="n">
-        <v>-1541</v>
+        <v>-1494</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>13184</v>
+        <v>11542</v>
       </c>
       <c r="D105" t="n">
-        <v>11542</v>
+        <v>13135</v>
       </c>
       <c r="E105" t="n">
-        <v>-1643</v>
+        <v>-1593</v>
       </c>
     </row>
     <row r="106">
@@ -2067,13 +2067,13 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
-        <v>13204</v>
+        <v>11443</v>
       </c>
       <c r="D106" t="n">
-        <v>11443</v>
+        <v>13152</v>
       </c>
       <c r="E106" t="n">
-        <v>-1761</v>
+        <v>-1709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Endret en del variabelnavn og forbedret beregning av etterspørselen i basisåret.
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -803,17 +803,17 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Faglærere</t>
+          <t>Grunnskolelærere</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C23" t="n">
-        <v>16600</v>
+        <v>52497</v>
       </c>
       <c r="D23" t="n">
-        <v>16600</v>
+        <v>52497</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -825,13 +825,13 @@
         <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>17578</v>
+        <v>52773</v>
       </c>
       <c r="D24" t="n">
-        <v>16622</v>
+        <v>52459</v>
       </c>
       <c r="E24" t="n">
-        <v>956</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25">
@@ -840,13 +840,13 @@
         <v>2022</v>
       </c>
       <c r="C25" t="n">
-        <v>18647</v>
+        <v>53233</v>
       </c>
       <c r="D25" t="n">
-        <v>16681</v>
+        <v>52487</v>
       </c>
       <c r="E25" t="n">
-        <v>1966</v>
+        <v>746</v>
       </c>
     </row>
     <row r="26">
@@ -855,13 +855,13 @@
         <v>2023</v>
       </c>
       <c r="C26" t="n">
-        <v>19746</v>
+        <v>53749</v>
       </c>
       <c r="D26" t="n">
-        <v>16724</v>
+        <v>52346</v>
       </c>
       <c r="E26" t="n">
-        <v>3022</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="27">
@@ -870,13 +870,13 @@
         <v>2024</v>
       </c>
       <c r="C27" t="n">
-        <v>20847</v>
+        <v>54321</v>
       </c>
       <c r="D27" t="n">
-        <v>16749</v>
+        <v>52084</v>
       </c>
       <c r="E27" t="n">
-        <v>4098</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="28">
@@ -885,13 +885,13 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>21949</v>
+        <v>54931</v>
       </c>
       <c r="D28" t="n">
-        <v>16780</v>
+        <v>51638</v>
       </c>
       <c r="E28" t="n">
-        <v>5169</v>
+        <v>3294</v>
       </c>
     </row>
     <row r="29">
@@ -900,13 +900,13 @@
         <v>2026</v>
       </c>
       <c r="C29" t="n">
-        <v>23031</v>
+        <v>55547</v>
       </c>
       <c r="D29" t="n">
-        <v>16801</v>
+        <v>51095</v>
       </c>
       <c r="E29" t="n">
-        <v>6230</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="30">
@@ -915,13 +915,13 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>24103</v>
+        <v>56193</v>
       </c>
       <c r="D30" t="n">
-        <v>16800</v>
+        <v>50601</v>
       </c>
       <c r="E30" t="n">
-        <v>7303</v>
+        <v>5593</v>
       </c>
     </row>
     <row r="31">
@@ -930,13 +930,13 @@
         <v>2028</v>
       </c>
       <c r="C31" t="n">
-        <v>25145</v>
+        <v>56819</v>
       </c>
       <c r="D31" t="n">
-        <v>16746</v>
+        <v>50166</v>
       </c>
       <c r="E31" t="n">
-        <v>8400</v>
+        <v>6653</v>
       </c>
     </row>
     <row r="32">
@@ -945,13 +945,13 @@
         <v>2029</v>
       </c>
       <c r="C32" t="n">
-        <v>26173</v>
+        <v>57406</v>
       </c>
       <c r="D32" t="n">
-        <v>16669</v>
+        <v>49727</v>
       </c>
       <c r="E32" t="n">
-        <v>9503</v>
+        <v>7679</v>
       </c>
     </row>
     <row r="33">
@@ -960,13 +960,13 @@
         <v>2030</v>
       </c>
       <c r="C33" t="n">
-        <v>27167</v>
+        <v>57928</v>
       </c>
       <c r="D33" t="n">
-        <v>16591</v>
+        <v>49404</v>
       </c>
       <c r="E33" t="n">
-        <v>10576</v>
+        <v>8524</v>
       </c>
     </row>
     <row r="34">
@@ -975,13 +975,13 @@
         <v>2031</v>
       </c>
       <c r="C34" t="n">
-        <v>28127</v>
+        <v>58391</v>
       </c>
       <c r="D34" t="n">
-        <v>16535</v>
+        <v>49125</v>
       </c>
       <c r="E34" t="n">
-        <v>11592</v>
+        <v>9266</v>
       </c>
     </row>
     <row r="35">
@@ -990,13 +990,13 @@
         <v>2032</v>
       </c>
       <c r="C35" t="n">
-        <v>29061</v>
+        <v>58778</v>
       </c>
       <c r="D35" t="n">
-        <v>16495</v>
+        <v>48904</v>
       </c>
       <c r="E35" t="n">
-        <v>12567</v>
+        <v>9874</v>
       </c>
     </row>
     <row r="36">
@@ -1005,13 +1005,13 @@
         <v>2033</v>
       </c>
       <c r="C36" t="n">
-        <v>29976</v>
+        <v>59083</v>
       </c>
       <c r="D36" t="n">
-        <v>16480</v>
+        <v>48741</v>
       </c>
       <c r="E36" t="n">
-        <v>13496</v>
+        <v>10342</v>
       </c>
     </row>
     <row r="37">
@@ -1020,13 +1020,13 @@
         <v>2034</v>
       </c>
       <c r="C37" t="n">
-        <v>30886</v>
+        <v>59331</v>
       </c>
       <c r="D37" t="n">
-        <v>16440</v>
+        <v>48739</v>
       </c>
       <c r="E37" t="n">
-        <v>14447</v>
+        <v>10592</v>
       </c>
     </row>
     <row r="38">
@@ -1035,13 +1035,13 @@
         <v>2035</v>
       </c>
       <c r="C38" t="n">
-        <v>31782</v>
+        <v>59522</v>
       </c>
       <c r="D38" t="n">
-        <v>16386</v>
+        <v>48844</v>
       </c>
       <c r="E38" t="n">
-        <v>15396</v>
+        <v>10678</v>
       </c>
     </row>
     <row r="39">
@@ -1050,13 +1050,13 @@
         <v>2036</v>
       </c>
       <c r="C39" t="n">
-        <v>32658</v>
+        <v>59689</v>
       </c>
       <c r="D39" t="n">
-        <v>16345</v>
+        <v>49013</v>
       </c>
       <c r="E39" t="n">
-        <v>16313</v>
+        <v>10676</v>
       </c>
     </row>
     <row r="40">
@@ -1065,13 +1065,13 @@
         <v>2037</v>
       </c>
       <c r="C40" t="n">
-        <v>33531</v>
+        <v>59849</v>
       </c>
       <c r="D40" t="n">
-        <v>16350</v>
+        <v>49230</v>
       </c>
       <c r="E40" t="n">
-        <v>17181</v>
+        <v>10618</v>
       </c>
     </row>
     <row r="41">
@@ -1080,13 +1080,13 @@
         <v>2038</v>
       </c>
       <c r="C41" t="n">
-        <v>34404</v>
+        <v>60004</v>
       </c>
       <c r="D41" t="n">
-        <v>16381</v>
+        <v>49495</v>
       </c>
       <c r="E41" t="n">
-        <v>18024</v>
+        <v>10509</v>
       </c>
     </row>
     <row r="42">
@@ -1095,13 +1095,13 @@
         <v>2039</v>
       </c>
       <c r="C42" t="n">
-        <v>35275</v>
+        <v>60182</v>
       </c>
       <c r="D42" t="n">
-        <v>16417</v>
+        <v>49814</v>
       </c>
       <c r="E42" t="n">
-        <v>18858</v>
+        <v>10369</v>
       </c>
     </row>
     <row r="43">
@@ -1110,29 +1110,29 @@
         <v>2040</v>
       </c>
       <c r="C43" t="n">
-        <v>36130</v>
+        <v>60374</v>
       </c>
       <c r="D43" t="n">
-        <v>16463</v>
+        <v>50150</v>
       </c>
       <c r="E43" t="n">
-        <v>19667</v>
+        <v>10224</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Grunnskolelærere</t>
+          <t>Faglærere</t>
         </is>
       </c>
       <c r="B44" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C44" t="n">
-        <v>52497</v>
+        <v>16600</v>
       </c>
       <c r="D44" t="n">
-        <v>52497</v>
+        <v>16600</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
@@ -1144,13 +1144,13 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>52773</v>
+        <v>17578</v>
       </c>
       <c r="D45" t="n">
-        <v>52459</v>
+        <v>16622</v>
       </c>
       <c r="E45" t="n">
-        <v>314</v>
+        <v>956</v>
       </c>
     </row>
     <row r="46">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>53233</v>
+        <v>18647</v>
       </c>
       <c r="D46" t="n">
-        <v>52487</v>
+        <v>16681</v>
       </c>
       <c r="E46" t="n">
-        <v>746</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>53749</v>
+        <v>19746</v>
       </c>
       <c r="D47" t="n">
-        <v>52346</v>
+        <v>16724</v>
       </c>
       <c r="E47" t="n">
-        <v>1403</v>
+        <v>3022</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>54321</v>
+        <v>20847</v>
       </c>
       <c r="D48" t="n">
-        <v>52084</v>
+        <v>16749</v>
       </c>
       <c r="E48" t="n">
-        <v>2237</v>
+        <v>4098</v>
       </c>
     </row>
     <row r="49">
@@ -1204,13 +1204,13 @@
         <v>2025</v>
       </c>
       <c r="C49" t="n">
-        <v>54931</v>
+        <v>21949</v>
       </c>
       <c r="D49" t="n">
-        <v>51638</v>
+        <v>16780</v>
       </c>
       <c r="E49" t="n">
-        <v>3294</v>
+        <v>5169</v>
       </c>
     </row>
     <row r="50">
@@ -1219,13 +1219,13 @@
         <v>2026</v>
       </c>
       <c r="C50" t="n">
-        <v>55547</v>
+        <v>23031</v>
       </c>
       <c r="D50" t="n">
-        <v>51095</v>
+        <v>16801</v>
       </c>
       <c r="E50" t="n">
-        <v>4453</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>56193</v>
+        <v>24103</v>
       </c>
       <c r="D51" t="n">
-        <v>50601</v>
+        <v>16800</v>
       </c>
       <c r="E51" t="n">
-        <v>5593</v>
+        <v>7303</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>56819</v>
+        <v>25145</v>
       </c>
       <c r="D52" t="n">
-        <v>50166</v>
+        <v>16746</v>
       </c>
       <c r="E52" t="n">
-        <v>6653</v>
+        <v>8400</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>57406</v>
+        <v>26173</v>
       </c>
       <c r="D53" t="n">
-        <v>49727</v>
+        <v>16669</v>
       </c>
       <c r="E53" t="n">
-        <v>7679</v>
+        <v>9503</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1279,13 @@
         <v>2030</v>
       </c>
       <c r="C54" t="n">
-        <v>57928</v>
+        <v>27167</v>
       </c>
       <c r="D54" t="n">
-        <v>49404</v>
+        <v>16591</v>
       </c>
       <c r="E54" t="n">
-        <v>8524</v>
+        <v>10576</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>58391</v>
+        <v>28127</v>
       </c>
       <c r="D55" t="n">
-        <v>49125</v>
+        <v>16535</v>
       </c>
       <c r="E55" t="n">
-        <v>9266</v>
+        <v>11592</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>58778</v>
+        <v>29061</v>
       </c>
       <c r="D56" t="n">
-        <v>48904</v>
+        <v>16495</v>
       </c>
       <c r="E56" t="n">
-        <v>9874</v>
+        <v>12567</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>59083</v>
+        <v>29976</v>
       </c>
       <c r="D57" t="n">
-        <v>48741</v>
+        <v>16480</v>
       </c>
       <c r="E57" t="n">
-        <v>10342</v>
+        <v>13496</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>59331</v>
+        <v>30886</v>
       </c>
       <c r="D58" t="n">
-        <v>48739</v>
+        <v>16440</v>
       </c>
       <c r="E58" t="n">
-        <v>10592</v>
+        <v>14447</v>
       </c>
     </row>
     <row r="59">
@@ -1354,13 +1354,13 @@
         <v>2035</v>
       </c>
       <c r="C59" t="n">
-        <v>59522</v>
+        <v>31782</v>
       </c>
       <c r="D59" t="n">
-        <v>48844</v>
+        <v>16386</v>
       </c>
       <c r="E59" t="n">
-        <v>10678</v>
+        <v>15396</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>59689</v>
+        <v>32658</v>
       </c>
       <c r="D60" t="n">
-        <v>49013</v>
+        <v>16345</v>
       </c>
       <c r="E60" t="n">
-        <v>10676</v>
+        <v>16313</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>59849</v>
+        <v>33531</v>
       </c>
       <c r="D61" t="n">
-        <v>49230</v>
+        <v>16350</v>
       </c>
       <c r="E61" t="n">
-        <v>10618</v>
+        <v>17181</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>60004</v>
+        <v>34404</v>
       </c>
       <c r="D62" t="n">
-        <v>49495</v>
+        <v>16381</v>
       </c>
       <c r="E62" t="n">
-        <v>10509</v>
+        <v>18024</v>
       </c>
     </row>
     <row r="63">
@@ -1414,13 +1414,13 @@
         <v>2039</v>
       </c>
       <c r="C63" t="n">
-        <v>60182</v>
+        <v>35275</v>
       </c>
       <c r="D63" t="n">
-        <v>49814</v>
+        <v>16417</v>
       </c>
       <c r="E63" t="n">
-        <v>10369</v>
+        <v>18858</v>
       </c>
     </row>
     <row r="64">
@@ -1429,13 +1429,13 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>60374</v>
+        <v>36130</v>
       </c>
       <c r="D64" t="n">
-        <v>50150</v>
+        <v>16463</v>
       </c>
       <c r="E64" t="n">
-        <v>10224</v>
+        <v>19667</v>
       </c>
     </row>
     <row r="65">

</xml_diff>

<commit_message>
Ferdigstilt oppsplitting av faglærere.
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1122,17 +1122,17 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Faglærere</t>
+          <t>Lektorutdannede</t>
         </is>
       </c>
       <c r="B44" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C44" t="n">
-        <v>16600</v>
+        <v>5531</v>
       </c>
       <c r="D44" t="n">
-        <v>16600</v>
+        <v>5531</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
@@ -1144,13 +1144,13 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>17578</v>
+        <v>5860</v>
       </c>
       <c r="D45" t="n">
-        <v>16622</v>
+        <v>5538</v>
       </c>
       <c r="E45" t="n">
-        <v>956</v>
+        <v>322</v>
       </c>
     </row>
     <row r="46">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>18647</v>
+        <v>6218</v>
       </c>
       <c r="D46" t="n">
-        <v>16681</v>
+        <v>5558</v>
       </c>
       <c r="E46" t="n">
-        <v>1966</v>
+        <v>660</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>19746</v>
+        <v>6585</v>
       </c>
       <c r="D47" t="n">
-        <v>16723</v>
+        <v>5572</v>
       </c>
       <c r="E47" t="n">
-        <v>3023</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>20847</v>
+        <v>6955</v>
       </c>
       <c r="D48" t="n">
-        <v>16748</v>
+        <v>5580</v>
       </c>
       <c r="E48" t="n">
-        <v>4099</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="49">
@@ -1204,13 +1204,13 @@
         <v>2025</v>
       </c>
       <c r="C49" t="n">
-        <v>21949</v>
+        <v>7324</v>
       </c>
       <c r="D49" t="n">
-        <v>16779</v>
+        <v>5590</v>
       </c>
       <c r="E49" t="n">
-        <v>5170</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="50">
@@ -1219,13 +1219,13 @@
         <v>2026</v>
       </c>
       <c r="C50" t="n">
-        <v>23031</v>
+        <v>7687</v>
       </c>
       <c r="D50" t="n">
-        <v>16799</v>
+        <v>5597</v>
       </c>
       <c r="E50" t="n">
-        <v>6232</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>24103</v>
+        <v>8047</v>
       </c>
       <c r="D51" t="n">
-        <v>16799</v>
+        <v>5597</v>
       </c>
       <c r="E51" t="n">
-        <v>7304</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>25145</v>
+        <v>8396</v>
       </c>
       <c r="D52" t="n">
-        <v>16744</v>
+        <v>5579</v>
       </c>
       <c r="E52" t="n">
-        <v>8401</v>
+        <v>2817</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>26173</v>
+        <v>8740</v>
       </c>
       <c r="D53" t="n">
-        <v>16669</v>
+        <v>5554</v>
       </c>
       <c r="E53" t="n">
-        <v>9504</v>
+        <v>3186</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1279,13 @@
         <v>2030</v>
       </c>
       <c r="C54" t="n">
-        <v>27167</v>
+        <v>9072</v>
       </c>
       <c r="D54" t="n">
-        <v>16591</v>
+        <v>5528</v>
       </c>
       <c r="E54" t="n">
-        <v>10576</v>
+        <v>3544</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>28127</v>
+        <v>9395</v>
       </c>
       <c r="D55" t="n">
-        <v>16535</v>
+        <v>5509</v>
       </c>
       <c r="E55" t="n">
-        <v>11592</v>
+        <v>3886</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>29061</v>
+        <v>9709</v>
       </c>
       <c r="D56" t="n">
-        <v>16495</v>
+        <v>5496</v>
       </c>
       <c r="E56" t="n">
-        <v>12566</v>
+        <v>4213</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>29976</v>
+        <v>10015</v>
       </c>
       <c r="D57" t="n">
-        <v>16481</v>
+        <v>5491</v>
       </c>
       <c r="E57" t="n">
-        <v>13495</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>30886</v>
+        <v>10319</v>
       </c>
       <c r="D58" t="n">
-        <v>16441</v>
+        <v>5478</v>
       </c>
       <c r="E58" t="n">
-        <v>14446</v>
+        <v>4842</v>
       </c>
     </row>
     <row r="59">
@@ -1354,13 +1354,13 @@
         <v>2035</v>
       </c>
       <c r="C59" t="n">
-        <v>31782</v>
+        <v>10620</v>
       </c>
       <c r="D59" t="n">
-        <v>16388</v>
+        <v>5460</v>
       </c>
       <c r="E59" t="n">
-        <v>15394</v>
+        <v>5160</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>32658</v>
+        <v>10914</v>
       </c>
       <c r="D60" t="n">
-        <v>16348</v>
+        <v>5447</v>
       </c>
       <c r="E60" t="n">
-        <v>16310</v>
+        <v>5467</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>33531</v>
+        <v>11206</v>
       </c>
       <c r="D61" t="n">
-        <v>16353</v>
+        <v>5448</v>
       </c>
       <c r="E61" t="n">
-        <v>17178</v>
+        <v>5758</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>34404</v>
+        <v>11498</v>
       </c>
       <c r="D62" t="n">
-        <v>16384</v>
+        <v>5459</v>
       </c>
       <c r="E62" t="n">
-        <v>18021</v>
+        <v>6039</v>
       </c>
     </row>
     <row r="63">
@@ -1414,13 +1414,13 @@
         <v>2039</v>
       </c>
       <c r="C63" t="n">
-        <v>35275</v>
+        <v>11790</v>
       </c>
       <c r="D63" t="n">
-        <v>16420</v>
+        <v>5471</v>
       </c>
       <c r="E63" t="n">
-        <v>18855</v>
+        <v>6319</v>
       </c>
     </row>
     <row r="64">
@@ -1429,29 +1429,29 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>36130</v>
+        <v>12076</v>
       </c>
       <c r="D64" t="n">
-        <v>16466</v>
+        <v>5486</v>
       </c>
       <c r="E64" t="n">
-        <v>19664</v>
+        <v>6590</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>PPU</t>
+          <t>Faglærere</t>
         </is>
       </c>
       <c r="B65" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C65" t="n">
-        <v>30789</v>
+        <v>5534</v>
       </c>
       <c r="D65" t="n">
-        <v>30789</v>
+        <v>5534</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -1463,13 +1463,13 @@
         <v>2021</v>
       </c>
       <c r="C66" t="n">
-        <v>30793</v>
+        <v>5860</v>
       </c>
       <c r="D66" t="n">
-        <v>30824</v>
+        <v>5541</v>
       </c>
       <c r="E66" t="n">
-        <v>-31</v>
+        <v>319</v>
       </c>
     </row>
     <row r="67">
@@ -1478,13 +1478,13 @@
         <v>2022</v>
       </c>
       <c r="C67" t="n">
-        <v>30890</v>
+        <v>6218</v>
       </c>
       <c r="D67" t="n">
-        <v>30930</v>
+        <v>5561</v>
       </c>
       <c r="E67" t="n">
-        <v>-40</v>
+        <v>657</v>
       </c>
     </row>
     <row r="68">
@@ -1493,13 +1493,13 @@
         <v>2023</v>
       </c>
       <c r="C68" t="n">
-        <v>31004</v>
+        <v>6585</v>
       </c>
       <c r="D68" t="n">
-        <v>31003</v>
+        <v>5575</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="69">
@@ -1508,13 +1508,13 @@
         <v>2024</v>
       </c>
       <c r="C69" t="n">
-        <v>31130</v>
+        <v>6955</v>
       </c>
       <c r="D69" t="n">
-        <v>31043</v>
+        <v>5583</v>
       </c>
       <c r="E69" t="n">
-        <v>87</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="70">
@@ -1523,13 +1523,13 @@
         <v>2025</v>
       </c>
       <c r="C70" t="n">
-        <v>31256</v>
+        <v>7324</v>
       </c>
       <c r="D70" t="n">
-        <v>31097</v>
+        <v>5593</v>
       </c>
       <c r="E70" t="n">
-        <v>159</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="71">
@@ -1538,13 +1538,13 @@
         <v>2026</v>
       </c>
       <c r="C71" t="n">
-        <v>31384</v>
+        <v>7687</v>
       </c>
       <c r="D71" t="n">
-        <v>31132</v>
+        <v>5600</v>
       </c>
       <c r="E71" t="n">
-        <v>252</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="72">
@@ -1553,13 +1553,13 @@
         <v>2027</v>
       </c>
       <c r="C72" t="n">
-        <v>31496</v>
+        <v>8047</v>
       </c>
       <c r="D72" t="n">
-        <v>31124</v>
+        <v>5600</v>
       </c>
       <c r="E72" t="n">
-        <v>373</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="73">
@@ -1568,13 +1568,13 @@
         <v>2028</v>
       </c>
       <c r="C73" t="n">
-        <v>31594</v>
+        <v>8396</v>
       </c>
       <c r="D73" t="n">
-        <v>31006</v>
+        <v>5582</v>
       </c>
       <c r="E73" t="n">
-        <v>588</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="74">
@@ -1583,13 +1583,13 @@
         <v>2029</v>
       </c>
       <c r="C74" t="n">
-        <v>31672</v>
+        <v>8740</v>
       </c>
       <c r="D74" t="n">
-        <v>30845</v>
+        <v>5557</v>
       </c>
       <c r="E74" t="n">
-        <v>827</v>
+        <v>3183</v>
       </c>
     </row>
     <row r="75">
@@ -1598,13 +1598,13 @@
         <v>2030</v>
       </c>
       <c r="C75" t="n">
-        <v>31717</v>
+        <v>9072</v>
       </c>
       <c r="D75" t="n">
-        <v>30679</v>
+        <v>5531</v>
       </c>
       <c r="E75" t="n">
-        <v>1038</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="76">
@@ -1613,13 +1613,13 @@
         <v>2031</v>
       </c>
       <c r="C76" t="n">
-        <v>31726</v>
+        <v>9395</v>
       </c>
       <c r="D76" t="n">
-        <v>30555</v>
+        <v>5512</v>
       </c>
       <c r="E76" t="n">
-        <v>1170</v>
+        <v>3883</v>
       </c>
     </row>
     <row r="77">
@@ -1628,13 +1628,13 @@
         <v>2032</v>
       </c>
       <c r="C77" t="n">
-        <v>31699</v>
+        <v>9709</v>
       </c>
       <c r="D77" t="n">
-        <v>30462</v>
+        <v>5499</v>
       </c>
       <c r="E77" t="n">
-        <v>1238</v>
+        <v>4210</v>
       </c>
     </row>
     <row r="78">
@@ -1643,13 +1643,13 @@
         <v>2033</v>
       </c>
       <c r="C78" t="n">
-        <v>31633</v>
+        <v>10015</v>
       </c>
       <c r="D78" t="n">
-        <v>30416</v>
+        <v>5494</v>
       </c>
       <c r="E78" t="n">
-        <v>1217</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="79">
@@ -1658,13 +1658,13 @@
         <v>2034</v>
       </c>
       <c r="C79" t="n">
-        <v>31553</v>
+        <v>10319</v>
       </c>
       <c r="D79" t="n">
-        <v>30314</v>
+        <v>5481</v>
       </c>
       <c r="E79" t="n">
-        <v>1238</v>
+        <v>4839</v>
       </c>
     </row>
     <row r="80">
@@ -1673,13 +1673,13 @@
         <v>2035</v>
       </c>
       <c r="C80" t="n">
-        <v>31437</v>
+        <v>10620</v>
       </c>
       <c r="D80" t="n">
-        <v>30184</v>
+        <v>5463</v>
       </c>
       <c r="E80" t="n">
-        <v>1254</v>
+        <v>5157</v>
       </c>
     </row>
     <row r="81">
@@ -1688,13 +1688,13 @@
         <v>2036</v>
       </c>
       <c r="C81" t="n">
-        <v>31322</v>
+        <v>10914</v>
       </c>
       <c r="D81" t="n">
-        <v>30078</v>
+        <v>5450</v>
       </c>
       <c r="E81" t="n">
-        <v>1244</v>
+        <v>5464</v>
       </c>
     </row>
     <row r="82">
@@ -1703,13 +1703,13 @@
         <v>2037</v>
       </c>
       <c r="C82" t="n">
-        <v>31190</v>
+        <v>11206</v>
       </c>
       <c r="D82" t="n">
-        <v>30063</v>
+        <v>5451</v>
       </c>
       <c r="E82" t="n">
-        <v>1127</v>
+        <v>5755</v>
       </c>
     </row>
     <row r="83">
@@ -1718,13 +1718,13 @@
         <v>2038</v>
       </c>
       <c r="C83" t="n">
-        <v>31069</v>
+        <v>11498</v>
       </c>
       <c r="D83" t="n">
-        <v>30099</v>
+        <v>5461</v>
       </c>
       <c r="E83" t="n">
-        <v>970</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="84">
@@ -1733,13 +1733,13 @@
         <v>2039</v>
       </c>
       <c r="C84" t="n">
-        <v>30946</v>
+        <v>11790</v>
       </c>
       <c r="D84" t="n">
-        <v>30146</v>
+        <v>5474</v>
       </c>
       <c r="E84" t="n">
-        <v>800</v>
+        <v>6316</v>
       </c>
     </row>
     <row r="85">
@@ -1748,29 +1748,29 @@
         <v>2040</v>
       </c>
       <c r="C85" t="n">
-        <v>30834</v>
+        <v>12076</v>
       </c>
       <c r="D85" t="n">
-        <v>30213</v>
+        <v>5489</v>
       </c>
       <c r="E85" t="n">
-        <v>621</v>
+        <v>6587</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>PPU Yrkesfag</t>
+          <t>Yrkesfaglærere</t>
         </is>
       </c>
       <c r="B86" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C86" t="n">
-        <v>13299</v>
+        <v>5535</v>
       </c>
       <c r="D86" t="n">
-        <v>13299</v>
+        <v>5535</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>13226</v>
+        <v>5860</v>
       </c>
       <c r="D87" t="n">
-        <v>13325</v>
+        <v>5542</v>
       </c>
       <c r="E87" t="n">
-        <v>-100</v>
+        <v>318</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>13190</v>
+        <v>6218</v>
       </c>
       <c r="D88" t="n">
-        <v>13386</v>
+        <v>5562</v>
       </c>
       <c r="E88" t="n">
-        <v>-196</v>
+        <v>656</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>13140</v>
+        <v>6585</v>
       </c>
       <c r="D89" t="n">
-        <v>13443</v>
+        <v>5576</v>
       </c>
       <c r="E89" t="n">
-        <v>-304</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>13091</v>
+        <v>6955</v>
       </c>
       <c r="D90" t="n">
-        <v>13490</v>
+        <v>5584</v>
       </c>
       <c r="E90" t="n">
-        <v>-399</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>13024</v>
+        <v>7324</v>
       </c>
       <c r="D91" t="n">
-        <v>13559</v>
+        <v>5594</v>
       </c>
       <c r="E91" t="n">
-        <v>-535</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>12945</v>
+        <v>7687</v>
       </c>
       <c r="D92" t="n">
-        <v>13624</v>
+        <v>5601</v>
       </c>
       <c r="E92" t="n">
-        <v>-679</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>12866</v>
+        <v>8047</v>
       </c>
       <c r="D93" t="n">
-        <v>13657</v>
+        <v>5601</v>
       </c>
       <c r="E93" t="n">
-        <v>-792</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>12763</v>
+        <v>8396</v>
       </c>
       <c r="D94" t="n">
-        <v>13620</v>
+        <v>5583</v>
       </c>
       <c r="E94" t="n">
-        <v>-857</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>12664</v>
+        <v>8740</v>
       </c>
       <c r="D95" t="n">
-        <v>13556</v>
+        <v>5557</v>
       </c>
       <c r="E95" t="n">
-        <v>-893</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>12555</v>
+        <v>9072</v>
       </c>
       <c r="D96" t="n">
-        <v>13480</v>
+        <v>5532</v>
       </c>
       <c r="E96" t="n">
-        <v>-924</v>
+        <v>3540</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>12434</v>
+        <v>9395</v>
       </c>
       <c r="D97" t="n">
-        <v>13426</v>
+        <v>5513</v>
       </c>
       <c r="E97" t="n">
-        <v>-992</v>
+        <v>3882</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>12321</v>
+        <v>9709</v>
       </c>
       <c r="D98" t="n">
-        <v>13387</v>
+        <v>5500</v>
       </c>
       <c r="E98" t="n">
-        <v>-1066</v>
+        <v>4209</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>12191</v>
+        <v>10015</v>
       </c>
       <c r="D99" t="n">
-        <v>13373</v>
+        <v>5495</v>
       </c>
       <c r="E99" t="n">
-        <v>-1182</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>12080</v>
+        <v>10319</v>
       </c>
       <c r="D100" t="n">
-        <v>13314</v>
+        <v>5482</v>
       </c>
       <c r="E100" t="n">
-        <v>-1234</v>
+        <v>4838</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>11961</v>
+        <v>10620</v>
       </c>
       <c r="D101" t="n">
-        <v>13229</v>
+        <v>5464</v>
       </c>
       <c r="E101" t="n">
-        <v>-1267</v>
+        <v>5156</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>11852</v>
+        <v>10914</v>
       </c>
       <c r="D102" t="n">
-        <v>13153</v>
+        <v>5451</v>
       </c>
       <c r="E102" t="n">
-        <v>-1301</v>
+        <v>5463</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>11748</v>
+        <v>11206</v>
       </c>
       <c r="D103" t="n">
-        <v>13129</v>
+        <v>5452</v>
       </c>
       <c r="E103" t="n">
-        <v>-1381</v>
+        <v>5754</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>11635</v>
+        <v>11498</v>
       </c>
       <c r="D104" t="n">
-        <v>13132</v>
+        <v>5462</v>
       </c>
       <c r="E104" t="n">
-        <v>-1498</v>
+        <v>6036</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>11542</v>
+        <v>11790</v>
       </c>
       <c r="D105" t="n">
-        <v>13138</v>
+        <v>5475</v>
       </c>
       <c r="E105" t="n">
-        <v>-1597</v>
+        <v>6315</v>
       </c>
     </row>
     <row r="106">
@@ -2067,21 +2067,661 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
+        <v>12076</v>
+      </c>
+      <c r="D106" t="n">
+        <v>5490</v>
+      </c>
+      <c r="E106" t="n">
+        <v>6586</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>PPU</t>
+        </is>
+      </c>
+      <c r="B107" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C107" t="n">
+        <v>30789</v>
+      </c>
+      <c r="D107" t="n">
+        <v>30789</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n"/>
+      <c r="B108" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C108" t="n">
+        <v>30793</v>
+      </c>
+      <c r="D108" t="n">
+        <v>30824</v>
+      </c>
+      <c r="E108" t="n">
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n"/>
+      <c r="B109" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C109" t="n">
+        <v>30890</v>
+      </c>
+      <c r="D109" t="n">
+        <v>30930</v>
+      </c>
+      <c r="E109" t="n">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n"/>
+      <c r="B110" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C110" t="n">
+        <v>31004</v>
+      </c>
+      <c r="D110" t="n">
+        <v>31003</v>
+      </c>
+      <c r="E110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n"/>
+      <c r="B111" s="1" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C111" t="n">
+        <v>31130</v>
+      </c>
+      <c r="D111" t="n">
+        <v>31043</v>
+      </c>
+      <c r="E111" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n"/>
+      <c r="B112" s="1" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C112" t="n">
+        <v>31256</v>
+      </c>
+      <c r="D112" t="n">
+        <v>31097</v>
+      </c>
+      <c r="E112" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n"/>
+      <c r="B113" s="1" t="n">
+        <v>2026</v>
+      </c>
+      <c r="C113" t="n">
+        <v>31384</v>
+      </c>
+      <c r="D113" t="n">
+        <v>31132</v>
+      </c>
+      <c r="E113" t="n">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n"/>
+      <c r="B114" s="1" t="n">
+        <v>2027</v>
+      </c>
+      <c r="C114" t="n">
+        <v>31496</v>
+      </c>
+      <c r="D114" t="n">
+        <v>31124</v>
+      </c>
+      <c r="E114" t="n">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n"/>
+      <c r="B115" s="1" t="n">
+        <v>2028</v>
+      </c>
+      <c r="C115" t="n">
+        <v>31594</v>
+      </c>
+      <c r="D115" t="n">
+        <v>31006</v>
+      </c>
+      <c r="E115" t="n">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n"/>
+      <c r="B116" s="1" t="n">
+        <v>2029</v>
+      </c>
+      <c r="C116" t="n">
+        <v>31672</v>
+      </c>
+      <c r="D116" t="n">
+        <v>30845</v>
+      </c>
+      <c r="E116" t="n">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n"/>
+      <c r="B117" s="1" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C117" t="n">
+        <v>31717</v>
+      </c>
+      <c r="D117" t="n">
+        <v>30679</v>
+      </c>
+      <c r="E117" t="n">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n"/>
+      <c r="B118" s="1" t="n">
+        <v>2031</v>
+      </c>
+      <c r="C118" t="n">
+        <v>31726</v>
+      </c>
+      <c r="D118" t="n">
+        <v>30555</v>
+      </c>
+      <c r="E118" t="n">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n"/>
+      <c r="B119" s="1" t="n">
+        <v>2032</v>
+      </c>
+      <c r="C119" t="n">
+        <v>31699</v>
+      </c>
+      <c r="D119" t="n">
+        <v>30462</v>
+      </c>
+      <c r="E119" t="n">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n"/>
+      <c r="B120" s="1" t="n">
+        <v>2033</v>
+      </c>
+      <c r="C120" t="n">
+        <v>31633</v>
+      </c>
+      <c r="D120" t="n">
+        <v>30416</v>
+      </c>
+      <c r="E120" t="n">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n"/>
+      <c r="B121" s="1" t="n">
+        <v>2034</v>
+      </c>
+      <c r="C121" t="n">
+        <v>31553</v>
+      </c>
+      <c r="D121" t="n">
+        <v>30314</v>
+      </c>
+      <c r="E121" t="n">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n"/>
+      <c r="B122" s="1" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C122" t="n">
+        <v>31437</v>
+      </c>
+      <c r="D122" t="n">
+        <v>30184</v>
+      </c>
+      <c r="E122" t="n">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n"/>
+      <c r="B123" s="1" t="n">
+        <v>2036</v>
+      </c>
+      <c r="C123" t="n">
+        <v>31322</v>
+      </c>
+      <c r="D123" t="n">
+        <v>30078</v>
+      </c>
+      <c r="E123" t="n">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n"/>
+      <c r="B124" s="1" t="n">
+        <v>2037</v>
+      </c>
+      <c r="C124" t="n">
+        <v>31190</v>
+      </c>
+      <c r="D124" t="n">
+        <v>30063</v>
+      </c>
+      <c r="E124" t="n">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n"/>
+      <c r="B125" s="1" t="n">
+        <v>2038</v>
+      </c>
+      <c r="C125" t="n">
+        <v>31069</v>
+      </c>
+      <c r="D125" t="n">
+        <v>30099</v>
+      </c>
+      <c r="E125" t="n">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n"/>
+      <c r="B126" s="1" t="n">
+        <v>2039</v>
+      </c>
+      <c r="C126" t="n">
+        <v>30946</v>
+      </c>
+      <c r="D126" t="n">
+        <v>30146</v>
+      </c>
+      <c r="E126" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n"/>
+      <c r="B127" s="1" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C127" t="n">
+        <v>30834</v>
+      </c>
+      <c r="D127" t="n">
+        <v>30213</v>
+      </c>
+      <c r="E127" t="n">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>PPU Yrkesfag</t>
+        </is>
+      </c>
+      <c r="B128" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C128" t="n">
+        <v>13299</v>
+      </c>
+      <c r="D128" t="n">
+        <v>13299</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n"/>
+      <c r="B129" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C129" t="n">
+        <v>13226</v>
+      </c>
+      <c r="D129" t="n">
+        <v>13325</v>
+      </c>
+      <c r="E129" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n"/>
+      <c r="B130" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C130" t="n">
+        <v>13190</v>
+      </c>
+      <c r="D130" t="n">
+        <v>13386</v>
+      </c>
+      <c r="E130" t="n">
+        <v>-196</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n"/>
+      <c r="B131" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C131" t="n">
+        <v>13140</v>
+      </c>
+      <c r="D131" t="n">
+        <v>13443</v>
+      </c>
+      <c r="E131" t="n">
+        <v>-304</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n"/>
+      <c r="B132" s="1" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C132" t="n">
+        <v>13091</v>
+      </c>
+      <c r="D132" t="n">
+        <v>13490</v>
+      </c>
+      <c r="E132" t="n">
+        <v>-399</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n"/>
+      <c r="B133" s="1" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C133" t="n">
+        <v>13024</v>
+      </c>
+      <c r="D133" t="n">
+        <v>13559</v>
+      </c>
+      <c r="E133" t="n">
+        <v>-535</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n"/>
+      <c r="B134" s="1" t="n">
+        <v>2026</v>
+      </c>
+      <c r="C134" t="n">
+        <v>12945</v>
+      </c>
+      <c r="D134" t="n">
+        <v>13624</v>
+      </c>
+      <c r="E134" t="n">
+        <v>-679</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n"/>
+      <c r="B135" s="1" t="n">
+        <v>2027</v>
+      </c>
+      <c r="C135" t="n">
+        <v>12866</v>
+      </c>
+      <c r="D135" t="n">
+        <v>13657</v>
+      </c>
+      <c r="E135" t="n">
+        <v>-792</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n"/>
+      <c r="B136" s="1" t="n">
+        <v>2028</v>
+      </c>
+      <c r="C136" t="n">
+        <v>12763</v>
+      </c>
+      <c r="D136" t="n">
+        <v>13620</v>
+      </c>
+      <c r="E136" t="n">
+        <v>-857</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n"/>
+      <c r="B137" s="1" t="n">
+        <v>2029</v>
+      </c>
+      <c r="C137" t="n">
+        <v>12664</v>
+      </c>
+      <c r="D137" t="n">
+        <v>13556</v>
+      </c>
+      <c r="E137" t="n">
+        <v>-893</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n"/>
+      <c r="B138" s="1" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C138" t="n">
+        <v>12555</v>
+      </c>
+      <c r="D138" t="n">
+        <v>13480</v>
+      </c>
+      <c r="E138" t="n">
+        <v>-924</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n"/>
+      <c r="B139" s="1" t="n">
+        <v>2031</v>
+      </c>
+      <c r="C139" t="n">
+        <v>12434</v>
+      </c>
+      <c r="D139" t="n">
+        <v>13426</v>
+      </c>
+      <c r="E139" t="n">
+        <v>-992</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n"/>
+      <c r="B140" s="1" t="n">
+        <v>2032</v>
+      </c>
+      <c r="C140" t="n">
+        <v>12321</v>
+      </c>
+      <c r="D140" t="n">
+        <v>13387</v>
+      </c>
+      <c r="E140" t="n">
+        <v>-1066</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n"/>
+      <c r="B141" s="1" t="n">
+        <v>2033</v>
+      </c>
+      <c r="C141" t="n">
+        <v>12191</v>
+      </c>
+      <c r="D141" t="n">
+        <v>13373</v>
+      </c>
+      <c r="E141" t="n">
+        <v>-1182</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n"/>
+      <c r="B142" s="1" t="n">
+        <v>2034</v>
+      </c>
+      <c r="C142" t="n">
+        <v>12080</v>
+      </c>
+      <c r="D142" t="n">
+        <v>13314</v>
+      </c>
+      <c r="E142" t="n">
+        <v>-1234</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n"/>
+      <c r="B143" s="1" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C143" t="n">
+        <v>11961</v>
+      </c>
+      <c r="D143" t="n">
+        <v>13229</v>
+      </c>
+      <c r="E143" t="n">
+        <v>-1267</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n"/>
+      <c r="B144" s="1" t="n">
+        <v>2036</v>
+      </c>
+      <c r="C144" t="n">
+        <v>11852</v>
+      </c>
+      <c r="D144" t="n">
+        <v>13153</v>
+      </c>
+      <c r="E144" t="n">
+        <v>-1301</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n"/>
+      <c r="B145" s="1" t="n">
+        <v>2037</v>
+      </c>
+      <c r="C145" t="n">
+        <v>11748</v>
+      </c>
+      <c r="D145" t="n">
+        <v>13129</v>
+      </c>
+      <c r="E145" t="n">
+        <v>-1381</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n"/>
+      <c r="B146" s="1" t="n">
+        <v>2038</v>
+      </c>
+      <c r="C146" t="n">
+        <v>11635</v>
+      </c>
+      <c r="D146" t="n">
+        <v>13132</v>
+      </c>
+      <c r="E146" t="n">
+        <v>-1498</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n"/>
+      <c r="B147" s="1" t="n">
+        <v>2039</v>
+      </c>
+      <c r="C147" t="n">
+        <v>11542</v>
+      </c>
+      <c r="D147" t="n">
+        <v>13138</v>
+      </c>
+      <c r="E147" t="n">
+        <v>-1597</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n"/>
+      <c r="B148" s="1" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C148" t="n">
         <v>11443</v>
       </c>
-      <c r="D106" t="n">
+      <c r="D148" t="n">
         <v>13155</v>
       </c>
-      <c r="E106" t="n">
+      <c r="E148" t="n">
         <v>-1712</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="A44:A64"/>
     <mergeCell ref="A65:A85"/>
+    <mergeCell ref="A107:A127"/>
     <mergeCell ref="A86:A106"/>
     <mergeCell ref="A23:A43"/>
+    <mergeCell ref="A128:A148"/>
     <mergeCell ref="A2:A22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Opprettet ny innfil for Kandidatproduksjon.
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -1144,13 +1144,13 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>5744</v>
+        <v>5963</v>
       </c>
       <c r="D45" t="n">
         <v>5541</v>
       </c>
       <c r="E45" t="n">
-        <v>203</v>
+        <v>421</v>
       </c>
     </row>
     <row r="46">
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>5980</v>
+        <v>6431</v>
       </c>
       <c r="D46" t="n">
         <v>5561</v>
       </c>
       <c r="E46" t="n">
-        <v>419</v>
+        <v>870</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>6221</v>
+        <v>6896</v>
       </c>
       <c r="D47" t="n">
         <v>5575</v>
       </c>
       <c r="E47" t="n">
-        <v>646</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>6460</v>
+        <v>7360</v>
       </c>
       <c r="D48" t="n">
         <v>5583</v>
       </c>
       <c r="E48" t="n">
-        <v>877</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="49">
@@ -1204,13 +1204,13 @@
         <v>2025</v>
       </c>
       <c r="C49" t="n">
-        <v>6699</v>
+        <v>7821</v>
       </c>
       <c r="D49" t="n">
         <v>5593</v>
       </c>
       <c r="E49" t="n">
-        <v>1106</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="50">
@@ -1219,13 +1219,13 @@
         <v>2026</v>
       </c>
       <c r="C50" t="n">
-        <v>6931</v>
+        <v>8272</v>
       </c>
       <c r="D50" t="n">
         <v>5600</v>
       </c>
       <c r="E50" t="n">
-        <v>1331</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>7160</v>
+        <v>8718</v>
       </c>
       <c r="D51" t="n">
         <v>5600</v>
       </c>
       <c r="E51" t="n">
-        <v>1560</v>
+        <v>3118</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>7380</v>
+        <v>9151</v>
       </c>
       <c r="D52" t="n">
         <v>5582</v>
       </c>
       <c r="E52" t="n">
-        <v>1798</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>7596</v>
+        <v>9578</v>
       </c>
       <c r="D53" t="n">
         <v>5557</v>
       </c>
       <c r="E53" t="n">
-        <v>2039</v>
+        <v>4021</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1279,13 @@
         <v>2030</v>
       </c>
       <c r="C54" t="n">
-        <v>7801</v>
+        <v>9990</v>
       </c>
       <c r="D54" t="n">
         <v>5531</v>
       </c>
       <c r="E54" t="n">
-        <v>2271</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>7999</v>
+        <v>10396</v>
       </c>
       <c r="D55" t="n">
         <v>5512</v>
       </c>
       <c r="E55" t="n">
-        <v>2487</v>
+        <v>4884</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>8189</v>
+        <v>10790</v>
       </c>
       <c r="D56" t="n">
         <v>5499</v>
       </c>
       <c r="E56" t="n">
-        <v>2690</v>
+        <v>5291</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>8372</v>
+        <v>11177</v>
       </c>
       <c r="D57" t="n">
         <v>5494</v>
       </c>
       <c r="E57" t="n">
-        <v>2878</v>
+        <v>5684</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>8554</v>
+        <v>11561</v>
       </c>
       <c r="D58" t="n">
         <v>5481</v>
       </c>
       <c r="E58" t="n">
-        <v>3074</v>
+        <v>6081</v>
       </c>
     </row>
     <row r="59">
@@ -1354,13 +1354,13 @@
         <v>2035</v>
       </c>
       <c r="C59" t="n">
-        <v>8734</v>
+        <v>11940</v>
       </c>
       <c r="D59" t="n">
         <v>5463</v>
       </c>
       <c r="E59" t="n">
-        <v>3271</v>
+        <v>6477</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>8908</v>
+        <v>12308</v>
       </c>
       <c r="D60" t="n">
         <v>5450</v>
       </c>
       <c r="E60" t="n">
-        <v>3459</v>
+        <v>6859</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>9083</v>
+        <v>12677</v>
       </c>
       <c r="D61" t="n">
         <v>5451</v>
       </c>
       <c r="E61" t="n">
-        <v>3631</v>
+        <v>7225</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>9258</v>
+        <v>13044</v>
       </c>
       <c r="D62" t="n">
         <v>5461</v>
       </c>
       <c r="E62" t="n">
-        <v>3797</v>
+        <v>7583</v>
       </c>
     </row>
     <row r="63">
@@ -1414,13 +1414,13 @@
         <v>2039</v>
       </c>
       <c r="C63" t="n">
-        <v>9434</v>
+        <v>13409</v>
       </c>
       <c r="D63" t="n">
         <v>5474</v>
       </c>
       <c r="E63" t="n">
-        <v>3961</v>
+        <v>7936</v>
       </c>
     </row>
     <row r="64">
@@ -1429,13 +1429,13 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>9607</v>
+        <v>13769</v>
       </c>
       <c r="D64" t="n">
         <v>5489</v>
       </c>
       <c r="E64" t="n">
-        <v>4118</v>
+        <v>8280</v>
       </c>
     </row>
     <row r="65">
@@ -1463,13 +1463,13 @@
         <v>2021</v>
       </c>
       <c r="C66" t="n">
-        <v>5976</v>
+        <v>5812</v>
       </c>
       <c r="D66" t="n">
         <v>5541</v>
       </c>
       <c r="E66" t="n">
-        <v>435</v>
+        <v>271</v>
       </c>
     </row>
     <row r="67">
@@ -1478,13 +1478,13 @@
         <v>2022</v>
       </c>
       <c r="C67" t="n">
-        <v>6455</v>
+        <v>6122</v>
       </c>
       <c r="D67" t="n">
         <v>5561</v>
       </c>
       <c r="E67" t="n">
-        <v>894</v>
+        <v>561</v>
       </c>
     </row>
     <row r="68">
@@ -1493,13 +1493,13 @@
         <v>2023</v>
       </c>
       <c r="C68" t="n">
-        <v>6950</v>
+        <v>6427</v>
       </c>
       <c r="D68" t="n">
         <v>5575</v>
       </c>
       <c r="E68" t="n">
-        <v>1375</v>
+        <v>852</v>
       </c>
     </row>
     <row r="69">
@@ -1508,13 +1508,13 @@
         <v>2024</v>
       </c>
       <c r="C69" t="n">
-        <v>7449</v>
+        <v>6728</v>
       </c>
       <c r="D69" t="n">
         <v>5583</v>
       </c>
       <c r="E69" t="n">
-        <v>1866</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="70">
@@ -1523,13 +1523,13 @@
         <v>2025</v>
       </c>
       <c r="C70" t="n">
-        <v>7949</v>
+        <v>7026</v>
       </c>
       <c r="D70" t="n">
         <v>5593</v>
       </c>
       <c r="E70" t="n">
-        <v>2356</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="71">
@@ -1538,13 +1538,13 @@
         <v>2026</v>
       </c>
       <c r="C71" t="n">
-        <v>8443</v>
+        <v>7315</v>
       </c>
       <c r="D71" t="n">
         <v>5600</v>
       </c>
       <c r="E71" t="n">
-        <v>2843</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="72">
@@ -1553,13 +1553,13 @@
         <v>2027</v>
       </c>
       <c r="C72" t="n">
-        <v>8933</v>
+        <v>7600</v>
       </c>
       <c r="D72" t="n">
         <v>5600</v>
       </c>
       <c r="E72" t="n">
-        <v>3333</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="73">
@@ -1568,13 +1568,13 @@
         <v>2028</v>
       </c>
       <c r="C73" t="n">
-        <v>9411</v>
+        <v>7874</v>
       </c>
       <c r="D73" t="n">
         <v>5582</v>
       </c>
       <c r="E73" t="n">
-        <v>3829</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="74">
@@ -1583,13 +1583,13 @@
         <v>2029</v>
       </c>
       <c r="C74" t="n">
-        <v>9883</v>
+        <v>8144</v>
       </c>
       <c r="D74" t="n">
         <v>5557</v>
       </c>
       <c r="E74" t="n">
-        <v>4327</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="75">
@@ -1598,13 +1598,13 @@
         <v>2030</v>
       </c>
       <c r="C75" t="n">
-        <v>10343</v>
+        <v>8401</v>
       </c>
       <c r="D75" t="n">
         <v>5531</v>
       </c>
       <c r="E75" t="n">
-        <v>4812</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="76">
@@ -1613,13 +1613,13 @@
         <v>2031</v>
       </c>
       <c r="C76" t="n">
-        <v>10791</v>
+        <v>8652</v>
       </c>
       <c r="D76" t="n">
         <v>5512</v>
       </c>
       <c r="E76" t="n">
-        <v>5278</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="77">
@@ -1628,13 +1628,13 @@
         <v>2032</v>
       </c>
       <c r="C77" t="n">
-        <v>11229</v>
+        <v>8894</v>
       </c>
       <c r="D77" t="n">
         <v>5499</v>
       </c>
       <c r="E77" t="n">
-        <v>5730</v>
+        <v>3395</v>
       </c>
     </row>
     <row r="78">
@@ -1643,13 +1643,13 @@
         <v>2033</v>
       </c>
       <c r="C78" t="n">
-        <v>11658</v>
+        <v>9130</v>
       </c>
       <c r="D78" t="n">
         <v>5494</v>
       </c>
       <c r="E78" t="n">
-        <v>6164</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="79">
@@ -1658,13 +1658,13 @@
         <v>2034</v>
       </c>
       <c r="C79" t="n">
-        <v>12084</v>
+        <v>9363</v>
       </c>
       <c r="D79" t="n">
         <v>5481</v>
       </c>
       <c r="E79" t="n">
-        <v>6604</v>
+        <v>3883</v>
       </c>
     </row>
     <row r="80">
@@ -1673,13 +1673,13 @@
         <v>2035</v>
       </c>
       <c r="C80" t="n">
-        <v>12506</v>
+        <v>9594</v>
       </c>
       <c r="D80" t="n">
         <v>5463</v>
       </c>
       <c r="E80" t="n">
-        <v>7043</v>
+        <v>4131</v>
       </c>
     </row>
     <row r="81">
@@ -1688,13 +1688,13 @@
         <v>2036</v>
       </c>
       <c r="C81" t="n">
-        <v>12919</v>
+        <v>9816</v>
       </c>
       <c r="D81" t="n">
         <v>5450</v>
       </c>
       <c r="E81" t="n">
-        <v>7470</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="82">
@@ -1703,13 +1703,13 @@
         <v>2037</v>
       </c>
       <c r="C82" t="n">
-        <v>13329</v>
+        <v>10039</v>
       </c>
       <c r="D82" t="n">
         <v>5451</v>
       </c>
       <c r="E82" t="n">
-        <v>7878</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="83">
@@ -1718,13 +1718,13 @@
         <v>2038</v>
       </c>
       <c r="C83" t="n">
-        <v>13738</v>
+        <v>10264</v>
       </c>
       <c r="D83" t="n">
         <v>5461</v>
       </c>
       <c r="E83" t="n">
-        <v>8276</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="84">
@@ -1733,13 +1733,13 @@
         <v>2039</v>
       </c>
       <c r="C84" t="n">
-        <v>14145</v>
+        <v>10487</v>
       </c>
       <c r="D84" t="n">
         <v>5474</v>
       </c>
       <c r="E84" t="n">
-        <v>8671</v>
+        <v>5014</v>
       </c>
     </row>
     <row r="85">
@@ -1748,13 +1748,13 @@
         <v>2040</v>
       </c>
       <c r="C85" t="n">
-        <v>14545</v>
+        <v>10707</v>
       </c>
       <c r="D85" t="n">
         <v>5489</v>
       </c>
       <c r="E85" t="n">
-        <v>9056</v>
+        <v>5218</v>
       </c>
     </row>
     <row r="86">
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>5860</v>
+        <v>5633</v>
       </c>
       <c r="D87" t="n">
         <v>5541</v>
       </c>
       <c r="E87" t="n">
-        <v>319</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>6218</v>
+        <v>5781</v>
       </c>
       <c r="D88" t="n">
         <v>5561</v>
       </c>
       <c r="E88" t="n">
-        <v>657</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>6585</v>
+        <v>5927</v>
       </c>
       <c r="D89" t="n">
         <v>5575</v>
       </c>
       <c r="E89" t="n">
-        <v>1010</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>6955</v>
+        <v>6078</v>
       </c>
       <c r="D90" t="n">
         <v>5583</v>
       </c>
       <c r="E90" t="n">
-        <v>1372</v>
+        <v>495</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>7324</v>
+        <v>6231</v>
       </c>
       <c r="D91" t="n">
         <v>5593</v>
       </c>
       <c r="E91" t="n">
-        <v>1731</v>
+        <v>637</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>7687</v>
+        <v>6378</v>
       </c>
       <c r="D92" t="n">
         <v>5600</v>
       </c>
       <c r="E92" t="n">
-        <v>2087</v>
+        <v>778</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>8047</v>
+        <v>6524</v>
       </c>
       <c r="D93" t="n">
         <v>5600</v>
       </c>
       <c r="E93" t="n">
-        <v>2447</v>
+        <v>924</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>8396</v>
+        <v>6662</v>
       </c>
       <c r="D94" t="n">
         <v>5582</v>
       </c>
       <c r="E94" t="n">
-        <v>2814</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>8740</v>
+        <v>6798</v>
       </c>
       <c r="D95" t="n">
         <v>5557</v>
       </c>
       <c r="E95" t="n">
-        <v>3183</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>9072</v>
+        <v>6924</v>
       </c>
       <c r="D96" t="n">
         <v>5531</v>
       </c>
       <c r="E96" t="n">
-        <v>3541</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>9395</v>
+        <v>7045</v>
       </c>
       <c r="D97" t="n">
         <v>5512</v>
       </c>
       <c r="E97" t="n">
-        <v>3883</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>9709</v>
+        <v>7156</v>
       </c>
       <c r="D98" t="n">
         <v>5499</v>
       </c>
       <c r="E98" t="n">
-        <v>4210</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>10015</v>
+        <v>7263</v>
       </c>
       <c r="D99" t="n">
         <v>5494</v>
       </c>
       <c r="E99" t="n">
-        <v>4521</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>10319</v>
+        <v>7368</v>
       </c>
       <c r="D100" t="n">
         <v>5481</v>
       </c>
       <c r="E100" t="n">
-        <v>4839</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>10620</v>
+        <v>7472</v>
       </c>
       <c r="D101" t="n">
         <v>5463</v>
       </c>
       <c r="E101" t="n">
-        <v>5157</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>10914</v>
+        <v>7572</v>
       </c>
       <c r="D102" t="n">
         <v>5450</v>
       </c>
       <c r="E102" t="n">
-        <v>5464</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>11206</v>
+        <v>7674</v>
       </c>
       <c r="D103" t="n">
         <v>5451</v>
       </c>
       <c r="E103" t="n">
-        <v>5755</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>11498</v>
+        <v>7777</v>
       </c>
       <c r="D104" t="n">
         <v>5461</v>
       </c>
       <c r="E104" t="n">
-        <v>6037</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>11790</v>
+        <v>7881</v>
       </c>
       <c r="D105" t="n">
         <v>5474</v>
       </c>
       <c r="E105" t="n">
-        <v>6316</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="106">
@@ -2067,13 +2067,13 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
-        <v>12076</v>
+        <v>7983</v>
       </c>
       <c r="D106" t="n">
         <v>5489</v>
       </c>
       <c r="E106" t="n">
-        <v>6587</v>
+        <v>2494</v>
       </c>
     </row>
     <row r="107">

</xml_diff>

<commit_message>
Detaljert likninger for tilbudet og kuttet høyeste alder for lærerstudenter.
</commit_message>
<xml_diff>
--- a/resultater/Lærermod.xlsx
+++ b/resultater/Lærermod.xlsx
@@ -506,7 +506,7 @@
         <v>2021</v>
       </c>
       <c r="C3" t="n">
-        <v>48005</v>
+        <v>48006</v>
       </c>
       <c r="D3" t="n">
         <v>46522</v>
@@ -521,13 +521,13 @@
         <v>2022</v>
       </c>
       <c r="C4" t="n">
-        <v>49055</v>
+        <v>49060</v>
       </c>
       <c r="D4" t="n">
         <v>45972</v>
       </c>
       <c r="E4" t="n">
-        <v>3084</v>
+        <v>3088</v>
       </c>
     </row>
     <row r="5">
@@ -536,13 +536,13 @@
         <v>2023</v>
       </c>
       <c r="C5" t="n">
-        <v>50112</v>
+        <v>50122</v>
       </c>
       <c r="D5" t="n">
         <v>45817</v>
       </c>
       <c r="E5" t="n">
-        <v>4295</v>
+        <v>4304</v>
       </c>
     </row>
     <row r="6">
@@ -551,13 +551,13 @@
         <v>2024</v>
       </c>
       <c r="C6" t="n">
-        <v>51175</v>
+        <v>51189</v>
       </c>
       <c r="D6" t="n">
         <v>45549</v>
       </c>
       <c r="E6" t="n">
-        <v>5626</v>
+        <v>5640</v>
       </c>
     </row>
     <row r="7">
@@ -566,13 +566,13 @@
         <v>2025</v>
       </c>
       <c r="C7" t="n">
-        <v>52234</v>
+        <v>52255</v>
       </c>
       <c r="D7" t="n">
         <v>45402</v>
       </c>
       <c r="E7" t="n">
-        <v>6832</v>
+        <v>6853</v>
       </c>
     </row>
     <row r="8">
@@ -581,13 +581,13 @@
         <v>2026</v>
       </c>
       <c r="C8" t="n">
-        <v>53293</v>
+        <v>53320</v>
       </c>
       <c r="D8" t="n">
         <v>45341</v>
       </c>
       <c r="E8" t="n">
-        <v>7952</v>
+        <v>7979</v>
       </c>
     </row>
     <row r="9">
@@ -596,13 +596,13 @@
         <v>2027</v>
       </c>
       <c r="C9" t="n">
-        <v>54325</v>
+        <v>54361</v>
       </c>
       <c r="D9" t="n">
         <v>45379</v>
       </c>
       <c r="E9" t="n">
-        <v>8946</v>
+        <v>8982</v>
       </c>
     </row>
     <row r="10">
@@ -611,13 +611,13 @@
         <v>2028</v>
       </c>
       <c r="C10" t="n">
-        <v>55330</v>
+        <v>55376</v>
       </c>
       <c r="D10" t="n">
         <v>45502</v>
       </c>
       <c r="E10" t="n">
-        <v>9828</v>
+        <v>9874</v>
       </c>
     </row>
     <row r="11">
@@ -626,13 +626,13 @@
         <v>2029</v>
       </c>
       <c r="C11" t="n">
-        <v>56277</v>
+        <v>56336</v>
       </c>
       <c r="D11" t="n">
         <v>45707</v>
       </c>
       <c r="E11" t="n">
-        <v>10570</v>
+        <v>10630</v>
       </c>
     </row>
     <row r="12">
@@ -641,13 +641,13 @@
         <v>2030</v>
       </c>
       <c r="C12" t="n">
-        <v>57146</v>
+        <v>57221</v>
       </c>
       <c r="D12" t="n">
         <v>45943</v>
       </c>
       <c r="E12" t="n">
-        <v>11203</v>
+        <v>11278</v>
       </c>
     </row>
     <row r="13">
@@ -656,13 +656,13 @@
         <v>2031</v>
       </c>
       <c r="C13" t="n">
-        <v>57939</v>
+        <v>58032</v>
       </c>
       <c r="D13" t="n">
         <v>46193</v>
       </c>
       <c r="E13" t="n">
-        <v>11746</v>
+        <v>11839</v>
       </c>
     </row>
     <row r="14">
@@ -671,13 +671,13 @@
         <v>2032</v>
       </c>
       <c r="C14" t="n">
-        <v>58633</v>
+        <v>58747</v>
       </c>
       <c r="D14" t="n">
         <v>46442</v>
       </c>
       <c r="E14" t="n">
-        <v>12191</v>
+        <v>12305</v>
       </c>
     </row>
     <row r="15">
@@ -686,13 +686,13 @@
         <v>2033</v>
       </c>
       <c r="C15" t="n">
-        <v>59232</v>
+        <v>59369</v>
       </c>
       <c r="D15" t="n">
         <v>46696</v>
       </c>
       <c r="E15" t="n">
-        <v>12536</v>
+        <v>12673</v>
       </c>
     </row>
     <row r="16">
@@ -701,13 +701,13 @@
         <v>2034</v>
       </c>
       <c r="C16" t="n">
-        <v>59752</v>
+        <v>59914</v>
       </c>
       <c r="D16" t="n">
         <v>46987</v>
       </c>
       <c r="E16" t="n">
-        <v>12766</v>
+        <v>12928</v>
       </c>
     </row>
     <row r="17">
@@ -716,13 +716,13 @@
         <v>2035</v>
       </c>
       <c r="C17" t="n">
-        <v>60185</v>
+        <v>60372</v>
       </c>
       <c r="D17" t="n">
         <v>47308</v>
       </c>
       <c r="E17" t="n">
-        <v>12878</v>
+        <v>13065</v>
       </c>
     </row>
     <row r="18">
@@ -731,13 +731,13 @@
         <v>2036</v>
       </c>
       <c r="C18" t="n">
-        <v>60574</v>
+        <v>60786</v>
       </c>
       <c r="D18" t="n">
         <v>47652</v>
       </c>
       <c r="E18" t="n">
-        <v>12921</v>
+        <v>13134</v>
       </c>
     </row>
     <row r="19">
@@ -746,13 +746,13 @@
         <v>2037</v>
       </c>
       <c r="C19" t="n">
-        <v>60940</v>
+        <v>61179</v>
       </c>
       <c r="D19" t="n">
         <v>48014</v>
       </c>
       <c r="E19" t="n">
-        <v>12926</v>
+        <v>13165</v>
       </c>
     </row>
     <row r="20">
@@ -761,13 +761,13 @@
         <v>2038</v>
       </c>
       <c r="C20" t="n">
-        <v>61317</v>
+        <v>61582</v>
       </c>
       <c r="D20" t="n">
         <v>48348</v>
       </c>
       <c r="E20" t="n">
-        <v>12969</v>
+        <v>13234</v>
       </c>
     </row>
     <row r="21">
@@ -776,13 +776,13 @@
         <v>2039</v>
       </c>
       <c r="C21" t="n">
-        <v>61723</v>
+        <v>62014</v>
       </c>
       <c r="D21" t="n">
         <v>48608</v>
       </c>
       <c r="E21" t="n">
-        <v>13115</v>
+        <v>13405</v>
       </c>
     </row>
     <row r="22">
@@ -791,13 +791,13 @@
         <v>2040</v>
       </c>
       <c r="C22" t="n">
-        <v>62181</v>
+        <v>62497</v>
       </c>
       <c r="D22" t="n">
         <v>48793</v>
       </c>
       <c r="E22" t="n">
-        <v>13387</v>
+        <v>13703</v>
       </c>
     </row>
     <row r="23">
@@ -825,13 +825,13 @@
         <v>2021</v>
       </c>
       <c r="C24" t="n">
-        <v>52773</v>
+        <v>52777</v>
       </c>
       <c r="D24" t="n">
         <v>52459</v>
       </c>
       <c r="E24" t="n">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25">
@@ -840,13 +840,13 @@
         <v>2022</v>
       </c>
       <c r="C25" t="n">
-        <v>53233</v>
+        <v>53242</v>
       </c>
       <c r="D25" t="n">
         <v>52487</v>
       </c>
       <c r="E25" t="n">
-        <v>746</v>
+        <v>755</v>
       </c>
     </row>
     <row r="26">
@@ -855,13 +855,13 @@
         <v>2023</v>
       </c>
       <c r="C26" t="n">
-        <v>53749</v>
+        <v>53765</v>
       </c>
       <c r="D26" t="n">
         <v>52346</v>
       </c>
       <c r="E26" t="n">
-        <v>1403</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="27">
@@ -870,13 +870,13 @@
         <v>2024</v>
       </c>
       <c r="C27" t="n">
-        <v>54321</v>
+        <v>54345</v>
       </c>
       <c r="D27" t="n">
         <v>52084</v>
       </c>
       <c r="E27" t="n">
-        <v>2237</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="28">
@@ -885,13 +885,13 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>54931</v>
+        <v>54965</v>
       </c>
       <c r="D28" t="n">
         <v>51637</v>
       </c>
       <c r="E28" t="n">
-        <v>3294</v>
+        <v>3328</v>
       </c>
     </row>
     <row r="29">
@@ -900,13 +900,13 @@
         <v>2026</v>
       </c>
       <c r="C29" t="n">
-        <v>55547</v>
+        <v>55593</v>
       </c>
       <c r="D29" t="n">
         <v>51094</v>
       </c>
       <c r="E29" t="n">
-        <v>4453</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="30">
@@ -915,13 +915,13 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>56193</v>
+        <v>56253</v>
       </c>
       <c r="D30" t="n">
         <v>50600</v>
       </c>
       <c r="E30" t="n">
-        <v>5594</v>
+        <v>5653</v>
       </c>
     </row>
     <row r="31">
@@ -930,13 +930,13 @@
         <v>2028</v>
       </c>
       <c r="C31" t="n">
-        <v>56819</v>
+        <v>56894</v>
       </c>
       <c r="D31" t="n">
         <v>50165</v>
       </c>
       <c r="E31" t="n">
-        <v>6654</v>
+        <v>6729</v>
       </c>
     </row>
     <row r="32">
@@ -945,13 +945,13 @@
         <v>2029</v>
       </c>
       <c r="C32" t="n">
-        <v>57406</v>
+        <v>57499</v>
       </c>
       <c r="D32" t="n">
         <v>49726</v>
       </c>
       <c r="E32" t="n">
-        <v>7680</v>
+        <v>7773</v>
       </c>
     </row>
     <row r="33">
@@ -960,13 +960,13 @@
         <v>2030</v>
       </c>
       <c r="C33" t="n">
-        <v>57928</v>
+        <v>58042</v>
       </c>
       <c r="D33" t="n">
         <v>49404</v>
       </c>
       <c r="E33" t="n">
-        <v>8524</v>
+        <v>8638</v>
       </c>
     </row>
     <row r="34">
@@ -975,13 +975,13 @@
         <v>2031</v>
       </c>
       <c r="C34" t="n">
-        <v>58391</v>
+        <v>58526</v>
       </c>
       <c r="D34" t="n">
         <v>49125</v>
       </c>
       <c r="E34" t="n">
-        <v>9266</v>
+        <v>9401</v>
       </c>
     </row>
     <row r="35">
@@ -990,13 +990,13 @@
         <v>2032</v>
       </c>
       <c r="C35" t="n">
-        <v>58778</v>
+        <v>58935</v>
       </c>
       <c r="D35" t="n">
         <v>48904</v>
       </c>
       <c r="E35" t="n">
-        <v>9874</v>
+        <v>10031</v>
       </c>
     </row>
     <row r="36">
@@ -1005,13 +1005,13 @@
         <v>2033</v>
       </c>
       <c r="C36" t="n">
-        <v>59083</v>
+        <v>59263</v>
       </c>
       <c r="D36" t="n">
         <v>48742</v>
       </c>
       <c r="E36" t="n">
-        <v>10341</v>
+        <v>10521</v>
       </c>
     </row>
     <row r="37">
@@ -1020,13 +1020,13 @@
         <v>2034</v>
       </c>
       <c r="C37" t="n">
-        <v>59331</v>
+        <v>59534</v>
       </c>
       <c r="D37" t="n">
         <v>48740</v>
       </c>
       <c r="E37" t="n">
-        <v>10591</v>
+        <v>10794</v>
       </c>
     </row>
     <row r="38">
@@ -1035,13 +1035,13 @@
         <v>2035</v>
       </c>
       <c r="C38" t="n">
-        <v>59522</v>
+        <v>59748</v>
       </c>
       <c r="D38" t="n">
         <v>48845</v>
       </c>
       <c r="E38" t="n">
-        <v>10677</v>
+        <v>10904</v>
       </c>
     </row>
     <row r="39">
@@ -1050,13 +1050,13 @@
         <v>2036</v>
       </c>
       <c r="C39" t="n">
-        <v>59689</v>
+        <v>59940</v>
       </c>
       <c r="D39" t="n">
         <v>49015</v>
       </c>
       <c r="E39" t="n">
-        <v>10674</v>
+        <v>10925</v>
       </c>
     </row>
     <row r="40">
@@ -1065,13 +1065,13 @@
         <v>2037</v>
       </c>
       <c r="C40" t="n">
-        <v>59849</v>
+        <v>60123</v>
       </c>
       <c r="D40" t="n">
         <v>49232</v>
       </c>
       <c r="E40" t="n">
-        <v>10617</v>
+        <v>10891</v>
       </c>
     </row>
     <row r="41">
@@ -1080,13 +1080,13 @@
         <v>2038</v>
       </c>
       <c r="C41" t="n">
-        <v>60004</v>
+        <v>60302</v>
       </c>
       <c r="D41" t="n">
         <v>49496</v>
       </c>
       <c r="E41" t="n">
-        <v>10507</v>
+        <v>10805</v>
       </c>
     </row>
     <row r="42">
@@ -1095,13 +1095,13 @@
         <v>2039</v>
       </c>
       <c r="C42" t="n">
-        <v>60182</v>
+        <v>60504</v>
       </c>
       <c r="D42" t="n">
         <v>49815</v>
       </c>
       <c r="E42" t="n">
-        <v>10367</v>
+        <v>10689</v>
       </c>
     </row>
     <row r="43">
@@ -1110,13 +1110,13 @@
         <v>2040</v>
       </c>
       <c r="C43" t="n">
-        <v>60374</v>
+        <v>60720</v>
       </c>
       <c r="D43" t="n">
         <v>50152</v>
       </c>
       <c r="E43" t="n">
-        <v>10223</v>
+        <v>10568</v>
       </c>
     </row>
     <row r="44">
@@ -1144,7 +1144,7 @@
         <v>2021</v>
       </c>
       <c r="C45" t="n">
-        <v>5963</v>
+        <v>5962</v>
       </c>
       <c r="D45" t="n">
         <v>5541</v>
@@ -1159,13 +1159,13 @@
         <v>2022</v>
       </c>
       <c r="C46" t="n">
-        <v>6431</v>
+        <v>6432</v>
       </c>
       <c r="D46" t="n">
         <v>5561</v>
       </c>
       <c r="E46" t="n">
-        <v>870</v>
+        <v>872</v>
       </c>
     </row>
     <row r="47">
@@ -1174,13 +1174,13 @@
         <v>2023</v>
       </c>
       <c r="C47" t="n">
-        <v>6896</v>
+        <v>6903</v>
       </c>
       <c r="D47" t="n">
         <v>5575</v>
       </c>
       <c r="E47" t="n">
-        <v>1322</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="48">
@@ -1189,13 +1189,13 @@
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>7360</v>
+        <v>7374</v>
       </c>
       <c r="D48" t="n">
         <v>5583</v>
       </c>
       <c r="E48" t="n">
-        <v>1777</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="49">
@@ -1204,13 +1204,13 @@
         <v>2025</v>
       </c>
       <c r="C49" t="n">
-        <v>7821</v>
+        <v>7844</v>
       </c>
       <c r="D49" t="n">
         <v>5593</v>
       </c>
       <c r="E49" t="n">
-        <v>2227</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="50">
@@ -1219,13 +1219,13 @@
         <v>2026</v>
       </c>
       <c r="C50" t="n">
-        <v>8272</v>
+        <v>8308</v>
       </c>
       <c r="D50" t="n">
         <v>5600</v>
       </c>
       <c r="E50" t="n">
-        <v>2672</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         <v>2027</v>
       </c>
       <c r="C51" t="n">
-        <v>8718</v>
+        <v>8769</v>
       </c>
       <c r="D51" t="n">
         <v>5600</v>
       </c>
       <c r="E51" t="n">
-        <v>3118</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>2028</v>
       </c>
       <c r="C52" t="n">
-        <v>9151</v>
+        <v>9220</v>
       </c>
       <c r="D52" t="n">
         <v>5582</v>
       </c>
       <c r="E52" t="n">
-        <v>3569</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="53">
@@ -1264,13 +1264,13 @@
         <v>2029</v>
       </c>
       <c r="C53" t="n">
-        <v>9578</v>
+        <v>9668</v>
       </c>
       <c r="D53" t="n">
         <v>5557</v>
       </c>
       <c r="E53" t="n">
-        <v>4021</v>
+        <v>4111</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1279,13 @@
         <v>2030</v>
       </c>
       <c r="C54" t="n">
-        <v>9990</v>
+        <v>10103</v>
       </c>
       <c r="D54" t="n">
         <v>5531</v>
       </c>
       <c r="E54" t="n">
-        <v>4459</v>
+        <v>4572</v>
       </c>
     </row>
     <row r="55">
@@ -1294,13 +1294,13 @@
         <v>2031</v>
       </c>
       <c r="C55" t="n">
-        <v>10396</v>
+        <v>10533</v>
       </c>
       <c r="D55" t="n">
         <v>5512</v>
       </c>
       <c r="E55" t="n">
-        <v>4884</v>
+        <v>5021</v>
       </c>
     </row>
     <row r="56">
@@ -1309,13 +1309,13 @@
         <v>2032</v>
       </c>
       <c r="C56" t="n">
-        <v>10790</v>
+        <v>10954</v>
       </c>
       <c r="D56" t="n">
         <v>5499</v>
       </c>
       <c r="E56" t="n">
-        <v>5291</v>
+        <v>5455</v>
       </c>
     </row>
     <row r="57">
@@ -1324,13 +1324,13 @@
         <v>2033</v>
       </c>
       <c r="C57" t="n">
-        <v>11177</v>
+        <v>11370</v>
       </c>
       <c r="D57" t="n">
         <v>5494</v>
       </c>
       <c r="E57" t="n">
-        <v>5684</v>
+        <v>5876</v>
       </c>
     </row>
     <row r="58">
@@ -1339,13 +1339,13 @@
         <v>2034</v>
       </c>
       <c r="C58" t="n">
-        <v>11561</v>
+        <v>11782</v>
       </c>
       <c r="D58" t="n">
         <v>5481</v>
       </c>
       <c r="E58" t="n">
-        <v>6081</v>
+        <v>6302</v>
       </c>
     </row>
     <row r="59">
@@ -1354,13 +1354,13 @@
         <v>2035</v>
       </c>
       <c r="C59" t="n">
-        <v>11940</v>
+        <v>12191</v>
       </c>
       <c r="D59" t="n">
         <v>5463</v>
       </c>
       <c r="E59" t="n">
-        <v>6477</v>
+        <v>6728</v>
       </c>
     </row>
     <row r="60">
@@ -1369,13 +1369,13 @@
         <v>2036</v>
       </c>
       <c r="C60" t="n">
-        <v>12308</v>
+        <v>12590</v>
       </c>
       <c r="D60" t="n">
         <v>5450</v>
       </c>
       <c r="E60" t="n">
-        <v>6859</v>
+        <v>7141</v>
       </c>
     </row>
     <row r="61">
@@ -1384,13 +1384,13 @@
         <v>2037</v>
       </c>
       <c r="C61" t="n">
-        <v>12677</v>
+        <v>12990</v>
       </c>
       <c r="D61" t="n">
         <v>5451</v>
       </c>
       <c r="E61" t="n">
-        <v>7225</v>
+        <v>7538</v>
       </c>
     </row>
     <row r="62">
@@ -1399,13 +1399,13 @@
         <v>2038</v>
       </c>
       <c r="C62" t="n">
-        <v>13044</v>
+        <v>13389</v>
       </c>
       <c r="D62" t="n">
         <v>5461</v>
       </c>
       <c r="E62" t="n">
-        <v>7583</v>
+        <v>7928</v>
       </c>
     </row>
     <row r="63">
@@ -1414,13 +1414,13 @@
         <v>2039</v>
       </c>
       <c r="C63" t="n">
-        <v>13409</v>
+        <v>13786</v>
       </c>
       <c r="D63" t="n">
         <v>5474</v>
       </c>
       <c r="E63" t="n">
-        <v>7936</v>
+        <v>8312</v>
       </c>
     </row>
     <row r="64">
@@ -1429,29 +1429,29 @@
         <v>2040</v>
       </c>
       <c r="C64" t="n">
-        <v>13769</v>
+        <v>14177</v>
       </c>
       <c r="D64" t="n">
         <v>5489</v>
       </c>
       <c r="E64" t="n">
-        <v>8280</v>
+        <v>8688</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Faglærere</t>
+          <t>PPU</t>
         </is>
       </c>
       <c r="B65" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C65" t="n">
-        <v>5534</v>
+        <v>30789</v>
       </c>
       <c r="D65" t="n">
-        <v>5534</v>
+        <v>30789</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -1463,13 +1463,13 @@
         <v>2021</v>
       </c>
       <c r="C66" t="n">
-        <v>5812</v>
+        <v>30791</v>
       </c>
       <c r="D66" t="n">
-        <v>5541</v>
+        <v>30824</v>
       </c>
       <c r="E66" t="n">
-        <v>271</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="67">
@@ -1478,13 +1478,13 @@
         <v>2022</v>
       </c>
       <c r="C67" t="n">
-        <v>6122</v>
+        <v>30887</v>
       </c>
       <c r="D67" t="n">
-        <v>5561</v>
+        <v>30930</v>
       </c>
       <c r="E67" t="n">
-        <v>561</v>
+        <v>-43</v>
       </c>
     </row>
     <row r="68">
@@ -1493,13 +1493,13 @@
         <v>2023</v>
       </c>
       <c r="C68" t="n">
-        <v>6427</v>
+        <v>31002</v>
       </c>
       <c r="D68" t="n">
-        <v>5575</v>
+        <v>31003</v>
       </c>
       <c r="E68" t="n">
-        <v>852</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1508,13 +1508,13 @@
         <v>2024</v>
       </c>
       <c r="C69" t="n">
-        <v>6728</v>
+        <v>31131</v>
       </c>
       <c r="D69" t="n">
-        <v>5583</v>
+        <v>31043</v>
       </c>
       <c r="E69" t="n">
-        <v>1145</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70">
@@ -1523,13 +1523,13 @@
         <v>2025</v>
       </c>
       <c r="C70" t="n">
-        <v>7026</v>
+        <v>31262</v>
       </c>
       <c r="D70" t="n">
-        <v>5593</v>
+        <v>31097</v>
       </c>
       <c r="E70" t="n">
-        <v>1433</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71">
@@ -1538,13 +1538,13 @@
         <v>2026</v>
       </c>
       <c r="C71" t="n">
-        <v>7315</v>
+        <v>31395</v>
       </c>
       <c r="D71" t="n">
-        <v>5600</v>
+        <v>31132</v>
       </c>
       <c r="E71" t="n">
-        <v>1715</v>
+        <v>263</v>
       </c>
     </row>
     <row r="72">
@@ -1553,13 +1553,13 @@
         <v>2027</v>
       </c>
       <c r="C72" t="n">
-        <v>7600</v>
+        <v>31514</v>
       </c>
       <c r="D72" t="n">
-        <v>5600</v>
+        <v>31124</v>
       </c>
       <c r="E72" t="n">
-        <v>2001</v>
+        <v>391</v>
       </c>
     </row>
     <row r="73">
@@ -1568,13 +1568,13 @@
         <v>2028</v>
       </c>
       <c r="C73" t="n">
-        <v>7874</v>
+        <v>31621</v>
       </c>
       <c r="D73" t="n">
-        <v>5582</v>
+        <v>31006</v>
       </c>
       <c r="E73" t="n">
-        <v>2293</v>
+        <v>615</v>
       </c>
     </row>
     <row r="74">
@@ -1583,13 +1583,13 @@
         <v>2029</v>
       </c>
       <c r="C74" t="n">
-        <v>8144</v>
+        <v>31711</v>
       </c>
       <c r="D74" t="n">
-        <v>5557</v>
+        <v>30845</v>
       </c>
       <c r="E74" t="n">
-        <v>2587</v>
+        <v>866</v>
       </c>
     </row>
     <row r="75">
@@ -1598,13 +1598,13 @@
         <v>2030</v>
       </c>
       <c r="C75" t="n">
-        <v>8401</v>
+        <v>31771</v>
       </c>
       <c r="D75" t="n">
-        <v>5531</v>
+        <v>30679</v>
       </c>
       <c r="E75" t="n">
-        <v>2870</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="76">
@@ -1613,13 +1613,13 @@
         <v>2031</v>
       </c>
       <c r="C76" t="n">
-        <v>8652</v>
+        <v>31797</v>
       </c>
       <c r="D76" t="n">
-        <v>5512</v>
+        <v>30555</v>
       </c>
       <c r="E76" t="n">
-        <v>3140</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="77">
@@ -1628,13 +1628,13 @@
         <v>2032</v>
       </c>
       <c r="C77" t="n">
-        <v>8894</v>
+        <v>31791</v>
       </c>
       <c r="D77" t="n">
-        <v>5499</v>
+        <v>30462</v>
       </c>
       <c r="E77" t="n">
-        <v>3395</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="78">
@@ -1643,13 +1643,13 @@
         <v>2033</v>
       </c>
       <c r="C78" t="n">
-        <v>9130</v>
+        <v>31748</v>
       </c>
       <c r="D78" t="n">
-        <v>5494</v>
+        <v>30416</v>
       </c>
       <c r="E78" t="n">
-        <v>3636</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="79">
@@ -1658,13 +1658,13 @@
         <v>2034</v>
       </c>
       <c r="C79" t="n">
-        <v>9363</v>
+        <v>31695</v>
       </c>
       <c r="D79" t="n">
-        <v>5481</v>
+        <v>30314</v>
       </c>
       <c r="E79" t="n">
-        <v>3883</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="80">
@@ -1673,13 +1673,13 @@
         <v>2035</v>
       </c>
       <c r="C80" t="n">
-        <v>9594</v>
+        <v>31610</v>
       </c>
       <c r="D80" t="n">
-        <v>5463</v>
+        <v>30184</v>
       </c>
       <c r="E80" t="n">
-        <v>4131</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="81">
@@ -1688,13 +1688,13 @@
         <v>2036</v>
       </c>
       <c r="C81" t="n">
-        <v>9816</v>
+        <v>31526</v>
       </c>
       <c r="D81" t="n">
-        <v>5450</v>
+        <v>30078</v>
       </c>
       <c r="E81" t="n">
-        <v>4366</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="82">
@@ -1703,13 +1703,13 @@
         <v>2037</v>
       </c>
       <c r="C82" t="n">
-        <v>10039</v>
+        <v>31428</v>
       </c>
       <c r="D82" t="n">
-        <v>5451</v>
+        <v>30063</v>
       </c>
       <c r="E82" t="n">
-        <v>4588</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="83">
@@ -1718,13 +1718,13 @@
         <v>2038</v>
       </c>
       <c r="C83" t="n">
-        <v>10264</v>
+        <v>31343</v>
       </c>
       <c r="D83" t="n">
-        <v>5461</v>
+        <v>30099</v>
       </c>
       <c r="E83" t="n">
-        <v>4803</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="84">
@@ -1733,13 +1733,13 @@
         <v>2039</v>
       </c>
       <c r="C84" t="n">
-        <v>10487</v>
+        <v>31256</v>
       </c>
       <c r="D84" t="n">
-        <v>5474</v>
+        <v>30146</v>
       </c>
       <c r="E84" t="n">
-        <v>5014</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="85">
@@ -1748,19 +1748,19 @@
         <v>2040</v>
       </c>
       <c r="C85" t="n">
-        <v>10707</v>
+        <v>31181</v>
       </c>
       <c r="D85" t="n">
-        <v>5489</v>
+        <v>30213</v>
       </c>
       <c r="E85" t="n">
-        <v>5218</v>
+        <v>968</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>Yrkesfaglærere</t>
+          <t>Praktiske og estetiske fag</t>
         </is>
       </c>
       <c r="B86" s="1" t="n">
@@ -1782,13 +1782,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>5633</v>
+        <v>5812</v>
       </c>
       <c r="D87" t="n">
         <v>5541</v>
       </c>
       <c r="E87" t="n">
-        <v>92</v>
+        <v>270</v>
       </c>
     </row>
     <row r="88">
@@ -1797,13 +1797,13 @@
         <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>5781</v>
+        <v>6123</v>
       </c>
       <c r="D88" t="n">
         <v>5561</v>
       </c>
       <c r="E88" t="n">
-        <v>220</v>
+        <v>562</v>
       </c>
     </row>
     <row r="89">
@@ -1812,13 +1812,13 @@
         <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>5927</v>
+        <v>6431</v>
       </c>
       <c r="D89" t="n">
         <v>5575</v>
       </c>
       <c r="E89" t="n">
-        <v>352</v>
+        <v>857</v>
       </c>
     </row>
     <row r="90">
@@ -1827,13 +1827,13 @@
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>6078</v>
+        <v>6738</v>
       </c>
       <c r="D90" t="n">
         <v>5583</v>
       </c>
       <c r="E90" t="n">
-        <v>495</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="91">
@@ -1842,13 +1842,13 @@
         <v>2025</v>
       </c>
       <c r="C91" t="n">
-        <v>6231</v>
+        <v>7043</v>
       </c>
       <c r="D91" t="n">
         <v>5593</v>
       </c>
       <c r="E91" t="n">
-        <v>637</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="92">
@@ -1857,13 +1857,13 @@
         <v>2026</v>
       </c>
       <c r="C92" t="n">
-        <v>6378</v>
+        <v>7341</v>
       </c>
       <c r="D92" t="n">
         <v>5600</v>
       </c>
       <c r="E92" t="n">
-        <v>778</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="93">
@@ -1872,13 +1872,13 @@
         <v>2027</v>
       </c>
       <c r="C93" t="n">
-        <v>6524</v>
+        <v>7637</v>
       </c>
       <c r="D93" t="n">
         <v>5600</v>
       </c>
       <c r="E93" t="n">
-        <v>924</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="94">
@@ -1887,13 +1887,13 @@
         <v>2028</v>
       </c>
       <c r="C94" t="n">
-        <v>6662</v>
+        <v>7924</v>
       </c>
       <c r="D94" t="n">
         <v>5582</v>
       </c>
       <c r="E94" t="n">
-        <v>1080</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="95">
@@ -1902,13 +1902,13 @@
         <v>2029</v>
       </c>
       <c r="C95" t="n">
-        <v>6798</v>
+        <v>8208</v>
       </c>
       <c r="D95" t="n">
         <v>5557</v>
       </c>
       <c r="E95" t="n">
-        <v>1241</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="96">
@@ -1917,13 +1917,13 @@
         <v>2030</v>
       </c>
       <c r="C96" t="n">
-        <v>6924</v>
+        <v>8481</v>
       </c>
       <c r="D96" t="n">
         <v>5531</v>
       </c>
       <c r="E96" t="n">
-        <v>1393</v>
+        <v>2951</v>
       </c>
     </row>
     <row r="97">
@@ -1932,13 +1932,13 @@
         <v>2031</v>
       </c>
       <c r="C97" t="n">
-        <v>7045</v>
+        <v>8750</v>
       </c>
       <c r="D97" t="n">
         <v>5512</v>
       </c>
       <c r="E97" t="n">
-        <v>1533</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="98">
@@ -1947,13 +1947,13 @@
         <v>2032</v>
       </c>
       <c r="C98" t="n">
-        <v>7156</v>
+        <v>9011</v>
       </c>
       <c r="D98" t="n">
         <v>5499</v>
       </c>
       <c r="E98" t="n">
-        <v>1657</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="99">
@@ -1962,13 +1962,13 @@
         <v>2033</v>
       </c>
       <c r="C99" t="n">
-        <v>7263</v>
+        <v>9267</v>
       </c>
       <c r="D99" t="n">
         <v>5494</v>
       </c>
       <c r="E99" t="n">
-        <v>1769</v>
+        <v>3773</v>
       </c>
     </row>
     <row r="100">
@@ -1977,13 +1977,13 @@
         <v>2034</v>
       </c>
       <c r="C100" t="n">
-        <v>7368</v>
+        <v>9521</v>
       </c>
       <c r="D100" t="n">
         <v>5481</v>
       </c>
       <c r="E100" t="n">
-        <v>1887</v>
+        <v>4041</v>
       </c>
     </row>
     <row r="101">
@@ -1992,13 +1992,13 @@
         <v>2035</v>
       </c>
       <c r="C101" t="n">
-        <v>7472</v>
+        <v>9773</v>
       </c>
       <c r="D101" t="n">
         <v>5463</v>
       </c>
       <c r="E101" t="n">
-        <v>2009</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="102">
@@ -2007,13 +2007,13 @@
         <v>2036</v>
       </c>
       <c r="C102" t="n">
-        <v>7572</v>
+        <v>10017</v>
       </c>
       <c r="D102" t="n">
         <v>5450</v>
       </c>
       <c r="E102" t="n">
-        <v>2122</v>
+        <v>4567</v>
       </c>
     </row>
     <row r="103">
@@ -2022,13 +2022,13 @@
         <v>2037</v>
       </c>
       <c r="C103" t="n">
-        <v>7674</v>
+        <v>10263</v>
       </c>
       <c r="D103" t="n">
         <v>5451</v>
       </c>
       <c r="E103" t="n">
-        <v>2223</v>
+        <v>4812</v>
       </c>
     </row>
     <row r="104">
@@ -2037,13 +2037,13 @@
         <v>2038</v>
       </c>
       <c r="C104" t="n">
-        <v>7777</v>
+        <v>10510</v>
       </c>
       <c r="D104" t="n">
         <v>5461</v>
       </c>
       <c r="E104" t="n">
-        <v>2315</v>
+        <v>5048</v>
       </c>
     </row>
     <row r="105">
@@ -2052,13 +2052,13 @@
         <v>2039</v>
       </c>
       <c r="C105" t="n">
-        <v>7881</v>
+        <v>10756</v>
       </c>
       <c r="D105" t="n">
         <v>5474</v>
       </c>
       <c r="E105" t="n">
-        <v>2407</v>
+        <v>5282</v>
       </c>
     </row>
     <row r="106">
@@ -2067,29 +2067,29 @@
         <v>2040</v>
       </c>
       <c r="C106" t="n">
-        <v>7983</v>
+        <v>10999</v>
       </c>
       <c r="D106" t="n">
         <v>5489</v>
       </c>
       <c r="E106" t="n">
-        <v>2494</v>
+        <v>5510</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>PPU</t>
+          <t>Yrkesfaglærere</t>
         </is>
       </c>
       <c r="B107" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="C107" t="n">
-        <v>30789</v>
+        <v>5534</v>
       </c>
       <c r="D107" t="n">
-        <v>30789</v>
+        <v>5534</v>
       </c>
       <c r="E107" t="n">
         <v>0</v>
@@ -2101,13 +2101,13 @@
         <v>2021</v>
       </c>
       <c r="C108" t="n">
-        <v>30793</v>
+        <v>5629</v>
       </c>
       <c r="D108" t="n">
-        <v>30824</v>
+        <v>5541</v>
       </c>
       <c r="E108" t="n">
-        <v>-31</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109">
@@ -2116,13 +2116,13 @@
         <v>2022</v>
       </c>
       <c r="C109" t="n">
-        <v>30890</v>
+        <v>5775</v>
       </c>
       <c r="D109" t="n">
-        <v>30930</v>
+        <v>5561</v>
       </c>
       <c r="E109" t="n">
-        <v>-40</v>
+        <v>214</v>
       </c>
     </row>
     <row r="110">
@@ -2131,13 +2131,13 @@
         <v>2023</v>
       </c>
       <c r="C110" t="n">
-        <v>31004</v>
+        <v>5921</v>
       </c>
       <c r="D110" t="n">
-        <v>31003</v>
+        <v>5575</v>
       </c>
       <c r="E110" t="n">
-        <v>1</v>
+        <v>346</v>
       </c>
     </row>
     <row r="111">
@@ -2146,13 +2146,13 @@
         <v>2024</v>
       </c>
       <c r="C111" t="n">
-        <v>31130</v>
+        <v>6073</v>
       </c>
       <c r="D111" t="n">
-        <v>31043</v>
+        <v>5583</v>
       </c>
       <c r="E111" t="n">
-        <v>87</v>
+        <v>490</v>
       </c>
     </row>
     <row r="112">
@@ -2161,13 +2161,13 @@
         <v>2025</v>
       </c>
       <c r="C112" t="n">
-        <v>31256</v>
+        <v>6228</v>
       </c>
       <c r="D112" t="n">
-        <v>31097</v>
+        <v>5593</v>
       </c>
       <c r="E112" t="n">
-        <v>159</v>
+        <v>635</v>
       </c>
     </row>
     <row r="113">
@@ -2176,13 +2176,13 @@
         <v>2026</v>
       </c>
       <c r="C113" t="n">
-        <v>31384</v>
+        <v>6379</v>
       </c>
       <c r="D113" t="n">
-        <v>31132</v>
+        <v>5600</v>
       </c>
       <c r="E113" t="n">
-        <v>252</v>
+        <v>779</v>
       </c>
     </row>
     <row r="114">
@@ -2191,13 +2191,13 @@
         <v>2027</v>
       </c>
       <c r="C114" t="n">
-        <v>31496</v>
+        <v>6530</v>
       </c>
       <c r="D114" t="n">
-        <v>31124</v>
+        <v>5600</v>
       </c>
       <c r="E114" t="n">
-        <v>373</v>
+        <v>930</v>
       </c>
     </row>
     <row r="115">
@@ -2206,13 +2206,13 @@
         <v>2028</v>
       </c>
       <c r="C115" t="n">
-        <v>31594</v>
+        <v>6673</v>
       </c>
       <c r="D115" t="n">
-        <v>31006</v>
+        <v>5582</v>
       </c>
       <c r="E115" t="n">
-        <v>588</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="116">
@@ -2221,13 +2221,13 @@
         <v>2029</v>
       </c>
       <c r="C116" t="n">
-        <v>31672</v>
+        <v>6816</v>
       </c>
       <c r="D116" t="n">
-        <v>30845</v>
+        <v>5557</v>
       </c>
       <c r="E116" t="n">
-        <v>827</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="117">
@@ -2236,13 +2236,13 @@
         <v>2030</v>
       </c>
       <c r="C117" t="n">
-        <v>31717</v>
+        <v>6951</v>
       </c>
       <c r="D117" t="n">
-        <v>30679</v>
+        <v>5531</v>
       </c>
       <c r="E117" t="n">
-        <v>1038</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="118">
@@ -2251,13 +2251,13 @@
         <v>2031</v>
       </c>
       <c r="C118" t="n">
-        <v>31726</v>
+        <v>7081</v>
       </c>
       <c r="D118" t="n">
-        <v>30555</v>
+        <v>5512</v>
       </c>
       <c r="E118" t="n">
-        <v>1170</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="119">
@@ -2266,13 +2266,13 @@
         <v>2032</v>
       </c>
       <c r="C119" t="n">
-        <v>31699</v>
+        <v>7203</v>
       </c>
       <c r="D119" t="n">
-        <v>30462</v>
+        <v>5499</v>
       </c>
       <c r="E119" t="n">
-        <v>1238</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="120">
@@ -2281,13 +2281,13 @@
         <v>2033</v>
       </c>
       <c r="C120" t="n">
-        <v>31633</v>
+        <v>7321</v>
       </c>
       <c r="D120" t="n">
-        <v>30416</v>
+        <v>5494</v>
       </c>
       <c r="E120" t="n">
-        <v>1217</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="121">
@@ -2296,13 +2296,13 @@
         <v>2034</v>
       </c>
       <c r="C121" t="n">
-        <v>31553</v>
+        <v>7438</v>
       </c>
       <c r="D121" t="n">
-        <v>30314</v>
+        <v>5481</v>
       </c>
       <c r="E121" t="n">
-        <v>1238</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="122">
@@ -2311,13 +2311,13 @@
         <v>2035</v>
       </c>
       <c r="C122" t="n">
-        <v>31437</v>
+        <v>7555</v>
       </c>
       <c r="D122" t="n">
-        <v>30184</v>
+        <v>5463</v>
       </c>
       <c r="E122" t="n">
-        <v>1254</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="123">
@@ -2326,13 +2326,13 @@
         <v>2036</v>
       </c>
       <c r="C123" t="n">
-        <v>31322</v>
+        <v>7668</v>
       </c>
       <c r="D123" t="n">
-        <v>30078</v>
+        <v>5450</v>
       </c>
       <c r="E123" t="n">
-        <v>1244</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="124">
@@ -2341,13 +2341,13 @@
         <v>2037</v>
       </c>
       <c r="C124" t="n">
-        <v>31190</v>
+        <v>7784</v>
       </c>
       <c r="D124" t="n">
-        <v>30063</v>
+        <v>5451</v>
       </c>
       <c r="E124" t="n">
-        <v>1127</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="125">
@@ -2356,13 +2356,13 @@
         <v>2038</v>
       </c>
       <c r="C125" t="n">
-        <v>31069</v>
+        <v>7901</v>
       </c>
       <c r="D125" t="n">
-        <v>30099</v>
+        <v>5461</v>
       </c>
       <c r="E125" t="n">
-        <v>970</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="126">
@@ -2371,13 +2371,13 @@
         <v>2039</v>
       </c>
       <c r="C126" t="n">
-        <v>30946</v>
+        <v>8019</v>
       </c>
       <c r="D126" t="n">
-        <v>30146</v>
+        <v>5474</v>
       </c>
       <c r="E126" t="n">
-        <v>800</v>
+        <v>2546</v>
       </c>
     </row>
     <row r="127">
@@ -2386,13 +2386,13 @@
         <v>2040</v>
       </c>
       <c r="C127" t="n">
-        <v>30834</v>
+        <v>8136</v>
       </c>
       <c r="D127" t="n">
-        <v>30213</v>
+        <v>5489</v>
       </c>
       <c r="E127" t="n">
-        <v>621</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="128">
@@ -2426,7 +2426,7 @@
         <v>13325</v>
       </c>
       <c r="E129" t="n">
-        <v>-100</v>
+        <v>-99</v>
       </c>
     </row>
     <row r="130">
@@ -2435,13 +2435,13 @@
         <v>2022</v>
       </c>
       <c r="C130" t="n">
-        <v>13190</v>
+        <v>13193</v>
       </c>
       <c r="D130" t="n">
         <v>13386</v>
       </c>
       <c r="E130" t="n">
-        <v>-196</v>
+        <v>-193</v>
       </c>
     </row>
     <row r="131">
@@ -2450,13 +2450,13 @@
         <v>2023</v>
       </c>
       <c r="C131" t="n">
-        <v>13140</v>
+        <v>13145</v>
       </c>
       <c r="D131" t="n">
         <v>13443</v>
       </c>
       <c r="E131" t="n">
-        <v>-304</v>
+        <v>-299</v>
       </c>
     </row>
     <row r="132">
@@ -2465,13 +2465,13 @@
         <v>2024</v>
       </c>
       <c r="C132" t="n">
-        <v>13091</v>
+        <v>13099</v>
       </c>
       <c r="D132" t="n">
         <v>13490</v>
       </c>
       <c r="E132" t="n">
-        <v>-399</v>
+        <v>-390</v>
       </c>
     </row>
     <row r="133">
@@ -2480,13 +2480,13 @@
         <v>2025</v>
       </c>
       <c r="C133" t="n">
-        <v>13024</v>
+        <v>13037</v>
       </c>
       <c r="D133" t="n">
         <v>13559</v>
       </c>
       <c r="E133" t="n">
-        <v>-535</v>
+        <v>-522</v>
       </c>
     </row>
     <row r="134">
@@ -2495,13 +2495,13 @@
         <v>2026</v>
       </c>
       <c r="C134" t="n">
-        <v>12945</v>
+        <v>12964</v>
       </c>
       <c r="D134" t="n">
         <v>13624</v>
       </c>
       <c r="E134" t="n">
-        <v>-679</v>
+        <v>-660</v>
       </c>
     </row>
     <row r="135">
@@ -2510,13 +2510,13 @@
         <v>2027</v>
       </c>
       <c r="C135" t="n">
-        <v>12866</v>
+        <v>12893</v>
       </c>
       <c r="D135" t="n">
         <v>13657</v>
       </c>
       <c r="E135" t="n">
-        <v>-792</v>
+        <v>-765</v>
       </c>
     </row>
     <row r="136">
@@ -2525,13 +2525,13 @@
         <v>2028</v>
       </c>
       <c r="C136" t="n">
-        <v>12763</v>
+        <v>12801</v>
       </c>
       <c r="D136" t="n">
         <v>13620</v>
       </c>
       <c r="E136" t="n">
-        <v>-857</v>
+        <v>-819</v>
       </c>
     </row>
     <row r="137">
@@ -2540,13 +2540,13 @@
         <v>2029</v>
       </c>
       <c r="C137" t="n">
-        <v>12664</v>
+        <v>12715</v>
       </c>
       <c r="D137" t="n">
         <v>13556</v>
       </c>
       <c r="E137" t="n">
-        <v>-893</v>
+        <v>-841</v>
       </c>
     </row>
     <row r="138">
@@ -2555,13 +2555,13 @@
         <v>2030</v>
       </c>
       <c r="C138" t="n">
-        <v>12555</v>
+        <v>12623</v>
       </c>
       <c r="D138" t="n">
         <v>13480</v>
       </c>
       <c r="E138" t="n">
-        <v>-924</v>
+        <v>-857</v>
       </c>
     </row>
     <row r="139">
@@ -2570,13 +2570,13 @@
         <v>2031</v>
       </c>
       <c r="C139" t="n">
-        <v>12434</v>
+        <v>12523</v>
       </c>
       <c r="D139" t="n">
         <v>13426</v>
       </c>
       <c r="E139" t="n">
-        <v>-992</v>
+        <v>-903</v>
       </c>
     </row>
     <row r="140">
@@ -2585,13 +2585,13 @@
         <v>2032</v>
       </c>
       <c r="C140" t="n">
-        <v>12321</v>
+        <v>12434</v>
       </c>
       <c r="D140" t="n">
         <v>13387</v>
       </c>
       <c r="E140" t="n">
-        <v>-1066</v>
+        <v>-952</v>
       </c>
     </row>
     <row r="141">
@@ -2600,13 +2600,13 @@
         <v>2033</v>
       </c>
       <c r="C141" t="n">
-        <v>12191</v>
+        <v>12335</v>
       </c>
       <c r="D141" t="n">
         <v>13373</v>
       </c>
       <c r="E141" t="n">
-        <v>-1182</v>
+        <v>-1038</v>
       </c>
     </row>
     <row r="142">
@@ -2615,13 +2615,13 @@
         <v>2034</v>
       </c>
       <c r="C142" t="n">
-        <v>12080</v>
+        <v>12258</v>
       </c>
       <c r="D142" t="n">
         <v>13314</v>
       </c>
       <c r="E142" t="n">
-        <v>-1234</v>
+        <v>-1056</v>
       </c>
     </row>
     <row r="143">
@@ -2630,13 +2630,13 @@
         <v>2035</v>
       </c>
       <c r="C143" t="n">
-        <v>11961</v>
+        <v>12177</v>
       </c>
       <c r="D143" t="n">
         <v>13229</v>
       </c>
       <c r="E143" t="n">
-        <v>-1267</v>
+        <v>-1052</v>
       </c>
     </row>
     <row r="144">
@@ -2645,13 +2645,13 @@
         <v>2036</v>
       </c>
       <c r="C144" t="n">
-        <v>11852</v>
+        <v>12107</v>
       </c>
       <c r="D144" t="n">
         <v>13153</v>
       </c>
       <c r="E144" t="n">
-        <v>-1301</v>
+        <v>-1046</v>
       </c>
     </row>
     <row r="145">
@@ -2660,13 +2660,13 @@
         <v>2037</v>
       </c>
       <c r="C145" t="n">
-        <v>11748</v>
+        <v>12046</v>
       </c>
       <c r="D145" t="n">
         <v>13129</v>
       </c>
       <c r="E145" t="n">
-        <v>-1381</v>
+        <v>-1083</v>
       </c>
     </row>
     <row r="146">
@@ -2675,13 +2675,13 @@
         <v>2038</v>
       </c>
       <c r="C146" t="n">
-        <v>11635</v>
+        <v>11975</v>
       </c>
       <c r="D146" t="n">
         <v>13132</v>
       </c>
       <c r="E146" t="n">
-        <v>-1498</v>
+        <v>-1157</v>
       </c>
     </row>
     <row r="147">
@@ -2690,13 +2690,13 @@
         <v>2039</v>
       </c>
       <c r="C147" t="n">
-        <v>11542</v>
+        <v>11925</v>
       </c>
       <c r="D147" t="n">
         <v>13138</v>
       </c>
       <c r="E147" t="n">
-        <v>-1597</v>
+        <v>-1213</v>
       </c>
     </row>
     <row r="148">
@@ -2705,13 +2705,13 @@
         <v>2040</v>
       </c>
       <c r="C148" t="n">
-        <v>11443</v>
+        <v>11869</v>
       </c>
       <c r="D148" t="n">
         <v>13155</v>
       </c>
       <c r="E148" t="n">
-        <v>-1712</v>
+        <v>-1286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>